<commit_message>
Generated output after fixing #252 and #258.
</commit_message>
<xml_diff>
--- a/mappings/package_F21/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F21/transformation/conceptual_mappings.xlsx
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>4.2.0</t>
+    <t>4.2.1</t>
   </si>
   <si>
     <r>
@@ -2628,7 +2628,7 @@
     <t>CONTRACTING_BODY/URL_TOOL</t>
   </si>
   <si>
-    <t>epo:Procedure / epo:Channel / xsd:anyURI</t>
+    <t>epo:Procedure / cv:Channel / xsd:anyURI</t>
   </si>
   <si>
     <r>

</xml_diff>

<commit_message>
Generated output and validation reports for form F21.
</commit_message>
<xml_diff>
--- a/mappings/package_F21/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F21/transformation/conceptual_mappings.xlsx
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>4.2.1</t>
+    <t>5.1.0</t>
   </si>
   <si>
     <r>
@@ -224,7 +224,7 @@
     <t>CONTRACTING_BODY/ADDRESS_CONTRACTING_BODY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:AgentInRole (from CL1)</t>
+    <t>epo:Notice / epo:AgentInRole (from CL1)</t>
   </si>
   <si>
     <t>?this epo:refersToRole ?value</t>
@@ -1547,7 +1547,7 @@
     <t>CONTRACTING_BODY/JOINT_PROCUREMENT_INVOLVED</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Procedure / xsd:boolean</t>
+    <t>epo:Notice / epo:Procedure / xsd:boolean</t>
   </si>
   <si>
     <r>
@@ -1604,7 +1604,7 @@
     <t>CONTRACTING_BODY/PROCUREMENT_LAW</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Procedure / epo:ProcedureSpecificTerm / rdf:langString</t>
+    <t>epo:Notice / epo:Procedure / epo:ProcedureSpecificTerm / rdf:langString</t>
   </si>
   <si>
     <r>
@@ -1655,7 +1655,7 @@
     <t>CONTRACTING_BODY/CENTRAL_PURCHASING</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Procedure / epo:ProcedureSpecificTerm / xsd:boolean</t>
+    <t>epo:Notice / epo:Procedure / epo:ProcedureSpecificTerm / xsd:boolean</t>
   </si>
   <si>
     <r>
@@ -3272,7 +3272,7 @@
     <t>OBJECT_CONTRACT</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation</t>
+    <t>epo:Notice / epo:NoticeAwardInformation</t>
   </si>
   <si>
     <t>?this epo:announcesNoticeAwardInformation ?value .</t>
@@ -3287,7 +3287,7 @@
     <t>OBJECT_CONTRACT/VAL_TOTAL</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation / epo:MonetaryValue / xsd:decimal</t>
+    <t>epo:Notice / epo:NoticeAwardInformation / epo:MonetaryValue / xsd:decimal</t>
   </si>
   <si>
     <t>?this epo:announcesNoticeAwardInformation / epo:hasTotalAwardedValue / epo:hasAmountValue ?value .</t>
@@ -3371,7 +3371,7 @@
     <t>OBJECT_CONTRACT/VAL_TOTAL/@CURRENCY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:NoticeAwardInformation / epo:MonetaryValue / at-voc:currency (from currency.json)</t>
+    <t>epo:Notice / epo:NoticeAwardInformation / epo:MonetaryValue / at-voc:currency (from currency.json)</t>
   </si>
   <si>
     <r>
@@ -3411,7 +3411,7 @@
     <t>II.2</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Lot</t>
+    <t>epo:Notice / epo:Lot</t>
   </si>
   <si>
     <t>?this epo:refersToLot ?value .</t>
@@ -4004,7 +4004,7 @@
     <t>OBJECT_CONTRACT/DATE_PUBLICATION_NOTICE</t>
   </si>
   <si>
-    <t>epo:ResultNotice / xsd:date</t>
+    <t>epo:Notice / xsd:date</t>
   </si>
   <si>
     <t>?this epo:hasPublicationDate ?value</t>
@@ -4548,7 +4548,7 @@
     <t>PROCEDURE/NOTICE_NUMBER_OJ</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Notice /  epo:Identifier / xsd:string</t>
+    <t>epo:Notice / epo:Notice /  epo:Identifier / xsd:string</t>
   </si>
   <si>
     <r>
@@ -4771,7 +4771,7 @@
     <t>if(exists(AWARDED_CONTRACT))</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Contract</t>
+    <t>epo:Notice / epo:Contract</t>
   </si>
   <si>
     <t>?this epo:announcesContract ?value</t>
@@ -6753,7 +6753,7 @@
     <t>COMPLEMENTARY_INFO/ADDRESS_MEDIATION_BODY</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:Mediator</t>
+    <t>epo:Notice / epo:Mediator</t>
   </si>
   <si>
     <t>VI.4.2.1</t>
@@ -7304,7 +7304,7 @@
     <t>COMPLEMENTARY_INFO/DATE_DISPATCH_NOTICE</t>
   </si>
   <si>
-    <t>epo:ResultNotice</t>
+    <t>epo:Notice</t>
   </si>
   <si>
     <r>
@@ -7988,7 +7988,7 @@
     <t>annex_d1.rml.ttl</t>
   </si>
   <si>
-    <t>result_notice.rml.ttl</t>
+    <t>notice.rml.ttl</t>
   </si>
   <si>
     <t>Informal (if possible to become formal)</t>
@@ -20829,7 +20829,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="21" t="s">
         <v>1209</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generated output for packages F06, F21, F22 and F25, based on CM v 5.5.0, as part of TX1.3 delivery. F22 was not properly generated.
Generated output for packages F06, F21, F22 and F25, based on CM v 5.5.0, as part of TX1.3 delivery. F22 was not properly generated.
</commit_message>
<xml_diff>
--- a/mappings/package_F21/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F21/transformation/conceptual_mappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="1257">
   <si>
     <t>Field</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>5.4.0</t>
+    <t>5.5.0</t>
   </si>
   <si>
     <r>
@@ -5070,7 +5070,10 @@
     <t>epo:LotAwardOutcome / epo:TenderAwardOutcome / epo:Winner</t>
   </si>
   <si>
-    <t>?this epo:comprisesTenderAwardOutcome / epo:awardsLotToWinner ?value</t>
+    <t>?this epo:comprisesTenderAwardOutcome / epo:indicatesAwardOfLotToWinner ?value</t>
+  </si>
+  <si>
+    <t>Winner is created only if there is a contractor identified through the `AWARD_CONTRACT/AWARDED_CONTRACT/CONTRACTORS/CONTRACTOR` XPath</t>
   </si>
   <si>
     <t>V.2.1</t>
@@ -8519,7 +8522,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="187">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8854,37 +8857,13 @@
     <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -16603,14 +16582,14 @@
       <c r="D136" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="E136" s="114" t="s">
+      <c r="E136" s="4" t="s">
         <v>583</v>
       </c>
       <c r="F136" s="4"/>
       <c r="G136" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="H136" s="115" t="s">
+      <c r="H136" s="114" t="s">
         <v>584</v>
       </c>
       <c r="I136" s="6"/>
@@ -16628,7 +16607,7 @@
         <v>587</v>
       </c>
       <c r="D137" s="6"/>
-      <c r="E137" s="116" t="s">
+      <c r="E137" s="4" t="s">
         <v>588</v>
       </c>
       <c r="F137" s="4"/>
@@ -16653,7 +16632,7 @@
       </c>
       <c r="C138" s="13"/>
       <c r="D138" s="13"/>
-      <c r="E138" s="36"/>
+      <c r="E138" s="49"/>
       <c r="F138" s="36"/>
       <c r="G138" s="49"/>
       <c r="H138" s="49"/>
@@ -16702,7 +16681,7 @@
       <c r="B141" s="55" t="s">
         <v>599</v>
       </c>
-      <c r="C141" s="117" t="s">
+      <c r="C141" s="115" t="s">
         <v>600</v>
       </c>
       <c r="D141" s="13"/>
@@ -16729,7 +16708,7 @@
       </c>
       <c r="C142" s="13"/>
       <c r="D142" s="13"/>
-      <c r="E142" s="118"/>
+      <c r="E142" s="49"/>
       <c r="F142" s="36"/>
       <c r="G142" s="49"/>
       <c r="H142" s="49"/>
@@ -16747,8 +16726,8 @@
       <c r="C143" s="36" t="s">
         <v>608</v>
       </c>
-      <c r="D143" s="119"/>
-      <c r="E143" s="120" t="s">
+      <c r="D143" s="13"/>
+      <c r="E143" s="49" t="s">
         <v>609</v>
       </c>
       <c r="F143" s="36" t="s">
@@ -16757,7 +16736,7 @@
       <c r="G143" s="49" t="s">
         <v>611</v>
       </c>
-      <c r="H143" s="121" t="s">
+      <c r="H143" s="116" t="s">
         <v>612</v>
       </c>
       <c r="I143" s="6"/>
@@ -16775,7 +16754,7 @@
         <v>615</v>
       </c>
       <c r="D144" s="13"/>
-      <c r="E144" s="118" t="s">
+      <c r="E144" s="49" t="s">
         <v>616</v>
       </c>
       <c r="F144" s="13" t="s">
@@ -16784,7 +16763,7 @@
       <c r="G144" s="49" t="s">
         <v>617</v>
       </c>
-      <c r="H144" s="121" t="s">
+      <c r="H144" s="116" t="s">
         <v>618</v>
       </c>
       <c r="I144" s="6"/>
@@ -16801,8 +16780,8 @@
       <c r="C145" s="13" t="s">
         <v>608</v>
       </c>
-      <c r="D145" s="119"/>
-      <c r="E145" s="120" t="s">
+      <c r="D145" s="13"/>
+      <c r="E145" s="49" t="s">
         <v>621</v>
       </c>
       <c r="F145" s="36" t="s">
@@ -16938,7 +16917,7 @@
       </c>
       <c r="C151" s="13"/>
       <c r="D151" s="13"/>
-      <c r="E151" s="118"/>
+      <c r="E151" s="49"/>
       <c r="F151" s="36"/>
       <c r="G151" s="49"/>
       <c r="H151" s="49"/>
@@ -16956,8 +16935,8 @@
       <c r="C152" s="96" t="s">
         <v>647</v>
       </c>
-      <c r="D152" s="122"/>
-      <c r="E152" s="123" t="s">
+      <c r="D152" s="97"/>
+      <c r="E152" s="80" t="s">
         <v>648</v>
       </c>
       <c r="F152" s="96" t="s">
@@ -16983,8 +16962,8 @@
       <c r="C153" s="97" t="s">
         <v>647</v>
       </c>
-      <c r="D153" s="122"/>
-      <c r="E153" s="124" t="s">
+      <c r="D153" s="97"/>
+      <c r="E153" s="56" t="s">
         <v>648</v>
       </c>
       <c r="F153" s="96" t="s">
@@ -17001,7 +16980,7 @@
       <c r="K153" s="6"/>
     </row>
     <row r="154">
-      <c r="A154" s="125" t="s">
+      <c r="A154" s="117" t="s">
         <v>653</v>
       </c>
       <c r="B154" s="91" t="s">
@@ -17073,7 +17052,7 @@
       <c r="G157" s="36" t="s">
         <v>664</v>
       </c>
-      <c r="H157" s="126" t="s">
+      <c r="H157" s="118" t="s">
         <v>665</v>
       </c>
       <c r="I157" s="6"/>
@@ -17100,7 +17079,7 @@
       <c r="G158" s="36" t="s">
         <v>664</v>
       </c>
-      <c r="H158" s="126" t="s">
+      <c r="H158" s="118" t="s">
         <v>669</v>
       </c>
       <c r="I158" s="6"/>
@@ -17154,7 +17133,7 @@
       <c r="G160" s="36" t="s">
         <v>664</v>
       </c>
-      <c r="H160" s="126" t="s">
+      <c r="H160" s="118" t="s">
         <v>677</v>
       </c>
       <c r="I160" s="6"/>
@@ -17254,7 +17233,7 @@
       <c r="B165" s="55" t="s">
         <v>696</v>
       </c>
-      <c r="C165" s="127" t="s">
+      <c r="C165" s="119" t="s">
         <v>228</v>
       </c>
       <c r="D165" s="82"/>
@@ -17265,7 +17244,7 @@
       <c r="G165" s="6" t="s">
         <v>698</v>
       </c>
-      <c r="H165" s="128" t="s">
+      <c r="H165" s="120" t="s">
         <v>699</v>
       </c>
       <c r="I165" s="6"/>
@@ -17290,7 +17269,7 @@
       <c r="G166" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="H166" s="129" t="s">
+      <c r="H166" s="121" t="s">
         <v>704</v>
       </c>
       <c r="I166" s="6"/>
@@ -17403,7 +17382,7 @@
       <c r="G171" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="H171" s="130" t="s">
+      <c r="H171" s="122" t="s">
         <v>725</v>
       </c>
       <c r="I171" s="6"/>
@@ -17428,7 +17407,7 @@
       <c r="G172" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="H172" s="131" t="s">
+      <c r="H172" s="123" t="s">
         <v>731</v>
       </c>
       <c r="I172" s="6"/>
@@ -17505,7 +17484,7 @@
       <c r="K175" s="6"/>
     </row>
     <row r="176">
-      <c r="A176" s="125" t="s">
+      <c r="A176" s="117" t="s">
         <v>746</v>
       </c>
       <c r="B176" s="34" t="s">
@@ -17530,14 +17509,14 @@
       <c r="K176" s="6"/>
     </row>
     <row r="177">
-      <c r="A177" s="132" t="s">
+      <c r="A177" s="124" t="s">
         <v>746</v>
       </c>
-      <c r="B177" s="133" t="s">
+      <c r="B177" s="125" t="s">
         <v>747</v>
       </c>
-      <c r="C177" s="134"/>
-      <c r="D177" s="134"/>
+      <c r="C177" s="126"/>
+      <c r="D177" s="126"/>
       <c r="E177" s="56" t="s">
         <v>748</v>
       </c>
@@ -17547,7 +17526,7 @@
       <c r="G177" s="40" t="s">
         <v>752</v>
       </c>
-      <c r="H177" s="135" t="s">
+      <c r="H177" s="127" t="s">
         <v>753</v>
       </c>
       <c r="I177" s="6"/>
@@ -17557,15 +17536,15 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="132" t="s">
+      <c r="A178" s="124" t="s">
         <v>746</v>
       </c>
-      <c r="B178" s="133" t="s">
+      <c r="B178" s="125" t="s">
         <v>747</v>
       </c>
       <c r="C178" s="13"/>
       <c r="D178" s="13"/>
-      <c r="E178" s="136" t="s">
+      <c r="E178" s="128" t="s">
         <v>748</v>
       </c>
       <c r="F178" s="36"/>
@@ -17665,10 +17644,10 @@
       <c r="K181" s="6"/>
     </row>
     <row r="182">
-      <c r="A182" s="137" t="s">
+      <c r="A182" s="129" t="s">
         <v>770</v>
       </c>
-      <c r="B182" s="138" t="s">
+      <c r="B182" s="130" t="s">
         <v>771</v>
       </c>
       <c r="C182" s="112" t="s">
@@ -17684,7 +17663,7 @@
       <c r="G182" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="H182" s="131" t="s">
+      <c r="H182" s="123" t="s">
         <v>779</v>
       </c>
       <c r="I182" s="6"/>
@@ -17698,7 +17677,7 @@
       <c r="B183" s="38" t="s">
         <v>781</v>
       </c>
-      <c r="C183" s="139" t="s">
+      <c r="C183" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D183" s="13"/>
@@ -17717,7 +17696,7 @@
       <c r="B184" s="47" t="s">
         <v>784</v>
       </c>
-      <c r="C184" s="139" t="s">
+      <c r="C184" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D184" s="13"/>
@@ -17776,7 +17755,7 @@
       <c r="G186" s="4" t="s">
         <v>790</v>
       </c>
-      <c r="H186" s="131" t="s">
+      <c r="H186" s="123" t="s">
         <v>795</v>
       </c>
       <c r="I186" s="6"/>
@@ -17790,7 +17769,7 @@
       <c r="B187" s="55" t="s">
         <v>797</v>
       </c>
-      <c r="C187" s="140" t="s">
+      <c r="C187" s="132" t="s">
         <v>635</v>
       </c>
       <c r="D187" s="13"/>
@@ -17815,7 +17794,7 @@
       <c r="B188" s="38" t="s">
         <v>747</v>
       </c>
-      <c r="C188" s="139" t="s">
+      <c r="C188" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D188" s="13"/>
@@ -17867,30 +17846,32 @@
       </c>
       <c r="I190" s="6"/>
       <c r="J190" s="6"/>
-      <c r="K190" s="6"/>
+      <c r="K190" s="6" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="48" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B191" s="47" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D191" s="13" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="E191" s="49" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="F191" s="49"/>
       <c r="G191" s="39" t="s">
-        <v>812</v>
-      </c>
-      <c r="H191" s="131" t="s">
         <v>813</v>
+      </c>
+      <c r="H191" s="123" t="s">
+        <v>814</v>
       </c>
       <c r="I191" s="6"/>
       <c r="J191" s="6"/>
@@ -17898,22 +17879,22 @@
     </row>
     <row r="192">
       <c r="A192" s="48" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B192" s="47" t="s">
-        <v>815</v>
-      </c>
-      <c r="C192" s="141"/>
-      <c r="D192" s="141"/>
+        <v>816</v>
+      </c>
+      <c r="C192" s="133"/>
+      <c r="D192" s="133"/>
       <c r="E192" s="56" t="s">
         <v>774</v>
       </c>
-      <c r="F192" s="142"/>
+      <c r="F192" s="134"/>
       <c r="G192" s="49" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="H192" s="36" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="I192" s="6"/>
       <c r="J192" s="6"/>
@@ -17921,26 +17902,26 @@
     </row>
     <row r="193">
       <c r="A193" s="93" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B193" s="55" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="D193" s="13" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="E193" s="49" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="F193" s="49"/>
       <c r="G193" s="36" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="H193" s="36" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="I193" s="6"/>
       <c r="J193" s="6"/>
@@ -17948,22 +17929,22 @@
     </row>
     <row r="194">
       <c r="A194" s="93" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B194" s="55" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
       <c r="E194" s="49" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="F194" s="49"/>
       <c r="G194" s="4" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H194" s="39" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="I194" s="6"/>
       <c r="J194" s="6"/>
@@ -17971,22 +17952,22 @@
     </row>
     <row r="195">
       <c r="A195" s="93" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B195" s="55" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C195" s="13"/>
       <c r="D195" s="13"/>
       <c r="E195" s="49" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="F195" s="63"/>
       <c r="G195" s="4" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H195" s="39" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="I195" s="6"/>
       <c r="J195" s="6"/>
@@ -17994,22 +17975,22 @@
     </row>
     <row r="196">
       <c r="A196" s="93" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B196" s="55" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C196" s="13"/>
       <c r="D196" s="13"/>
       <c r="E196" s="49" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="F196" s="49"/>
       <c r="G196" s="4" t="s">
-        <v>828</v>
-      </c>
-      <c r="H196" s="131" t="s">
-        <v>837</v>
+        <v>829</v>
+      </c>
+      <c r="H196" s="123" t="s">
+        <v>838</v>
       </c>
       <c r="I196" s="6"/>
       <c r="J196" s="6"/>
@@ -18017,22 +17998,22 @@
     </row>
     <row r="197">
       <c r="A197" s="93" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B197" s="55" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C197" s="13"/>
       <c r="D197" s="13"/>
       <c r="E197" s="49" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="F197" s="49"/>
       <c r="G197" s="4" t="s">
-        <v>828</v>
-      </c>
-      <c r="H197" s="129" t="s">
-        <v>841</v>
+        <v>829</v>
+      </c>
+      <c r="H197" s="121" t="s">
+        <v>842</v>
       </c>
       <c r="I197" s="6"/>
       <c r="J197" s="6"/>
@@ -18040,17 +18021,17 @@
     </row>
     <row r="198">
       <c r="A198" s="93" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B198" s="55" t="s">
-        <v>843</v>
-      </c>
-      <c r="C198" s="143" t="s">
         <v>844</v>
+      </c>
+      <c r="C198" s="135" t="s">
+        <v>845</v>
       </c>
       <c r="D198" s="13"/>
       <c r="E198" s="49" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F198" s="39"/>
       <c r="G198" s="36" t="s">
@@ -18065,12 +18046,12 @@
     </row>
     <row r="199">
       <c r="A199" s="48" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B199" s="47" t="s">
-        <v>847</v>
-      </c>
-      <c r="C199" s="139" t="s">
+        <v>848</v>
+      </c>
+      <c r="C199" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D199" s="13"/>
@@ -18084,7 +18065,7 @@
     </row>
     <row r="200">
       <c r="A200" s="93" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B200" s="55" t="s">
         <v>56</v>
@@ -18096,14 +18077,14 @@
         <v>58</v>
       </c>
       <c r="E200" s="49" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="F200" s="49"/>
       <c r="G200" s="43" t="s">
         <v>60</v>
       </c>
       <c r="H200" s="43" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="I200" s="6"/>
       <c r="J200" s="6"/>
@@ -18111,7 +18092,7 @@
     </row>
     <row r="201">
       <c r="A201" s="93" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B201" s="55" t="s">
         <v>63</v>
@@ -18123,14 +18104,14 @@
         <v>65</v>
       </c>
       <c r="E201" s="49" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="F201" s="49"/>
       <c r="G201" s="45" t="s">
         <v>67</v>
       </c>
       <c r="H201" s="45" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="I201" s="6"/>
       <c r="J201" s="6"/>
@@ -18138,7 +18119,7 @@
     </row>
     <row r="202">
       <c r="A202" s="93" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B202" s="55" t="s">
         <v>70</v>
@@ -18150,14 +18131,14 @@
         <v>72</v>
       </c>
       <c r="E202" s="49" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="F202" s="49"/>
       <c r="G202" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H202" s="39" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="I202" s="6"/>
       <c r="J202" s="6"/>
@@ -18165,7 +18146,7 @@
     </row>
     <row r="203">
       <c r="A203" s="93" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B203" s="55" t="s">
         <v>77</v>
@@ -18176,15 +18157,15 @@
       <c r="D203" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="E203" s="144" t="s">
-        <v>858</v>
-      </c>
-      <c r="F203" s="144"/>
+      <c r="E203" s="136" t="s">
+        <v>859</v>
+      </c>
+      <c r="F203" s="136"/>
       <c r="G203" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H203" s="39" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="I203" s="6"/>
       <c r="J203" s="6"/>
@@ -18192,7 +18173,7 @@
     </row>
     <row r="204">
       <c r="A204" s="93" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B204" s="55" t="s">
         <v>83</v>
@@ -18204,16 +18185,16 @@
         <v>85</v>
       </c>
       <c r="E204" s="79" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="F204" s="79" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="G204" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H204" s="49" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="I204" s="6"/>
       <c r="J204" s="6"/>
@@ -18221,26 +18202,26 @@
     </row>
     <row r="205">
       <c r="A205" s="93" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B205" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="C205" s="145" t="s">
+      <c r="C205" s="137" t="s">
         <v>92</v>
       </c>
-      <c r="D205" s="145" t="s">
-        <v>865</v>
-      </c>
-      <c r="E205" s="144" t="s">
+      <c r="D205" s="137" t="s">
         <v>866</v>
       </c>
-      <c r="F205" s="144"/>
+      <c r="E205" s="136" t="s">
+        <v>867</v>
+      </c>
+      <c r="F205" s="136"/>
       <c r="G205" s="4" t="s">
         <v>95</v>
       </c>
       <c r="H205" s="39" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="I205" s="6"/>
       <c r="J205" s="6"/>
@@ -18248,7 +18229,7 @@
     </row>
     <row r="206">
       <c r="A206" s="93" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B206" s="55" t="s">
         <v>98</v>
@@ -18259,15 +18240,15 @@
       <c r="D206" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E206" s="144" t="s">
-        <v>869</v>
-      </c>
-      <c r="F206" s="144"/>
+      <c r="E206" s="136" t="s">
+        <v>870</v>
+      </c>
+      <c r="F206" s="136"/>
       <c r="G206" s="77" t="s">
         <v>102</v>
       </c>
       <c r="H206" s="77" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="I206" s="6"/>
       <c r="J206" s="6"/>
@@ -18275,7 +18256,7 @@
     </row>
     <row r="207">
       <c r="A207" s="93" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B207" s="55" t="s">
         <v>118</v>
@@ -18286,15 +18267,15 @@
       <c r="D207" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E207" s="144" t="s">
-        <v>872</v>
-      </c>
-      <c r="F207" s="144"/>
+      <c r="E207" s="136" t="s">
+        <v>873</v>
+      </c>
+      <c r="F207" s="136"/>
       <c r="G207" s="63" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H207" s="63" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I207" s="6"/>
       <c r="J207" s="6"/>
@@ -18302,7 +18283,7 @@
     </row>
     <row r="208">
       <c r="A208" s="93" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B208" s="55" t="s">
         <v>112</v>
@@ -18313,15 +18294,15 @@
       <c r="D208" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E208" s="144" t="s">
-        <v>876</v>
-      </c>
-      <c r="F208" s="144"/>
+      <c r="E208" s="136" t="s">
+        <v>877</v>
+      </c>
+      <c r="F208" s="136"/>
       <c r="G208" s="49" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H208" s="49" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I208" s="6"/>
       <c r="J208" s="6"/>
@@ -18329,10 +18310,10 @@
     </row>
     <row r="209">
       <c r="A209" s="93" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B209" s="55" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C209" s="13" t="s">
         <v>134</v>
@@ -18340,15 +18321,15 @@
       <c r="D209" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="E209" s="144" t="s">
-        <v>881</v>
-      </c>
-      <c r="F209" s="144"/>
+      <c r="E209" s="136" t="s">
+        <v>882</v>
+      </c>
+      <c r="F209" s="136"/>
       <c r="G209" s="45" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H209" s="45" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="I209" s="6"/>
       <c r="J209" s="6"/>
@@ -18356,7 +18337,7 @@
     </row>
     <row r="210">
       <c r="A210" s="93" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B210" s="55" t="s">
         <v>125</v>
@@ -18367,15 +18348,15 @@
       <c r="D210" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E210" s="144" t="s">
-        <v>884</v>
-      </c>
-      <c r="F210" s="144"/>
+      <c r="E210" s="136" t="s">
+        <v>885</v>
+      </c>
+      <c r="F210" s="136"/>
       <c r="G210" s="49" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H210" s="49" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="I210" s="6"/>
       <c r="J210" s="6"/>
@@ -18383,26 +18364,26 @@
     </row>
     <row r="211">
       <c r="A211" s="93" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B211" s="55" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C211" s="13" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="D211" s="13" t="s">
-        <v>889</v>
-      </c>
-      <c r="E211" s="144" t="s">
         <v>890</v>
+      </c>
+      <c r="E211" s="136" t="s">
+        <v>891</v>
       </c>
       <c r="F211" s="79"/>
       <c r="G211" s="4" t="s">
-        <v>891</v>
-      </c>
-      <c r="H211" s="146" t="s">
         <v>892</v>
+      </c>
+      <c r="H211" s="138" t="s">
+        <v>893</v>
       </c>
       <c r="I211" s="6"/>
       <c r="J211" s="6"/>
@@ -18413,15 +18394,15 @@
       <c r="B212" s="4"/>
       <c r="C212" s="13"/>
       <c r="D212" s="13"/>
-      <c r="E212" s="147" t="s">
-        <v>890</v>
+      <c r="E212" s="139" t="s">
+        <v>891</v>
       </c>
       <c r="F212" s="79"/>
       <c r="G212" s="77" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="H212" s="77" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="I212" s="6"/>
       <c r="J212" s="6"/>
@@ -18429,12 +18410,12 @@
     </row>
     <row r="213">
       <c r="A213" s="48" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B213" s="47" t="s">
-        <v>896</v>
-      </c>
-      <c r="C213" s="139" t="s">
+        <v>897</v>
+      </c>
+      <c r="C213" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D213" s="13"/>
@@ -18448,10 +18429,10 @@
     </row>
     <row r="214">
       <c r="A214" s="93" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B214" s="55" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C214" s="13" t="s">
         <v>523</v>
@@ -18459,15 +18440,15 @@
       <c r="D214" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="E214" s="144" t="s">
-        <v>899</v>
-      </c>
-      <c r="F214" s="144"/>
+      <c r="E214" s="136" t="s">
+        <v>900</v>
+      </c>
+      <c r="F214" s="136"/>
       <c r="G214" s="36" t="s">
         <v>525</v>
       </c>
       <c r="H214" s="49" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="I214" s="6"/>
       <c r="J214" s="6"/>
@@ -18475,24 +18456,24 @@
     </row>
     <row r="215">
       <c r="A215" s="108" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B215" s="74" t="s">
         <v>413</v>
       </c>
-      <c r="C215" s="148" t="s">
+      <c r="C215" s="140" t="s">
         <v>228</v>
       </c>
-      <c r="D215" s="149"/>
-      <c r="E215" s="144" t="s">
-        <v>902</v>
-      </c>
-      <c r="F215" s="144"/>
+      <c r="D215" s="141"/>
+      <c r="E215" s="136" t="s">
+        <v>903</v>
+      </c>
+      <c r="F215" s="136"/>
       <c r="G215" s="36" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="H215" s="49" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="I215" s="6"/>
       <c r="J215" s="6"/>
@@ -18500,26 +18481,26 @@
     </row>
     <row r="216">
       <c r="A216" s="93" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B216" s="55" t="s">
-        <v>906</v>
-      </c>
-      <c r="C216" s="149" t="s">
         <v>907</v>
       </c>
-      <c r="D216" s="149" t="s">
+      <c r="C216" s="141" t="s">
         <v>908</v>
       </c>
-      <c r="E216" s="144" t="s">
+      <c r="D216" s="141" t="s">
         <v>909</v>
       </c>
-      <c r="F216" s="144"/>
+      <c r="E216" s="136" t="s">
+        <v>910</v>
+      </c>
+      <c r="F216" s="136"/>
       <c r="G216" s="4" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="H216" s="39" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="I216" s="6"/>
       <c r="J216" s="6"/>
@@ -18527,24 +18508,24 @@
     </row>
     <row r="217">
       <c r="A217" s="108" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B217" s="74" t="s">
         <v>413</v>
       </c>
-      <c r="C217" s="148" t="s">
+      <c r="C217" s="140" t="s">
         <v>228</v>
       </c>
-      <c r="D217" s="149"/>
-      <c r="E217" s="144" t="s">
-        <v>913</v>
-      </c>
-      <c r="F217" s="144"/>
+      <c r="D217" s="141"/>
+      <c r="E217" s="136" t="s">
+        <v>914</v>
+      </c>
+      <c r="F217" s="136"/>
       <c r="G217" s="4" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="H217" s="39" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="I217" s="6"/>
       <c r="J217" s="6"/>
@@ -18552,26 +18533,26 @@
     </row>
     <row r="218">
       <c r="A218" s="93" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B218" s="55" t="s">
         <v>460</v>
       </c>
-      <c r="C218" s="149" t="s">
+      <c r="C218" s="141" t="s">
         <v>461</v>
       </c>
-      <c r="D218" s="149" t="s">
+      <c r="D218" s="141" t="s">
         <v>462</v>
       </c>
-      <c r="E218" s="144" t="s">
-        <v>917</v>
-      </c>
-      <c r="F218" s="144"/>
+      <c r="E218" s="136" t="s">
+        <v>918</v>
+      </c>
+      <c r="F218" s="136"/>
       <c r="G218" s="36" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="H218" s="49" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="I218" s="6"/>
       <c r="J218" s="6"/>
@@ -18579,24 +18560,24 @@
     </row>
     <row r="219">
       <c r="A219" s="108" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B219" s="74" t="s">
         <v>413</v>
       </c>
-      <c r="C219" s="148" t="s">
+      <c r="C219" s="140" t="s">
         <v>228</v>
       </c>
-      <c r="D219" s="149"/>
-      <c r="E219" s="144" t="s">
-        <v>921</v>
-      </c>
-      <c r="F219" s="144"/>
+      <c r="D219" s="141"/>
+      <c r="E219" s="136" t="s">
+        <v>922</v>
+      </c>
+      <c r="F219" s="136"/>
       <c r="G219" s="36" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H219" s="49" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="I219" s="6"/>
       <c r="J219" s="6"/>
@@ -18604,26 +18585,26 @@
     </row>
     <row r="220">
       <c r="A220" s="93" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B220" s="55" t="s">
         <v>466</v>
       </c>
-      <c r="C220" s="149" t="s">
+      <c r="C220" s="141" t="s">
         <v>467</v>
       </c>
-      <c r="D220" s="149" t="s">
+      <c r="D220" s="141" t="s">
         <v>468</v>
       </c>
-      <c r="E220" s="144" t="s">
-        <v>925</v>
-      </c>
-      <c r="F220" s="144"/>
+      <c r="E220" s="136" t="s">
+        <v>926</v>
+      </c>
+      <c r="F220" s="136"/>
       <c r="G220" s="36" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="H220" s="49" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I220" s="6"/>
       <c r="J220" s="6"/>
@@ -18631,24 +18612,24 @@
     </row>
     <row r="221">
       <c r="A221" s="108" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B221" s="74" t="s">
         <v>413</v>
       </c>
-      <c r="C221" s="150" t="s">
+      <c r="C221" s="142" t="s">
         <v>228</v>
       </c>
       <c r="D221" s="13"/>
-      <c r="E221" s="147" t="s">
-        <v>921</v>
-      </c>
-      <c r="F221" s="144"/>
+      <c r="E221" s="139" t="s">
+        <v>922</v>
+      </c>
+      <c r="F221" s="136"/>
       <c r="G221" s="13" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H221" s="63" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="I221" s="6"/>
       <c r="J221" s="6"/>
@@ -18656,17 +18637,17 @@
     </row>
     <row r="222">
       <c r="A222" s="48" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B222" s="64" t="s">
-        <v>930</v>
-      </c>
-      <c r="C222" s="139" t="s">
+        <v>931</v>
+      </c>
+      <c r="C222" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D222" s="13"/>
-      <c r="E222" s="149"/>
-      <c r="F222" s="149"/>
+      <c r="E222" s="141"/>
+      <c r="F222" s="141"/>
       <c r="G222" s="4"/>
       <c r="H222" s="4"/>
       <c r="I222" s="6"/>
@@ -18675,26 +18656,26 @@
     </row>
     <row r="223">
       <c r="A223" s="93" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B223" s="89" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="D223" s="13" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E223" s="49" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="F223" s="63"/>
       <c r="G223" s="49" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="H223" s="101" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="I223" s="6"/>
       <c r="J223" s="6"/>
@@ -18702,10 +18683,10 @@
     </row>
     <row r="224">
       <c r="A224" s="93" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B224" s="89" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C224" s="6"/>
       <c r="D224" s="6"/>
@@ -18719,26 +18700,26 @@
     </row>
     <row r="225">
       <c r="A225" s="93" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B225" s="89" t="s">
         <v>406</v>
       </c>
       <c r="C225" s="63" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="D225" s="63" t="s">
-        <v>942</v>
-      </c>
-      <c r="E225" s="144" t="s">
         <v>943</v>
       </c>
-      <c r="F225" s="144"/>
+      <c r="E225" s="136" t="s">
+        <v>944</v>
+      </c>
+      <c r="F225" s="136"/>
       <c r="G225" s="36" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="H225" s="49" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="I225" s="6"/>
       <c r="J225" s="6"/>
@@ -18746,24 +18727,24 @@
     </row>
     <row r="226">
       <c r="A226" s="93" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B226" s="89" t="s">
         <v>413</v>
       </c>
-      <c r="C226" s="150" t="s">
+      <c r="C226" s="142" t="s">
         <v>228</v>
       </c>
       <c r="D226" s="13"/>
-      <c r="E226" s="144" t="s">
-        <v>947</v>
-      </c>
-      <c r="F226" s="144"/>
+      <c r="E226" s="136" t="s">
+        <v>948</v>
+      </c>
+      <c r="F226" s="136"/>
       <c r="G226" s="63" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="H226" s="13" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="I226" s="6"/>
       <c r="J226" s="6"/>
@@ -18771,26 +18752,26 @@
     </row>
     <row r="227">
       <c r="A227" s="93" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B227" s="89" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="C227" s="13" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="D227" s="13" t="s">
-        <v>953</v>
-      </c>
-      <c r="E227" s="144" t="s">
         <v>954</v>
       </c>
-      <c r="F227" s="144"/>
+      <c r="E227" s="136" t="s">
+        <v>955</v>
+      </c>
+      <c r="F227" s="136"/>
       <c r="G227" s="49" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="H227" s="49" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I227" s="6"/>
       <c r="J227" s="6"/>
@@ -18798,37 +18779,37 @@
     </row>
     <row r="228">
       <c r="A228" s="93" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B228" s="89" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C228" s="13" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="D228" s="13" t="s">
-        <v>960</v>
-      </c>
-      <c r="E228" s="144" t="s">
         <v>961</v>
       </c>
-      <c r="F228" s="144"/>
+      <c r="E228" s="136" t="s">
+        <v>962</v>
+      </c>
+      <c r="F228" s="136"/>
       <c r="G228" s="63" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="H228" s="63" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="I228" s="6"/>
       <c r="J228" s="6"/>
       <c r="K228" s="6"/>
     </row>
     <row r="229">
-      <c r="A229" s="125" t="s">
-        <v>964</v>
-      </c>
-      <c r="B229" s="151" t="s">
+      <c r="A229" s="117" t="s">
         <v>965</v>
+      </c>
+      <c r="B229" s="143" t="s">
+        <v>966</v>
       </c>
       <c r="C229" s="6"/>
       <c r="D229" s="6"/>
@@ -18842,15 +18823,15 @@
     </row>
     <row r="230">
       <c r="A230" s="37" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B230" s="61" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C230" s="97"/>
       <c r="D230" s="82"/>
-      <c r="E230" s="152"/>
-      <c r="F230" s="149"/>
+      <c r="E230" s="144"/>
+      <c r="F230" s="141"/>
       <c r="G230" s="63"/>
       <c r="H230" s="63"/>
       <c r="I230" s="6"/>
@@ -18859,24 +18840,24 @@
     </row>
     <row r="231">
       <c r="A231" s="46" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B231" s="64" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C231" s="97" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="D231" s="82"/>
-      <c r="E231" s="152" t="s">
-        <v>971</v>
-      </c>
-      <c r="F231" s="149"/>
+      <c r="E231" s="144" t="s">
+        <v>972</v>
+      </c>
+      <c r="F231" s="141"/>
       <c r="G231" s="4" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H231" s="105" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="I231" s="6"/>
       <c r="J231" s="6"/>
@@ -18884,24 +18865,24 @@
     </row>
     <row r="232">
       <c r="A232" s="46" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B232" s="64" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C232" s="97" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="D232" s="82"/>
-      <c r="E232" s="152" t="s">
-        <v>977</v>
-      </c>
-      <c r="F232" s="149"/>
+      <c r="E232" s="144" t="s">
+        <v>978</v>
+      </c>
+      <c r="F232" s="141"/>
       <c r="G232" s="4" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H232" s="105" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="I232" s="6"/>
       <c r="J232" s="6"/>
@@ -18909,24 +18890,24 @@
     </row>
     <row r="233">
       <c r="A233" s="46" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B233" s="64" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C233" s="97" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D233" s="82"/>
-      <c r="E233" s="152" t="s">
-        <v>982</v>
-      </c>
-      <c r="F233" s="149"/>
+      <c r="E233" s="144" t="s">
+        <v>983</v>
+      </c>
+      <c r="F233" s="141"/>
       <c r="G233" s="4" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H233" s="105" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="I233" s="6"/>
       <c r="J233" s="6"/>
@@ -18934,7 +18915,7 @@
     </row>
     <row r="234">
       <c r="A234" s="90" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B234" s="61" t="s">
         <v>580</v>
@@ -18945,15 +18926,15 @@
       <c r="D234" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="E234" s="144" t="s">
-        <v>985</v>
-      </c>
-      <c r="F234" s="144"/>
-      <c r="G234" s="153" t="s">
+      <c r="E234" s="136" t="s">
+        <v>986</v>
+      </c>
+      <c r="F234" s="136"/>
+      <c r="G234" s="145" t="s">
         <v>368</v>
       </c>
-      <c r="H234" s="154" t="s">
-        <v>986</v>
+      <c r="H234" s="146" t="s">
+        <v>987</v>
       </c>
       <c r="I234" s="6"/>
       <c r="J234" s="6"/>
@@ -18961,17 +18942,17 @@
     </row>
     <row r="235">
       <c r="A235" s="90" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B235" s="61" t="s">
-        <v>988</v>
-      </c>
-      <c r="C235" s="139" t="s">
+        <v>989</v>
+      </c>
+      <c r="C235" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D235" s="6"/>
-      <c r="E235" s="149"/>
-      <c r="F235" s="149"/>
+      <c r="E235" s="141"/>
+      <c r="F235" s="141"/>
       <c r="G235" s="6"/>
       <c r="H235" s="6"/>
       <c r="I235" s="6"/>
@@ -18980,17 +18961,17 @@
     </row>
     <row r="236">
       <c r="A236" s="48" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B236" s="64" t="s">
-        <v>990</v>
-      </c>
-      <c r="C236" s="155" t="s">
+        <v>991</v>
+      </c>
+      <c r="C236" s="147" t="s">
         <v>782</v>
       </c>
       <c r="D236" s="6"/>
       <c r="E236" s="87" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="F236" s="63"/>
       <c r="G236" s="13" t="s">
@@ -19005,7 +18986,7 @@
     </row>
     <row r="237">
       <c r="A237" s="93" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B237" s="89" t="s">
         <v>56</v>
@@ -19017,14 +18998,14 @@
         <v>58</v>
       </c>
       <c r="E237" s="63" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F237" s="63"/>
       <c r="G237" s="87" t="s">
         <v>60</v>
       </c>
       <c r="H237" s="87" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="I237" s="6"/>
       <c r="J237" s="6"/>
@@ -19032,7 +19013,7 @@
     </row>
     <row r="238">
       <c r="A238" s="93" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B238" s="89" t="s">
         <v>70</v>
@@ -19044,14 +19025,14 @@
         <v>72</v>
       </c>
       <c r="E238" s="63" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F238" s="63"/>
       <c r="G238" s="87" t="s">
         <v>74</v>
       </c>
       <c r="H238" s="87" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I238" s="6"/>
       <c r="J238" s="6"/>
@@ -19059,7 +19040,7 @@
     </row>
     <row r="239">
       <c r="A239" s="93" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B239" s="89" t="s">
         <v>77</v>
@@ -19071,14 +19052,14 @@
         <v>79</v>
       </c>
       <c r="E239" s="63" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F239" s="63"/>
       <c r="G239" s="87" t="s">
         <v>74</v>
       </c>
       <c r="H239" s="87" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I239" s="6"/>
       <c r="J239" s="6"/>
@@ -19086,7 +19067,7 @@
     </row>
     <row r="240">
       <c r="A240" s="93" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B240" s="89" t="s">
         <v>91</v>
@@ -19095,17 +19076,17 @@
         <v>92</v>
       </c>
       <c r="D240" s="13" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E240" s="63" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="F240" s="63"/>
       <c r="G240" s="87" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="H240" s="87" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="I240" s="6"/>
       <c r="J240" s="6"/>
@@ -19113,7 +19094,7 @@
     </row>
     <row r="241">
       <c r="A241" s="93" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B241" s="89" t="s">
         <v>98</v>
@@ -19125,14 +19106,14 @@
         <v>100</v>
       </c>
       <c r="E241" s="63" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="F241" s="63"/>
       <c r="G241" s="63" t="s">
         <v>102</v>
       </c>
       <c r="H241" s="63" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="I241" s="6"/>
       <c r="J241" s="6"/>
@@ -19140,7 +19121,7 @@
     </row>
     <row r="242">
       <c r="A242" s="93" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B242" s="89" t="s">
         <v>118</v>
@@ -19152,14 +19133,14 @@
         <v>120</v>
       </c>
       <c r="E242" s="63" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="F242" s="63"/>
       <c r="G242" s="63" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H242" s="63" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I242" s="6"/>
       <c r="J242" s="6"/>
@@ -19167,7 +19148,7 @@
     </row>
     <row r="243">
       <c r="A243" s="93" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B243" s="89" t="s">
         <v>112</v>
@@ -19179,14 +19160,14 @@
         <v>114</v>
       </c>
       <c r="E243" s="63" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="F243" s="63"/>
       <c r="G243" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H243" s="63" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I243" s="6"/>
       <c r="J243" s="6"/>
@@ -19194,10 +19175,10 @@
     </row>
     <row r="244">
       <c r="A244" s="93" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B244" s="89" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C244" s="13" t="s">
         <v>134</v>
@@ -19206,14 +19187,14 @@
         <v>135</v>
       </c>
       <c r="E244" s="63" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="F244" s="63"/>
       <c r="G244" s="60" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H244" s="60" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="I244" s="6"/>
       <c r="J244" s="6"/>
@@ -19221,7 +19202,7 @@
     </row>
     <row r="245">
       <c r="A245" s="93" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B245" s="89" t="s">
         <v>125</v>
@@ -19233,14 +19214,14 @@
         <v>127</v>
       </c>
       <c r="E245" s="63" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F245" s="63"/>
       <c r="G245" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H245" s="63" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="I245" s="6"/>
       <c r="J245" s="6"/>
@@ -19248,21 +19229,21 @@
     </row>
     <row r="246">
       <c r="A246" s="48" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B246" s="64" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C246" s="155" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C246" s="147" t="s">
         <v>782</v>
       </c>
-      <c r="D246" s="156"/>
+      <c r="D246" s="148"/>
       <c r="E246" s="87" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F246" s="13"/>
       <c r="G246" s="13" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="H246" s="13" t="s">
         <v>230</v>
@@ -19273,7 +19254,7 @@
     </row>
     <row r="247">
       <c r="A247" s="93" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B247" s="89" t="s">
         <v>56</v>
@@ -19285,14 +19266,14 @@
         <v>58</v>
       </c>
       <c r="E247" s="63" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="F247" s="63"/>
       <c r="G247" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="H247" s="130" t="s">
-        <v>1023</v>
+      <c r="H247" s="122" t="s">
+        <v>1024</v>
       </c>
       <c r="I247" s="6"/>
       <c r="J247" s="6"/>
@@ -19300,7 +19281,7 @@
     </row>
     <row r="248">
       <c r="A248" s="93" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B248" s="89" t="s">
         <v>70</v>
@@ -19312,14 +19293,14 @@
         <v>72</v>
       </c>
       <c r="E248" s="63" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="F248" s="63"/>
       <c r="G248" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="H248" s="130" t="s">
-        <v>1026</v>
+      <c r="H248" s="122" t="s">
+        <v>1027</v>
       </c>
       <c r="I248" s="6"/>
       <c r="J248" s="6"/>
@@ -19327,7 +19308,7 @@
     </row>
     <row r="249">
       <c r="A249" s="93" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B249" s="89" t="s">
         <v>77</v>
@@ -19339,14 +19320,14 @@
         <v>79</v>
       </c>
       <c r="E249" s="63" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F249" s="63"/>
       <c r="G249" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="H249" s="130" t="s">
-        <v>1029</v>
+      <c r="H249" s="122" t="s">
+        <v>1030</v>
       </c>
       <c r="I249" s="6"/>
       <c r="J249" s="6"/>
@@ -19354,7 +19335,7 @@
     </row>
     <row r="250">
       <c r="A250" s="93" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B250" s="89" t="s">
         <v>91</v>
@@ -19363,17 +19344,17 @@
         <v>92</v>
       </c>
       <c r="D250" s="13" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E250" s="63" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="F250" s="63"/>
       <c r="G250" s="87" t="s">
         <v>95</v>
       </c>
       <c r="H250" s="87" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="I250" s="6"/>
       <c r="J250" s="6"/>
@@ -19381,7 +19362,7 @@
     </row>
     <row r="251">
       <c r="A251" s="93" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B251" s="89" t="s">
         <v>98</v>
@@ -19393,14 +19374,14 @@
         <v>100</v>
       </c>
       <c r="E251" s="63" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="F251" s="63"/>
       <c r="G251" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="H251" s="130" t="s">
-        <v>1035</v>
+      <c r="H251" s="122" t="s">
+        <v>1036</v>
       </c>
       <c r="I251" s="6"/>
       <c r="J251" s="6"/>
@@ -19408,7 +19389,7 @@
     </row>
     <row r="252">
       <c r="A252" s="93" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B252" s="89" t="s">
         <v>118</v>
@@ -19420,14 +19401,14 @@
         <v>120</v>
       </c>
       <c r="E252" s="63" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F252" s="63"/>
       <c r="G252" s="63" t="s">
-        <v>873</v>
-      </c>
-      <c r="H252" s="157" t="s">
         <v>874</v>
+      </c>
+      <c r="H252" s="149" t="s">
+        <v>875</v>
       </c>
       <c r="I252" s="6"/>
       <c r="J252" s="6"/>
@@ -19435,7 +19416,7 @@
     </row>
     <row r="253">
       <c r="A253" s="93" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B253" s="89" t="s">
         <v>112</v>
@@ -19447,14 +19428,14 @@
         <v>114</v>
       </c>
       <c r="E253" s="63" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="F253" s="63"/>
       <c r="G253" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H253" s="63" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I253" s="6"/>
       <c r="J253" s="6"/>
@@ -19462,10 +19443,10 @@
     </row>
     <row r="254">
       <c r="A254" s="93" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B254" s="89" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C254" s="13" t="s">
         <v>134</v>
@@ -19474,14 +19455,14 @@
         <v>135</v>
       </c>
       <c r="E254" s="63" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F254" s="63"/>
       <c r="G254" s="60" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H254" s="60" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="I254" s="6"/>
       <c r="J254" s="6"/>
@@ -19489,7 +19470,7 @@
     </row>
     <row r="255">
       <c r="A255" s="93" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B255" s="89" t="s">
         <v>125</v>
@@ -19501,14 +19482,14 @@
         <v>127</v>
       </c>
       <c r="E255" s="63" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="F255" s="63"/>
       <c r="G255" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H255" s="63" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="I255" s="6"/>
       <c r="J255" s="6"/>
@@ -19516,26 +19497,26 @@
     </row>
     <row r="256">
       <c r="A256" s="48" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B256" s="64" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C256" s="13" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="D256" s="13" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="E256" s="63" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="F256" s="63"/>
-      <c r="G256" s="153" t="s">
-        <v>1050</v>
-      </c>
-      <c r="H256" s="154" t="s">
+      <c r="G256" s="145" t="s">
         <v>1051</v>
+      </c>
+      <c r="H256" s="146" t="s">
+        <v>1052</v>
       </c>
       <c r="I256" s="6"/>
       <c r="J256" s="6"/>
@@ -19543,21 +19524,21 @@
     </row>
     <row r="257">
       <c r="A257" s="48" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B257" s="64" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="C257" s="6"/>
       <c r="D257" s="6"/>
       <c r="E257" s="87" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="F257" s="13"/>
       <c r="G257" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H257" s="158" t="s">
+      <c r="H257" s="150" t="s">
         <v>230</v>
       </c>
       <c r="I257" s="6"/>
@@ -19566,7 +19547,7 @@
     </row>
     <row r="258">
       <c r="A258" s="93" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B258" s="89" t="s">
         <v>56</v>
@@ -19578,14 +19559,14 @@
         <v>58</v>
       </c>
       <c r="E258" s="63" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="F258" s="63"/>
       <c r="G258" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="H258" s="130" t="s">
-        <v>1057</v>
+      <c r="H258" s="122" t="s">
+        <v>1058</v>
       </c>
       <c r="I258" s="6"/>
       <c r="J258" s="6"/>
@@ -19593,7 +19574,7 @@
     </row>
     <row r="259">
       <c r="A259" s="93" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B259" s="89" t="s">
         <v>70</v>
@@ -19605,14 +19586,14 @@
         <v>72</v>
       </c>
       <c r="E259" s="63" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="F259" s="63"/>
       <c r="G259" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="H259" s="130" t="s">
-        <v>1060</v>
+      <c r="H259" s="122" t="s">
+        <v>1061</v>
       </c>
       <c r="I259" s="6"/>
       <c r="J259" s="6"/>
@@ -19620,7 +19601,7 @@
     </row>
     <row r="260">
       <c r="A260" s="93" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B260" s="89" t="s">
         <v>77</v>
@@ -19632,14 +19613,14 @@
         <v>79</v>
       </c>
       <c r="E260" s="63" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="F260" s="63"/>
       <c r="G260" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="H260" s="130" t="s">
-        <v>1063</v>
+      <c r="H260" s="122" t="s">
+        <v>1064</v>
       </c>
       <c r="I260" s="6"/>
       <c r="J260" s="6"/>
@@ -19647,7 +19628,7 @@
     </row>
     <row r="261">
       <c r="A261" s="93" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B261" s="89" t="s">
         <v>91</v>
@@ -19656,17 +19637,17 @@
         <v>92</v>
       </c>
       <c r="D261" s="13" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E261" s="63" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="F261" s="63"/>
       <c r="G261" s="87" t="s">
         <v>95</v>
       </c>
       <c r="H261" s="87" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="I261" s="6"/>
       <c r="J261" s="6"/>
@@ -19674,7 +19655,7 @@
     </row>
     <row r="262">
       <c r="A262" s="93" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B262" s="89" t="s">
         <v>98</v>
@@ -19686,14 +19667,14 @@
         <v>100</v>
       </c>
       <c r="E262" s="63" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="F262" s="63"/>
       <c r="G262" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="H262" s="157" t="s">
-        <v>1069</v>
+      <c r="H262" s="149" t="s">
+        <v>1070</v>
       </c>
       <c r="I262" s="6"/>
       <c r="J262" s="6"/>
@@ -19701,7 +19682,7 @@
     </row>
     <row r="263">
       <c r="A263" s="93" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B263" s="89" t="s">
         <v>118</v>
@@ -19713,14 +19694,14 @@
         <v>120</v>
       </c>
       <c r="E263" s="63" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="F263" s="63"/>
       <c r="G263" s="63" t="s">
-        <v>873</v>
-      </c>
-      <c r="H263" s="157" t="s">
         <v>874</v>
+      </c>
+      <c r="H263" s="149" t="s">
+        <v>875</v>
       </c>
       <c r="I263" s="6"/>
       <c r="J263" s="6"/>
@@ -19728,7 +19709,7 @@
     </row>
     <row r="264">
       <c r="A264" s="93" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B264" s="89" t="s">
         <v>112</v>
@@ -19740,14 +19721,14 @@
         <v>114</v>
       </c>
       <c r="E264" s="63" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="F264" s="63"/>
       <c r="G264" s="63" t="s">
-        <v>877</v>
-      </c>
-      <c r="H264" s="157" t="s">
         <v>878</v>
+      </c>
+      <c r="H264" s="149" t="s">
+        <v>879</v>
       </c>
       <c r="I264" s="6"/>
       <c r="J264" s="6"/>
@@ -19755,10 +19736,10 @@
     </row>
     <row r="265">
       <c r="A265" s="93" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B265" s="89" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C265" s="13" t="s">
         <v>134</v>
@@ -19767,14 +19748,14 @@
         <v>135</v>
       </c>
       <c r="E265" s="63" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="F265" s="63"/>
       <c r="G265" s="60" t="s">
-        <v>873</v>
-      </c>
-      <c r="H265" s="159" t="s">
-        <v>1076</v>
+        <v>874</v>
+      </c>
+      <c r="H265" s="151" t="s">
+        <v>1077</v>
       </c>
       <c r="I265" s="6"/>
       <c r="J265" s="6"/>
@@ -19782,7 +19763,7 @@
     </row>
     <row r="266">
       <c r="A266" s="93" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B266" s="89" t="s">
         <v>125</v>
@@ -19794,14 +19775,14 @@
         <v>127</v>
       </c>
       <c r="E266" s="63" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="F266" s="63"/>
       <c r="G266" s="63" t="s">
-        <v>877</v>
-      </c>
-      <c r="H266" s="157" t="s">
-        <v>885</v>
+        <v>878</v>
+      </c>
+      <c r="H266" s="149" t="s">
+        <v>886</v>
       </c>
       <c r="I266" s="6"/>
       <c r="J266" s="6"/>
@@ -19809,37 +19790,37 @@
     </row>
     <row r="267">
       <c r="A267" s="90" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B267" s="61" t="s">
-        <v>1080</v>
-      </c>
-      <c r="C267" s="160" t="s">
         <v>1081</v>
       </c>
-      <c r="D267" s="160" t="s">
+      <c r="C267" s="152" t="s">
         <v>1082</v>
       </c>
-      <c r="E267" s="161" t="s">
+      <c r="D267" s="152" t="s">
         <v>1083</v>
       </c>
-      <c r="F267" s="161"/>
+      <c r="E267" s="153" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F267" s="153"/>
       <c r="G267" s="87" t="s">
-        <v>1084</v>
-      </c>
-      <c r="H267" s="162" t="s">
         <v>1085</v>
+      </c>
+      <c r="H267" s="154" t="s">
+        <v>1086</v>
       </c>
       <c r="I267" s="6"/>
       <c r="J267" s="6"/>
       <c r="K267" s="6"/>
     </row>
     <row r="268">
-      <c r="A268" s="125" t="s">
-        <v>1086</v>
-      </c>
-      <c r="B268" s="151" t="s">
+      <c r="A268" s="117" t="s">
         <v>1087</v>
+      </c>
+      <c r="B268" s="143" t="s">
+        <v>1088</v>
       </c>
       <c r="C268" s="6"/>
       <c r="D268" s="6"/>
@@ -19853,17 +19834,17 @@
     </row>
     <row r="269">
       <c r="A269" s="90" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B269" s="61" t="s">
-        <v>1089</v>
-      </c>
-      <c r="C269" s="139" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C269" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D269" s="13"/>
       <c r="E269" s="63" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="F269" s="6"/>
       <c r="G269" s="6"/>
@@ -19874,16 +19855,16 @@
     </row>
     <row r="270">
       <c r="A270" s="48" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B270" s="64" t="s">
-        <v>1092</v>
-      </c>
-      <c r="C270" s="139" t="s">
         <v>1093</v>
       </c>
+      <c r="C270" s="131" t="s">
+        <v>1094</v>
+      </c>
       <c r="D270" s="13" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E270" s="87"/>
       <c r="F270" s="6"/>
@@ -19895,53 +19876,53 @@
     </row>
     <row r="271">
       <c r="A271" s="93" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B271" s="89" t="s">
         <v>660</v>
       </c>
       <c r="C271" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D271" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E271" s="63" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="F271" s="13"/>
       <c r="G271" s="87" t="s">
-        <v>1099</v>
-      </c>
-      <c r="H271" s="130" t="s">
         <v>1100</v>
+      </c>
+      <c r="H271" s="122" t="s">
+        <v>1101</v>
       </c>
       <c r="I271" s="6"/>
       <c r="J271" s="6"/>
       <c r="K271" s="6"/>
     </row>
     <row r="272">
-      <c r="A272" s="163" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B272" s="164" t="s">
+      <c r="A272" s="155" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B272" s="156" t="s">
         <v>660</v>
       </c>
-      <c r="C272" s="165" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D272" s="165" t="s">
+      <c r="C272" s="157" t="s">
         <v>1097</v>
       </c>
-      <c r="E272" s="166" t="s">
+      <c r="D272" s="157" t="s">
         <v>1098</v>
+      </c>
+      <c r="E272" s="158" t="s">
+        <v>1099</v>
       </c>
       <c r="F272" s="13"/>
       <c r="G272" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H272" s="130" t="s">
         <v>1102</v>
+      </c>
+      <c r="H272" s="122" t="s">
+        <v>1103</v>
       </c>
       <c r="I272" s="6"/>
       <c r="J272" s="6"/>
@@ -19949,53 +19930,53 @@
     </row>
     <row r="273">
       <c r="A273" s="93" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B273" s="89" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="C273" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D273" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E273" s="63" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="F273" s="13"/>
       <c r="G273" s="87" t="s">
-        <v>1099</v>
-      </c>
-      <c r="H273" s="130" t="s">
-        <v>1106</v>
+        <v>1100</v>
+      </c>
+      <c r="H273" s="122" t="s">
+        <v>1107</v>
       </c>
       <c r="I273" s="6"/>
       <c r="J273" s="6"/>
       <c r="K273" s="6"/>
     </row>
     <row r="274">
-      <c r="A274" s="163" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B274" s="164" t="s">
+      <c r="A274" s="155" t="s">
         <v>1104</v>
       </c>
-      <c r="C274" s="165" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D274" s="165" t="s">
+      <c r="B274" s="156" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C274" s="157" t="s">
         <v>1097</v>
       </c>
-      <c r="E274" s="166" t="s">
-        <v>1105</v>
+      <c r="D274" s="157" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E274" s="158" t="s">
+        <v>1106</v>
       </c>
       <c r="F274" s="13"/>
       <c r="G274" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H274" s="130" t="s">
-        <v>1107</v>
+        <v>1102</v>
+      </c>
+      <c r="H274" s="122" t="s">
+        <v>1108</v>
       </c>
       <c r="I274" s="6"/>
       <c r="J274" s="6"/>
@@ -20003,12 +19984,12 @@
     </row>
     <row r="275">
       <c r="A275" s="48" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B275" s="64" t="s">
-        <v>1109</v>
-      </c>
-      <c r="C275" s="139" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C275" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D275" s="13"/>
@@ -20022,26 +20003,26 @@
     </row>
     <row r="276">
       <c r="A276" s="93" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B276" s="89" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C276" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="D276" s="13" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E276" s="63" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="F276" s="6"/>
       <c r="G276" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H276" s="130" t="s">
-        <v>1113</v>
+        <v>1102</v>
+      </c>
+      <c r="H276" s="122" t="s">
+        <v>1114</v>
       </c>
       <c r="I276" s="6"/>
       <c r="J276" s="6"/>
@@ -20049,26 +20030,26 @@
     </row>
     <row r="277">
       <c r="A277" s="93" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B277" s="89" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C277" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="D277" s="13" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E277" s="63" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="F277" s="6"/>
       <c r="G277" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H277" s="130" t="s">
-        <v>1117</v>
+        <v>1102</v>
+      </c>
+      <c r="H277" s="122" t="s">
+        <v>1118</v>
       </c>
       <c r="I277" s="6"/>
       <c r="J277" s="6"/>
@@ -20076,26 +20057,26 @@
     </row>
     <row r="278">
       <c r="A278" s="93" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B278" s="89" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="C278" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="D278" s="13" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E278" s="63" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="F278" s="6"/>
       <c r="G278" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H278" s="130" t="s">
-        <v>1121</v>
+        <v>1102</v>
+      </c>
+      <c r="H278" s="122" t="s">
+        <v>1122</v>
       </c>
       <c r="I278" s="6"/>
       <c r="J278" s="6"/>
@@ -20103,26 +20084,26 @@
     </row>
     <row r="279">
       <c r="A279" s="48" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B279" s="64" t="s">
-        <v>1123</v>
-      </c>
-      <c r="C279" s="139" t="s">
-        <v>1093</v>
+        <v>1124</v>
+      </c>
+      <c r="C279" s="131" t="s">
+        <v>1094</v>
       </c>
       <c r="D279" s="13" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E279" s="63" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="F279" s="6"/>
       <c r="G279" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H279" s="130" t="s">
-        <v>1125</v>
+        <v>1102</v>
+      </c>
+      <c r="H279" s="122" t="s">
+        <v>1126</v>
       </c>
       <c r="I279" s="6"/>
       <c r="J279" s="6"/>
@@ -20130,26 +20111,26 @@
     </row>
     <row r="280">
       <c r="A280" s="48" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B280" s="64" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C280" s="139" t="s">
-        <v>1093</v>
+        <v>1128</v>
+      </c>
+      <c r="C280" s="131" t="s">
+        <v>1094</v>
       </c>
       <c r="D280" s="13" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E280" s="63" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="F280" s="6"/>
       <c r="G280" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H280" s="130" t="s">
-        <v>1129</v>
+        <v>1102</v>
+      </c>
+      <c r="H280" s="122" t="s">
+        <v>1130</v>
       </c>
       <c r="I280" s="6"/>
       <c r="J280" s="6"/>
@@ -20157,12 +20138,12 @@
     </row>
     <row r="281">
       <c r="A281" s="48" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B281" s="64" t="s">
-        <v>1131</v>
-      </c>
-      <c r="C281" s="139" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C281" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D281" s="13"/>
@@ -20176,26 +20157,26 @@
     </row>
     <row r="282">
       <c r="A282" s="93" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B282" s="89" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C282" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="D282" s="13" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E282" s="63" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="F282" s="6"/>
       <c r="G282" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H282" s="130" t="s">
-        <v>1135</v>
+        <v>1102</v>
+      </c>
+      <c r="H282" s="122" t="s">
+        <v>1136</v>
       </c>
       <c r="I282" s="6"/>
       <c r="J282" s="6"/>
@@ -20203,26 +20184,26 @@
     </row>
     <row r="283">
       <c r="A283" s="93" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B283" s="89" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="C283" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="D283" s="13" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E283" s="63" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="F283" s="6"/>
       <c r="G283" s="6" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H283" s="130" t="s">
-        <v>1139</v>
+        <v>1102</v>
+      </c>
+      <c r="H283" s="122" t="s">
+        <v>1140</v>
       </c>
       <c r="I283" s="6"/>
       <c r="J283" s="6"/>
@@ -20230,12 +20211,12 @@
     </row>
     <row r="284">
       <c r="A284" s="90" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B284" s="61" t="s">
-        <v>1141</v>
-      </c>
-      <c r="C284" s="139" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C284" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D284" s="13"/>
@@ -20249,24 +20230,24 @@
     </row>
     <row r="285">
       <c r="A285" s="48" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="B285" s="64" t="s">
-        <v>1143</v>
-      </c>
-      <c r="C285" s="167" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C285" s="159" t="s">
         <v>635</v>
       </c>
       <c r="D285" s="13"/>
       <c r="E285" s="63" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="F285" s="6"/>
       <c r="G285" s="13" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H285" s="157" t="s">
-        <v>1145</v>
+        <v>1102</v>
+      </c>
+      <c r="H285" s="149" t="s">
+        <v>1146</v>
       </c>
       <c r="I285" s="6"/>
       <c r="J285" s="6"/>
@@ -20274,12 +20255,12 @@
     </row>
     <row r="286">
       <c r="A286" s="90" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="B286" s="61" t="s">
-        <v>1147</v>
-      </c>
-      <c r="C286" s="139" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C286" s="131" t="s">
         <v>782</v>
       </c>
       <c r="D286" s="13"/>
@@ -20293,26 +20274,26 @@
     </row>
     <row r="287">
       <c r="A287" s="48" t="s">
-        <v>1148</v>
-      </c>
-      <c r="B287" s="168" t="s">
         <v>1149</v>
       </c>
-      <c r="C287" s="139" t="s">
+      <c r="B287" s="160" t="s">
         <v>1150</v>
       </c>
+      <c r="C287" s="131" t="s">
+        <v>1151</v>
+      </c>
       <c r="D287" s="13" t="s">
-        <v>1151</v>
-      </c>
-      <c r="E287" s="161" t="s">
         <v>1152</v>
+      </c>
+      <c r="E287" s="153" t="s">
+        <v>1153</v>
       </c>
       <c r="F287" s="6"/>
       <c r="G287" s="6" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="H287" s="87" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="I287" s="6"/>
       <c r="J287" s="6"/>
@@ -20423,22 +20404,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="170" t="s">
+      <c r="B1" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="170" t="s">
+      <c r="C1" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="170" t="s">
+      <c r="D1" s="162" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="170" t="s">
+      <c r="E1" s="162" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="170" t="s">
+      <c r="F1" s="162" t="s">
         <v>2</v>
       </c>
     </row>
@@ -20450,14 +20431,14 @@
         <v>422</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="87" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="F2" s="87" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="3">
@@ -20468,34 +20449,34 @@
         <v>422</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="87" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="F3" s="87" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="E4" s="87" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="F4" s="87" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="5">
@@ -20515,45 +20496,45 @@
         <v>777</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>843</v>
-      </c>
-      <c r="C6" s="171" t="s">
         <v>844</v>
+      </c>
+      <c r="C6" s="163" t="s">
+        <v>845</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="87" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="F6" s="87" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B7" s="87" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="E7" s="87" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="F7" s="87" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
     </row>
   </sheetData>
@@ -20576,108 +20557,108 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="172" t="s">
-        <v>1171</v>
-      </c>
-      <c r="B2" s="173" t="s">
+      <c r="A2" s="164" t="s">
         <v>1172</v>
       </c>
+      <c r="B2" s="165" t="s">
+        <v>1173</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="174" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B3" s="173" t="s">
+      <c r="A3" s="166" t="s">
         <v>1174</v>
       </c>
+      <c r="B3" s="165" t="s">
+        <v>1175</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="175" t="s">
-        <v>1175</v>
+      <c r="A4" s="167" t="s">
+        <v>1176</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="176" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B6" s="173" t="s">
+      <c r="A6" s="168" t="s">
         <v>1177</v>
       </c>
+      <c r="B6" s="165" t="s">
+        <v>1178</v>
+      </c>
     </row>
     <row r="7">
-      <c r="B7" s="173" t="s">
-        <v>1178</v>
+      <c r="B7" s="165" t="s">
+        <v>1179</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="173"/>
+      <c r="B8" s="165"/>
     </row>
     <row r="9">
-      <c r="B9" s="173"/>
+      <c r="B9" s="165"/>
     </row>
     <row r="10">
-      <c r="A10" s="176" t="s">
-        <v>1179</v>
+      <c r="A10" s="168" t="s">
+        <v>1180</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="176" t="s">
-        <v>1180</v>
-      </c>
-      <c r="B11" s="177" t="s">
+      <c r="A11" s="168" t="s">
         <v>1181</v>
       </c>
+      <c r="B11" s="169" t="s">
+        <v>1182</v>
+      </c>
     </row>
     <row r="12">
-      <c r="B12" s="178" t="s">
-        <v>1182</v>
+      <c r="B12" s="170" t="s">
+        <v>1183</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="179"/>
-      <c r="B13" s="180" t="s">
-        <v>1183</v>
+      <c r="A13" s="171"/>
+      <c r="B13" s="172" t="s">
+        <v>1184</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="181" t="s">
-        <v>1184</v>
+      <c r="B14" s="173" t="s">
+        <v>1185</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="182" t="s">
-        <v>1185</v>
+      <c r="B15" s="174" t="s">
+        <v>1186</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="183" t="s">
-        <v>1186</v>
+      <c r="B16" s="175" t="s">
+        <v>1187</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="176"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="28"/>
     </row>
     <row r="18">
-      <c r="A18" s="176" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B18" s="184" t="s">
+      <c r="A18" s="168" t="s">
         <v>1188</v>
+      </c>
+      <c r="B18" s="176" t="s">
+        <v>1189</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B19" s="81"/>
     </row>
     <row r="21">
-      <c r="A21" s="176" t="s">
-        <v>1190</v>
-      </c>
-      <c r="B21" s="185" t="s">
+      <c r="A21" s="168" t="s">
         <v>1191</v>
+      </c>
+      <c r="B21" s="177" t="s">
+        <v>1192</v>
       </c>
     </row>
   </sheetData>
@@ -20702,58 +20683,58 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="176" t="s">
-        <v>1192</v>
+      <c r="A1" s="168" t="s">
+        <v>1193</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="186" t="s">
-        <v>1193</v>
+      <c r="A2" s="178" t="s">
+        <v>1194</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="187" t="s">
-        <v>1194</v>
+      <c r="A3" s="179" t="s">
+        <v>1195</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="186" t="s">
-        <v>1195</v>
+      <c r="A4" s="178" t="s">
+        <v>1196</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="187" t="s">
-        <v>1196</v>
+      <c r="A5" s="179" t="s">
+        <v>1197</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="187" t="s">
-        <v>1197</v>
+      <c r="A6" s="179" t="s">
+        <v>1198</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="187" t="s">
-        <v>1198</v>
+      <c r="A7" s="179" t="s">
+        <v>1199</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="186" t="s">
-        <v>1199</v>
+      <c r="A8" s="178" t="s">
+        <v>1200</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="187" t="s">
-        <v>1200</v>
+      <c r="A9" s="179" t="s">
+        <v>1201</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="187" t="s">
-        <v>1201</v>
+      <c r="A10" s="179" t="s">
+        <v>1202</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="187" t="s">
-        <v>1202</v>
+      <c r="A11" s="179" t="s">
+        <v>1203</v>
       </c>
     </row>
   </sheetData>
@@ -20779,58 +20760,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1192</v>
-      </c>
-      <c r="B1" s="188" t="s">
-        <v>1203</v>
+        <v>1193</v>
+      </c>
+      <c r="B1" s="180" t="s">
+        <v>1204</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
     </row>
   </sheetData>
@@ -20849,7 +20830,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="177"/>
+      <c r="A1" s="169"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -20873,36 +20854,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="189" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C1" s="190" t="s">
+      <c r="A1" s="181" t="s">
         <v>1215</v>
+      </c>
+      <c r="C1" s="182" t="s">
+        <v>1216</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -20933,13 +20914,13 @@
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>1223</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>1221</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1222</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="1"/>
@@ -20970,13 +20951,13 @@
     </row>
     <row r="5">
       <c r="A5" s="39" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -21004,16 +20985,16 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -21040,16 +21021,16 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1222</v>
-      </c>
-      <c r="D7" s="191" t="s">
-        <v>1231</v>
+        <v>1223</v>
+      </c>
+      <c r="D7" s="183" t="s">
+        <v>1232</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -21076,16 +21057,16 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -21112,16 +21093,16 @@
     </row>
     <row r="9">
       <c r="A9" s="87" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -21148,16 +21129,16 @@
     </row>
     <row r="10">
       <c r="A10" s="87" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -21184,16 +21165,16 @@
     </row>
     <row r="11">
       <c r="A11" s="87" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -21220,16 +21201,16 @@
     </row>
     <row r="12">
       <c r="A12" s="87" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -21255,76 +21236,76 @@
       <c r="Z12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="192" t="s">
-        <v>1245</v>
-      </c>
-      <c r="B13" s="192" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C13" s="193" t="s">
-        <v>1222</v>
-      </c>
-      <c r="D13" s="193" t="s">
+      <c r="A13" s="184" t="s">
         <v>1246</v>
       </c>
-      <c r="E13" s="193"/>
-      <c r="F13" s="193"/>
-      <c r="G13" s="193"/>
-      <c r="H13" s="193"/>
-      <c r="I13" s="193"/>
-      <c r="J13" s="193"/>
-      <c r="K13" s="193"/>
-      <c r="L13" s="193"/>
-      <c r="M13" s="193"/>
-      <c r="N13" s="193"/>
-      <c r="O13" s="193"/>
-      <c r="P13" s="193"/>
-      <c r="Q13" s="193"/>
-      <c r="R13" s="193"/>
-      <c r="S13" s="193"/>
-      <c r="T13" s="193"/>
-      <c r="U13" s="193"/>
-      <c r="V13" s="193"/>
-      <c r="W13" s="193"/>
-      <c r="X13" s="193"/>
-      <c r="Y13" s="193"/>
-      <c r="Z13" s="193"/>
+      <c r="B13" s="184" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C13" s="185" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D13" s="185" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E13" s="185"/>
+      <c r="F13" s="185"/>
+      <c r="G13" s="185"/>
+      <c r="H13" s="185"/>
+      <c r="I13" s="185"/>
+      <c r="J13" s="185"/>
+      <c r="K13" s="185"/>
+      <c r="L13" s="185"/>
+      <c r="M13" s="185"/>
+      <c r="N13" s="185"/>
+      <c r="O13" s="185"/>
+      <c r="P13" s="185"/>
+      <c r="Q13" s="185"/>
+      <c r="R13" s="185"/>
+      <c r="S13" s="185"/>
+      <c r="T13" s="185"/>
+      <c r="U13" s="185"/>
+      <c r="V13" s="185"/>
+      <c r="W13" s="185"/>
+      <c r="X13" s="185"/>
+      <c r="Y13" s="185"/>
+      <c r="Z13" s="185"/>
     </row>
     <row r="14">
-      <c r="A14" s="192" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B14" s="192" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C14" s="193" t="s">
-        <v>1222</v>
-      </c>
-      <c r="D14" s="193" t="s">
+      <c r="A14" s="184" t="s">
         <v>1248</v>
       </c>
-      <c r="E14" s="193"/>
-      <c r="F14" s="193"/>
-      <c r="G14" s="193"/>
-      <c r="H14" s="193"/>
-      <c r="I14" s="193"/>
-      <c r="J14" s="193"/>
-      <c r="K14" s="193"/>
-      <c r="L14" s="193"/>
-      <c r="M14" s="193"/>
-      <c r="N14" s="193"/>
-      <c r="O14" s="193"/>
-      <c r="P14" s="193"/>
-      <c r="Q14" s="193"/>
-      <c r="R14" s="193"/>
-      <c r="S14" s="193"/>
-      <c r="T14" s="193"/>
-      <c r="U14" s="193"/>
-      <c r="V14" s="193"/>
-      <c r="W14" s="193"/>
-      <c r="X14" s="193"/>
-      <c r="Y14" s="193"/>
-      <c r="Z14" s="193"/>
+      <c r="B14" s="184" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C14" s="185" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D14" s="185" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E14" s="185"/>
+      <c r="F14" s="185"/>
+      <c r="G14" s="185"/>
+      <c r="H14" s="185"/>
+      <c r="I14" s="185"/>
+      <c r="J14" s="185"/>
+      <c r="K14" s="185"/>
+      <c r="L14" s="185"/>
+      <c r="M14" s="185"/>
+      <c r="N14" s="185"/>
+      <c r="O14" s="185"/>
+      <c r="P14" s="185"/>
+      <c r="Q14" s="185"/>
+      <c r="R14" s="185"/>
+      <c r="S14" s="185"/>
+      <c r="T14" s="185"/>
+      <c r="U14" s="185"/>
+      <c r="V14" s="185"/>
+      <c r="W14" s="185"/>
+      <c r="X14" s="185"/>
+      <c r="Y14" s="185"/>
+      <c r="Z14" s="185"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -21352,59 +21333,59 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="189" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C1" s="190" t="s">
+      <c r="A1" s="181" t="s">
         <v>1215</v>
+      </c>
+      <c r="C1" s="182" t="s">
+        <v>1216</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D2" s="188" t="s">
         <v>1219</v>
+      </c>
+      <c r="D2" s="180" t="s">
+        <v>1220</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C5" s="186" t="s">
         <v>1253</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>1254</v>
-      </c>
-      <c r="C5" s="194" t="s">
-        <v>1252</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for #323, including changes to the CM of F21, F22 and F23 (v.6.3.0)
</commit_message>
<xml_diff>
--- a/mappings/package_F21/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F21/transformation/conceptual_mappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="1259">
   <si>
     <t>Field</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.2.0</t>
+    <t>6.3.0</t>
   </si>
   <si>
     <r>
@@ -4578,7 +4578,11 @@
     <t>Time limit for receipt of tenders or requests to participate (Date/Time)</t>
   </si>
   <si>
-    <t>PROCEDURE/DATE_RECEIPT_TENDERS</t>
+    <t>PROCEDURE/DATE_RECEIPT_TENDERS
+PROCEDURE/TIME_RECEIPT_TENDERS</t>
+  </si>
+  <si>
+    <t>if(../NOTICE/@TYPE='CONTRACT' or ../NOTICE/@TYPE='PRI' or ../NOTICE/@TYPE='QSU_ONLY' or ../NOTICE/@TYPE='QSU_CALL_COMPETITION' or ../NOTICE/@TYPE='PER_ONLY')</t>
   </si>
   <si>
     <t>epo:Procedure / epo:SubmissionTerm / xsd:dateTime</t>
@@ -4623,16 +4627,10 @@
     </r>
   </si>
   <si>
-    <t>IV.2.2.1</t>
-  </si>
-  <si>
-    <t>Time limit for receipt of expressions of interest (Date/Time)</t>
-  </si>
-  <si>
-    <t>BT-630</t>
-  </si>
-  <si>
-    <t>PROCEDURE/TIME_RECEIPT_TENDERS</t>
+    <t>IV.2.3</t>
+  </si>
+  <si>
+    <t>if(../NOTICE/@TYPE='PRI_CALL_COMPETITION' or ../NOTICE/@TYPE='PER_CALL_COMPETITION')</t>
   </si>
   <si>
     <r>
@@ -8878,6 +8876,9 @@
     <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -8984,9 +8985,6 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -17397,40 +17395,44 @@
         <v>637</v>
       </c>
       <c r="D170" s="6"/>
-      <c r="E170" s="4" t="s">
+      <c r="E170" s="39" t="s">
         <v>721</v>
       </c>
-      <c r="F170" s="4"/>
+      <c r="F170" s="39" t="s">
+        <v>722</v>
+      </c>
       <c r="G170" s="39" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="H170" s="39" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="I170" s="6"/>
       <c r="J170" s="6"/>
       <c r="K170" s="6"/>
     </row>
     <row r="171">
-      <c r="A171" s="54" t="s">
-        <v>724</v>
-      </c>
-      <c r="B171" s="55" t="s">
+      <c r="A171" s="46" t="s">
         <v>725</v>
       </c>
+      <c r="B171" s="47" t="s">
+        <v>720</v>
+      </c>
       <c r="C171" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="D171" s="6"/>
+      <c r="E171" s="122" t="s">
+        <v>721</v>
+      </c>
+      <c r="F171" s="88" t="s">
         <v>726</v>
       </c>
-      <c r="D171" s="6"/>
-      <c r="E171" s="6" t="s">
+      <c r="G171" s="88" t="s">
+        <v>723</v>
+      </c>
+      <c r="H171" s="123" t="s">
         <v>727</v>
-      </c>
-      <c r="F171" s="6"/>
-      <c r="G171" s="88" t="s">
-        <v>722</v>
-      </c>
-      <c r="H171" s="122" t="s">
-        <v>728</v>
       </c>
       <c r="I171" s="6"/>
       <c r="J171" s="6"/>
@@ -17438,24 +17440,24 @@
     </row>
     <row r="172">
       <c r="A172" s="46" t="s">
+        <v>728</v>
+      </c>
+      <c r="B172" s="47" t="s">
         <v>729</v>
       </c>
-      <c r="B172" s="47" t="s">
+      <c r="C172" s="6" t="s">
         <v>730</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>731</v>
       </c>
       <c r="D172" s="4"/>
       <c r="E172" s="80" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F172" s="18"/>
       <c r="G172" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="H172" s="124" t="s">
         <v>733</v>
-      </c>
-      <c r="H172" s="123" t="s">
-        <v>734</v>
       </c>
       <c r="I172" s="6"/>
       <c r="J172" s="6"/>
@@ -17463,24 +17465,24 @@
     </row>
     <row r="173">
       <c r="A173" s="46" t="s">
+        <v>734</v>
+      </c>
+      <c r="B173" s="47" t="s">
         <v>735</v>
-      </c>
-      <c r="B173" s="47" t="s">
-        <v>736</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>637</v>
       </c>
       <c r="D173" s="6"/>
       <c r="E173" s="18" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F173" s="18"/>
       <c r="G173" s="88" t="s">
+        <v>737</v>
+      </c>
+      <c r="H173" s="88" t="s">
         <v>738</v>
-      </c>
-      <c r="H173" s="88" t="s">
-        <v>739</v>
       </c>
       <c r="I173" s="6"/>
       <c r="J173" s="6"/>
@@ -17488,10 +17490,10 @@
     </row>
     <row r="174">
       <c r="A174" s="48" t="s">
+        <v>739</v>
+      </c>
+      <c r="B174" s="47" t="s">
         <v>740</v>
-      </c>
-      <c r="B174" s="47" t="s">
-        <v>741</v>
       </c>
       <c r="C174" s="6"/>
       <c r="D174" s="6"/>
@@ -17505,26 +17507,26 @@
     </row>
     <row r="175">
       <c r="A175" s="94" t="s">
+        <v>741</v>
+      </c>
+      <c r="B175" s="55" t="s">
         <v>742</v>
       </c>
-      <c r="B175" s="55" t="s">
+      <c r="C175" s="13" t="s">
         <v>743</v>
       </c>
-      <c r="C175" s="13" t="s">
+      <c r="D175" s="13" t="s">
         <v>744</v>
       </c>
-      <c r="D175" s="13" t="s">
+      <c r="E175" s="49" t="s">
         <v>745</v>
-      </c>
-      <c r="E175" s="49" t="s">
-        <v>746</v>
       </c>
       <c r="F175" s="49"/>
       <c r="G175" s="36" t="s">
+        <v>746</v>
+      </c>
+      <c r="H175" s="36" t="s">
         <v>747</v>
-      </c>
-      <c r="H175" s="36" t="s">
-        <v>748</v>
       </c>
       <c r="I175" s="6"/>
       <c r="J175" s="6"/>
@@ -17532,74 +17534,74 @@
     </row>
     <row r="176">
       <c r="A176" s="117" t="s">
+        <v>748</v>
+      </c>
+      <c r="B176" s="34" t="s">
         <v>749</v>
-      </c>
-      <c r="B176" s="34" t="s">
-        <v>750</v>
       </c>
       <c r="C176" s="6"/>
       <c r="D176" s="6"/>
       <c r="E176" s="39" t="s">
+        <v>750</v>
+      </c>
+      <c r="F176" s="49" t="s">
         <v>751</v>
       </c>
-      <c r="F176" s="49" t="s">
+      <c r="G176" s="4" t="s">
         <v>752</v>
       </c>
-      <c r="G176" s="4" t="s">
+      <c r="H176" s="4" t="s">
         <v>753</v>
-      </c>
-      <c r="H176" s="4" t="s">
-        <v>754</v>
       </c>
       <c r="I176" s="6"/>
       <c r="J176" s="6"/>
       <c r="K176" s="6"/>
     </row>
     <row r="177">
-      <c r="A177" s="124" t="s">
+      <c r="A177" s="125" t="s">
+        <v>748</v>
+      </c>
+      <c r="B177" s="126" t="s">
         <v>749</v>
       </c>
-      <c r="B177" s="125" t="s">
+      <c r="C177" s="127"/>
+      <c r="D177" s="127"/>
+      <c r="E177" s="56" t="s">
         <v>750</v>
       </c>
-      <c r="C177" s="126"/>
-      <c r="D177" s="126"/>
-      <c r="E177" s="56" t="s">
+      <c r="F177" s="40" t="s">
         <v>751</v>
       </c>
-      <c r="F177" s="40" t="s">
-        <v>752</v>
-      </c>
       <c r="G177" s="40" t="s">
+        <v>754</v>
+      </c>
+      <c r="H177" s="128" t="s">
         <v>755</v>
-      </c>
-      <c r="H177" s="127" t="s">
-        <v>756</v>
       </c>
       <c r="I177" s="6"/>
       <c r="J177" s="6"/>
       <c r="K177" s="6" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="124" t="s">
+      <c r="A178" s="125" t="s">
+        <v>748</v>
+      </c>
+      <c r="B178" s="126" t="s">
         <v>749</v>
-      </c>
-      <c r="B178" s="125" t="s">
-        <v>750</v>
       </c>
       <c r="C178" s="13"/>
       <c r="D178" s="13"/>
-      <c r="E178" s="128" t="s">
-        <v>751</v>
+      <c r="E178" s="129" t="s">
+        <v>750</v>
       </c>
       <c r="F178" s="36"/>
       <c r="G178" s="36" t="s">
+        <v>757</v>
+      </c>
+      <c r="H178" s="36" t="s">
         <v>758</v>
-      </c>
-      <c r="H178" s="36" t="s">
-        <v>759</v>
       </c>
       <c r="I178" s="6"/>
       <c r="J178" s="6"/>
@@ -17607,28 +17609,28 @@
     </row>
     <row r="179">
       <c r="A179" s="48" t="s">
+        <v>759</v>
+      </c>
+      <c r="B179" s="47" t="s">
         <v>760</v>
       </c>
-      <c r="B179" s="47" t="s">
+      <c r="C179" s="13" t="s">
         <v>761</v>
       </c>
-      <c r="C179" s="13" t="s">
+      <c r="D179" s="13" t="s">
         <v>762</v>
       </c>
-      <c r="D179" s="13" t="s">
+      <c r="E179" s="49" t="s">
         <v>763</v>
       </c>
-      <c r="E179" s="49" t="s">
+      <c r="F179" s="49" t="s">
+        <v>751</v>
+      </c>
+      <c r="G179" s="4" t="s">
         <v>764</v>
       </c>
-      <c r="F179" s="49" t="s">
-        <v>752</v>
-      </c>
-      <c r="G179" s="4" t="s">
+      <c r="H179" s="4" t="s">
         <v>765</v>
-      </c>
-      <c r="H179" s="4" t="s">
-        <v>766</v>
       </c>
       <c r="I179" s="6" t="s">
         <v>71</v>
@@ -17638,28 +17640,28 @@
     </row>
     <row r="180">
       <c r="A180" s="48" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B180" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C180" s="36" t="s">
+        <v>767</v>
+      </c>
+      <c r="D180" s="13" t="s">
         <v>768</v>
       </c>
-      <c r="D180" s="13" t="s">
+      <c r="E180" s="49" t="s">
         <v>769</v>
       </c>
-      <c r="E180" s="49" t="s">
+      <c r="F180" s="49" t="s">
+        <v>751</v>
+      </c>
+      <c r="G180" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="F180" s="49" t="s">
-        <v>752</v>
-      </c>
-      <c r="G180" s="4" t="s">
+      <c r="H180" s="105" t="s">
         <v>771</v>
-      </c>
-      <c r="H180" s="105" t="s">
-        <v>772</v>
       </c>
       <c r="I180" s="6" t="s">
         <v>63</v>
@@ -17669,53 +17671,53 @@
     </row>
     <row r="181">
       <c r="A181" s="48" t="s">
+        <v>772</v>
+      </c>
+      <c r="B181" s="47" t="s">
         <v>773</v>
       </c>
-      <c r="B181" s="47" t="s">
+      <c r="C181" s="13" t="s">
         <v>774</v>
       </c>
-      <c r="C181" s="13" t="s">
+      <c r="D181" s="13" t="s">
         <v>775</v>
       </c>
-      <c r="D181" s="13" t="s">
+      <c r="E181" s="39" t="s">
         <v>776</v>
-      </c>
-      <c r="E181" s="39" t="s">
-        <v>777</v>
       </c>
       <c r="F181" s="4"/>
       <c r="G181" s="4" t="s">
+        <v>777</v>
+      </c>
+      <c r="H181" s="39" t="s">
         <v>778</v>
-      </c>
-      <c r="H181" s="39" t="s">
-        <v>779</v>
       </c>
       <c r="I181" s="6"/>
       <c r="J181" s="6"/>
       <c r="K181" s="6"/>
     </row>
     <row r="182">
-      <c r="A182" s="129" t="s">
+      <c r="A182" s="130" t="s">
+        <v>772</v>
+      </c>
+      <c r="B182" s="131" t="s">
         <v>773</v>
       </c>
-      <c r="B182" s="130" t="s">
+      <c r="C182" s="113" t="s">
         <v>774</v>
       </c>
-      <c r="C182" s="113" t="s">
+      <c r="D182" s="113" t="s">
         <v>775</v>
       </c>
-      <c r="D182" s="113" t="s">
-        <v>776</v>
-      </c>
       <c r="E182" s="39" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F182" s="4"/>
       <c r="G182" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="H182" s="124" t="s">
         <v>781</v>
-      </c>
-      <c r="H182" s="123" t="s">
-        <v>782</v>
       </c>
       <c r="I182" s="6"/>
       <c r="J182" s="6"/>
@@ -17723,13 +17725,13 @@
     </row>
     <row r="183">
       <c r="A183" s="91" t="s">
+        <v>782</v>
+      </c>
+      <c r="B183" s="38" t="s">
         <v>783</v>
       </c>
-      <c r="B183" s="38" t="s">
+      <c r="C183" s="132" t="s">
         <v>784</v>
-      </c>
-      <c r="C183" s="131" t="s">
-        <v>785</v>
       </c>
       <c r="D183" s="13"/>
       <c r="E183" s="4"/>
@@ -17742,13 +17744,13 @@
     </row>
     <row r="184">
       <c r="A184" s="48" t="s">
+        <v>785</v>
+      </c>
+      <c r="B184" s="47" t="s">
         <v>786</v>
       </c>
-      <c r="B184" s="47" t="s">
-        <v>787</v>
-      </c>
-      <c r="C184" s="131" t="s">
-        <v>785</v>
+      <c r="C184" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D184" s="13"/>
       <c r="E184" s="36"/>
@@ -17761,26 +17763,26 @@
     </row>
     <row r="185">
       <c r="A185" s="94" t="s">
+        <v>787</v>
+      </c>
+      <c r="B185" s="55" t="s">
         <v>788</v>
       </c>
-      <c r="B185" s="55" t="s">
+      <c r="C185" s="13" t="s">
         <v>789</v>
       </c>
-      <c r="C185" s="13" t="s">
+      <c r="D185" s="13" t="s">
         <v>790</v>
       </c>
-      <c r="D185" s="13" t="s">
+      <c r="E185" s="49" t="s">
         <v>791</v>
-      </c>
-      <c r="E185" s="49" t="s">
-        <v>792</v>
       </c>
       <c r="F185" s="49"/>
       <c r="G185" s="36" t="s">
+        <v>792</v>
+      </c>
+      <c r="H185" s="104" t="s">
         <v>793</v>
-      </c>
-      <c r="H185" s="104" t="s">
-        <v>794</v>
       </c>
       <c r="I185" s="6"/>
       <c r="J185" s="6"/>
@@ -17788,26 +17790,26 @@
     </row>
     <row r="186">
       <c r="A186" s="94" t="s">
+        <v>794</v>
+      </c>
+      <c r="B186" s="55" t="s">
         <v>795</v>
       </c>
-      <c r="B186" s="55" t="s">
+      <c r="C186" s="13" t="s">
+        <v>789</v>
+      </c>
+      <c r="D186" s="13" t="s">
+        <v>790</v>
+      </c>
+      <c r="E186" s="49" t="s">
         <v>796</v>
-      </c>
-      <c r="C186" s="13" t="s">
-        <v>790</v>
-      </c>
-      <c r="D186" s="13" t="s">
-        <v>791</v>
-      </c>
-      <c r="E186" s="49" t="s">
-        <v>797</v>
       </c>
       <c r="F186" s="49"/>
       <c r="G186" s="4" t="s">
-        <v>793</v>
-      </c>
-      <c r="H186" s="123" t="s">
-        <v>798</v>
+        <v>792</v>
+      </c>
+      <c r="H186" s="124" t="s">
+        <v>797</v>
       </c>
       <c r="I186" s="6"/>
       <c r="J186" s="6"/>
@@ -17815,24 +17817,24 @@
     </row>
     <row r="187">
       <c r="A187" s="94" t="s">
+        <v>798</v>
+      </c>
+      <c r="B187" s="55" t="s">
         <v>799</v>
       </c>
-      <c r="B187" s="55" t="s">
-        <v>800</v>
-      </c>
-      <c r="C187" s="132" t="s">
+      <c r="C187" s="133" t="s">
         <v>637</v>
       </c>
       <c r="D187" s="13"/>
       <c r="E187" s="40" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F187" s="40"/>
       <c r="G187" s="40" t="s">
+        <v>801</v>
+      </c>
+      <c r="H187" s="40" t="s">
         <v>802</v>
-      </c>
-      <c r="H187" s="40" t="s">
-        <v>803</v>
       </c>
       <c r="I187" s="6"/>
       <c r="J187" s="6"/>
@@ -17840,13 +17842,13 @@
     </row>
     <row r="188">
       <c r="A188" s="91" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B188" s="38" t="s">
-        <v>750</v>
-      </c>
-      <c r="C188" s="131" t="s">
-        <v>785</v>
+        <v>749</v>
+      </c>
+      <c r="C188" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D188" s="13"/>
       <c r="E188" s="36"/>
@@ -17859,20 +17861,20 @@
     </row>
     <row r="189">
       <c r="A189" s="94" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B189" s="55"/>
       <c r="C189" s="13"/>
       <c r="D189" s="6"/>
       <c r="E189" s="56" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F189" s="49"/>
       <c r="G189" s="36" t="s">
+        <v>805</v>
+      </c>
+      <c r="H189" s="104" t="s">
         <v>806</v>
-      </c>
-      <c r="H189" s="104" t="s">
-        <v>807</v>
       </c>
       <c r="I189" s="6"/>
       <c r="J189" s="6"/>
@@ -17880,49 +17882,49 @@
     </row>
     <row r="190">
       <c r="A190" s="94" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B190" s="89"/>
       <c r="C190" s="36"/>
       <c r="D190" s="6"/>
       <c r="E190" s="56" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F190" s="49"/>
       <c r="G190" s="36" t="s">
+        <v>807</v>
+      </c>
+      <c r="H190" s="49" t="s">
         <v>808</v>
-      </c>
-      <c r="H190" s="49" t="s">
-        <v>809</v>
       </c>
       <c r="I190" s="6"/>
       <c r="J190" s="6"/>
       <c r="K190" s="6" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="48" t="s">
+        <v>810</v>
+      </c>
+      <c r="B191" s="47" t="s">
         <v>811</v>
       </c>
-      <c r="B191" s="47" t="s">
+      <c r="C191" s="13" t="s">
         <v>812</v>
       </c>
-      <c r="C191" s="13" t="s">
+      <c r="D191" s="13" t="s">
         <v>813</v>
       </c>
-      <c r="D191" s="13" t="s">
+      <c r="E191" s="49" t="s">
         <v>814</v>
-      </c>
-      <c r="E191" s="49" t="s">
-        <v>815</v>
       </c>
       <c r="F191" s="49"/>
       <c r="G191" s="39" t="s">
+        <v>815</v>
+      </c>
+      <c r="H191" s="124" t="s">
         <v>816</v>
-      </c>
-      <c r="H191" s="123" t="s">
-        <v>817</v>
       </c>
       <c r="I191" s="6"/>
       <c r="J191" s="6"/>
@@ -17930,51 +17932,51 @@
     </row>
     <row r="192">
       <c r="A192" s="48" t="s">
+        <v>817</v>
+      </c>
+      <c r="B192" s="47" t="s">
         <v>818</v>
       </c>
-      <c r="B192" s="47" t="s">
+      <c r="C192" s="134"/>
+      <c r="D192" s="134"/>
+      <c r="E192" s="56" t="s">
+        <v>776</v>
+      </c>
+      <c r="F192" s="135"/>
+      <c r="G192" s="49" t="s">
         <v>819</v>
       </c>
-      <c r="C192" s="133"/>
-      <c r="D192" s="133"/>
-      <c r="E192" s="56" t="s">
-        <v>777</v>
-      </c>
-      <c r="F192" s="134"/>
-      <c r="G192" s="49" t="s">
+      <c r="H192" s="36" t="s">
         <v>820</v>
       </c>
-      <c r="H192" s="36" t="s">
+      <c r="I192" s="6" t="s">
         <v>821</v>
-      </c>
-      <c r="I192" s="6" t="s">
-        <v>822</v>
       </c>
       <c r="J192" s="6"/>
       <c r="K192" s="6"/>
     </row>
     <row r="193">
       <c r="A193" s="94" t="s">
+        <v>822</v>
+      </c>
+      <c r="B193" s="55" t="s">
         <v>823</v>
       </c>
-      <c r="B193" s="55" t="s">
+      <c r="C193" s="13" t="s">
         <v>824</v>
       </c>
-      <c r="C193" s="13" t="s">
+      <c r="D193" s="13" t="s">
         <v>825</v>
       </c>
-      <c r="D193" s="13" t="s">
+      <c r="E193" s="49" t="s">
         <v>826</v>
-      </c>
-      <c r="E193" s="49" t="s">
-        <v>827</v>
       </c>
       <c r="F193" s="49"/>
       <c r="G193" s="36" t="s">
+        <v>827</v>
+      </c>
+      <c r="H193" s="36" t="s">
         <v>828</v>
-      </c>
-      <c r="H193" s="36" t="s">
-        <v>829</v>
       </c>
       <c r="I193" s="6"/>
       <c r="J193" s="6"/>
@@ -17982,22 +17984,22 @@
     </row>
     <row r="194">
       <c r="A194" s="94" t="s">
+        <v>829</v>
+      </c>
+      <c r="B194" s="55" t="s">
         <v>830</v>
-      </c>
-      <c r="B194" s="55" t="s">
-        <v>831</v>
       </c>
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
       <c r="E194" s="49" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F194" s="49"/>
       <c r="G194" s="4" t="s">
+        <v>832</v>
+      </c>
+      <c r="H194" s="39" t="s">
         <v>833</v>
-      </c>
-      <c r="H194" s="39" t="s">
-        <v>834</v>
       </c>
       <c r="I194" s="6"/>
       <c r="J194" s="6"/>
@@ -18005,22 +18007,22 @@
     </row>
     <row r="195">
       <c r="A195" s="94" t="s">
+        <v>834</v>
+      </c>
+      <c r="B195" s="55" t="s">
         <v>835</v>
-      </c>
-      <c r="B195" s="55" t="s">
-        <v>836</v>
       </c>
       <c r="C195" s="13"/>
       <c r="D195" s="13"/>
       <c r="E195" s="49" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F195" s="63"/>
       <c r="G195" s="4" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H195" s="39" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="I195" s="6"/>
       <c r="J195" s="6"/>
@@ -18028,22 +18030,22 @@
     </row>
     <row r="196">
       <c r="A196" s="94" t="s">
+        <v>838</v>
+      </c>
+      <c r="B196" s="55" t="s">
         <v>839</v>
-      </c>
-      <c r="B196" s="55" t="s">
-        <v>840</v>
       </c>
       <c r="C196" s="13"/>
       <c r="D196" s="13"/>
       <c r="E196" s="49" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F196" s="49"/>
       <c r="G196" s="4" t="s">
-        <v>833</v>
-      </c>
-      <c r="H196" s="123" t="s">
-        <v>842</v>
+        <v>832</v>
+      </c>
+      <c r="H196" s="124" t="s">
+        <v>841</v>
       </c>
       <c r="I196" s="6"/>
       <c r="J196" s="6"/>
@@ -18051,22 +18053,22 @@
     </row>
     <row r="197">
       <c r="A197" s="94" t="s">
+        <v>842</v>
+      </c>
+      <c r="B197" s="55" t="s">
         <v>843</v>
-      </c>
-      <c r="B197" s="55" t="s">
-        <v>844</v>
       </c>
       <c r="C197" s="13"/>
       <c r="D197" s="13"/>
       <c r="E197" s="49" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F197" s="49"/>
       <c r="G197" s="4" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H197" s="121" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="I197" s="6"/>
       <c r="J197" s="6"/>
@@ -18074,17 +18076,17 @@
     </row>
     <row r="198">
       <c r="A198" s="94" t="s">
+        <v>846</v>
+      </c>
+      <c r="B198" s="55" t="s">
         <v>847</v>
       </c>
-      <c r="B198" s="55" t="s">
+      <c r="C198" s="136" t="s">
         <v>848</v>
-      </c>
-      <c r="C198" s="135" t="s">
-        <v>849</v>
       </c>
       <c r="D198" s="13"/>
       <c r="E198" s="49" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F198" s="39"/>
       <c r="G198" s="36" t="s">
@@ -18099,13 +18101,13 @@
     </row>
     <row r="199">
       <c r="A199" s="48" t="s">
+        <v>850</v>
+      </c>
+      <c r="B199" s="47" t="s">
         <v>851</v>
       </c>
-      <c r="B199" s="47" t="s">
-        <v>852</v>
-      </c>
-      <c r="C199" s="131" t="s">
-        <v>785</v>
+      <c r="C199" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D199" s="13"/>
       <c r="E199" s="39"/>
@@ -18118,7 +18120,7 @@
     </row>
     <row r="200">
       <c r="A200" s="94" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B200" s="55" t="s">
         <v>57</v>
@@ -18130,14 +18132,14 @@
         <v>59</v>
       </c>
       <c r="E200" s="49" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F200" s="49"/>
       <c r="G200" s="43" t="s">
         <v>61</v>
       </c>
       <c r="H200" s="43" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="I200" s="6" t="s">
         <v>63</v>
@@ -18147,7 +18149,7 @@
     </row>
     <row r="201">
       <c r="A201" s="94" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B201" s="55" t="s">
         <v>65</v>
@@ -18159,14 +18161,14 @@
         <v>67</v>
       </c>
       <c r="E201" s="49" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F201" s="49"/>
       <c r="G201" s="45" t="s">
         <v>69</v>
       </c>
       <c r="H201" s="45" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I201" s="6" t="s">
         <v>71</v>
@@ -18176,7 +18178,7 @@
     </row>
     <row r="202">
       <c r="A202" s="94" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B202" s="55" t="s">
         <v>73</v>
@@ -18188,14 +18190,14 @@
         <v>75</v>
       </c>
       <c r="E202" s="49" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="F202" s="49"/>
       <c r="G202" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H202" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="I202" s="6"/>
       <c r="J202" s="6"/>
@@ -18203,7 +18205,7 @@
     </row>
     <row r="203">
       <c r="A203" s="94" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B203" s="55" t="s">
         <v>80</v>
@@ -18214,15 +18216,15 @@
       <c r="D203" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E203" s="136" t="s">
-        <v>863</v>
-      </c>
-      <c r="F203" s="136"/>
+      <c r="E203" s="137" t="s">
+        <v>862</v>
+      </c>
+      <c r="F203" s="137"/>
       <c r="G203" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H203" s="39" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="I203" s="6"/>
       <c r="J203" s="6"/>
@@ -18230,7 +18232,7 @@
     </row>
     <row r="204">
       <c r="A204" s="94" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B204" s="55" t="s">
         <v>86</v>
@@ -18242,16 +18244,16 @@
         <v>88</v>
       </c>
       <c r="E204" s="80" t="s">
+        <v>865</v>
+      </c>
+      <c r="F204" s="80" t="s">
         <v>866</v>
-      </c>
-      <c r="F204" s="80" t="s">
-        <v>867</v>
       </c>
       <c r="G204" s="36" t="s">
         <v>91</v>
       </c>
       <c r="H204" s="49" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I204" s="6"/>
       <c r="J204" s="6"/>
@@ -18259,26 +18261,26 @@
     </row>
     <row r="205">
       <c r="A205" s="94" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B205" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C205" s="137" t="s">
+      <c r="C205" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="D205" s="137" t="s">
+      <c r="D205" s="138" t="s">
+        <v>869</v>
+      </c>
+      <c r="E205" s="137" t="s">
         <v>870</v>
       </c>
-      <c r="E205" s="136" t="s">
-        <v>871</v>
-      </c>
-      <c r="F205" s="136"/>
+      <c r="F205" s="137"/>
       <c r="G205" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H205" s="39" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I205" s="6"/>
       <c r="J205" s="6"/>
@@ -18286,7 +18288,7 @@
     </row>
     <row r="206">
       <c r="A206" s="94" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B206" s="55" t="s">
         <v>101</v>
@@ -18297,15 +18299,15 @@
       <c r="D206" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E206" s="136" t="s">
-        <v>874</v>
-      </c>
-      <c r="F206" s="136"/>
+      <c r="E206" s="137" t="s">
+        <v>873</v>
+      </c>
+      <c r="F206" s="137"/>
       <c r="G206" s="78" t="s">
         <v>105</v>
       </c>
       <c r="H206" s="78" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="I206" s="6"/>
       <c r="J206" s="6"/>
@@ -18313,7 +18315,7 @@
     </row>
     <row r="207">
       <c r="A207" s="94" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B207" s="55" t="s">
         <v>121</v>
@@ -18324,15 +18326,15 @@
       <c r="D207" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E207" s="136" t="s">
+      <c r="E207" s="137" t="s">
+        <v>876</v>
+      </c>
+      <c r="F207" s="137"/>
+      <c r="G207" s="63" t="s">
         <v>877</v>
       </c>
-      <c r="F207" s="136"/>
-      <c r="G207" s="63" t="s">
+      <c r="H207" s="63" t="s">
         <v>878</v>
-      </c>
-      <c r="H207" s="63" t="s">
-        <v>879</v>
       </c>
       <c r="I207" s="6"/>
       <c r="J207" s="6"/>
@@ -18340,7 +18342,7 @@
     </row>
     <row r="208">
       <c r="A208" s="94" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B208" s="55" t="s">
         <v>115</v>
@@ -18351,15 +18353,15 @@
       <c r="D208" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E208" s="136" t="s">
+      <c r="E208" s="137" t="s">
+        <v>880</v>
+      </c>
+      <c r="F208" s="137"/>
+      <c r="G208" s="49" t="s">
         <v>881</v>
       </c>
-      <c r="F208" s="136"/>
-      <c r="G208" s="49" t="s">
+      <c r="H208" s="49" t="s">
         <v>882</v>
-      </c>
-      <c r="H208" s="49" t="s">
-        <v>883</v>
       </c>
       <c r="I208" s="6"/>
       <c r="J208" s="6"/>
@@ -18367,10 +18369,10 @@
     </row>
     <row r="209">
       <c r="A209" s="94" t="s">
+        <v>883</v>
+      </c>
+      <c r="B209" s="55" t="s">
         <v>884</v>
-      </c>
-      <c r="B209" s="55" t="s">
-        <v>885</v>
       </c>
       <c r="C209" s="13" t="s">
         <v>137</v>
@@ -18378,15 +18380,15 @@
       <c r="D209" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E209" s="136" t="s">
+      <c r="E209" s="137" t="s">
+        <v>885</v>
+      </c>
+      <c r="F209" s="137"/>
+      <c r="G209" s="45" t="s">
+        <v>877</v>
+      </c>
+      <c r="H209" s="45" t="s">
         <v>886</v>
-      </c>
-      <c r="F209" s="136"/>
-      <c r="G209" s="45" t="s">
-        <v>878</v>
-      </c>
-      <c r="H209" s="45" t="s">
-        <v>887</v>
       </c>
       <c r="I209" s="6"/>
       <c r="J209" s="6"/>
@@ -18394,7 +18396,7 @@
     </row>
     <row r="210">
       <c r="A210" s="94" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B210" s="55" t="s">
         <v>128</v>
@@ -18405,15 +18407,15 @@
       <c r="D210" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E210" s="136" t="s">
+      <c r="E210" s="137" t="s">
+        <v>888</v>
+      </c>
+      <c r="F210" s="137"/>
+      <c r="G210" s="49" t="s">
+        <v>881</v>
+      </c>
+      <c r="H210" s="49" t="s">
         <v>889</v>
-      </c>
-      <c r="F210" s="136"/>
-      <c r="G210" s="49" t="s">
-        <v>882</v>
-      </c>
-      <c r="H210" s="49" t="s">
-        <v>890</v>
       </c>
       <c r="I210" s="6"/>
       <c r="J210" s="6"/>
@@ -18421,26 +18423,26 @@
     </row>
     <row r="211">
       <c r="A211" s="94" t="s">
+        <v>890</v>
+      </c>
+      <c r="B211" s="55" t="s">
         <v>891</v>
       </c>
-      <c r="B211" s="55" t="s">
+      <c r="C211" s="13" t="s">
         <v>892</v>
       </c>
-      <c r="C211" s="13" t="s">
+      <c r="D211" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="D211" s="13" t="s">
+      <c r="E211" s="137" t="s">
         <v>894</v>
-      </c>
-      <c r="E211" s="136" t="s">
-        <v>895</v>
       </c>
       <c r="F211" s="80"/>
       <c r="G211" s="4" t="s">
+        <v>895</v>
+      </c>
+      <c r="H211" s="139" t="s">
         <v>896</v>
-      </c>
-      <c r="H211" s="138" t="s">
-        <v>897</v>
       </c>
       <c r="I211" s="6"/>
       <c r="J211" s="6"/>
@@ -18451,15 +18453,15 @@
       <c r="B212" s="4"/>
       <c r="C212" s="13"/>
       <c r="D212" s="13"/>
-      <c r="E212" s="139" t="s">
-        <v>895</v>
+      <c r="E212" s="140" t="s">
+        <v>894</v>
       </c>
       <c r="F212" s="80"/>
       <c r="G212" s="78" t="s">
+        <v>897</v>
+      </c>
+      <c r="H212" s="78" t="s">
         <v>898</v>
-      </c>
-      <c r="H212" s="78" t="s">
-        <v>899</v>
       </c>
       <c r="I212" s="6"/>
       <c r="J212" s="6"/>
@@ -18467,13 +18469,13 @@
     </row>
     <row r="213">
       <c r="A213" s="48" t="s">
+        <v>899</v>
+      </c>
+      <c r="B213" s="47" t="s">
         <v>900</v>
       </c>
-      <c r="B213" s="47" t="s">
-        <v>901</v>
-      </c>
-      <c r="C213" s="131" t="s">
-        <v>785</v>
+      <c r="C213" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D213" s="13"/>
       <c r="E213" s="36"/>
@@ -18486,10 +18488,10 @@
     </row>
     <row r="214">
       <c r="A214" s="94" t="s">
+        <v>901</v>
+      </c>
+      <c r="B214" s="55" t="s">
         <v>902</v>
-      </c>
-      <c r="B214" s="55" t="s">
-        <v>903</v>
       </c>
       <c r="C214" s="13" t="s">
         <v>526</v>
@@ -18497,15 +18499,15 @@
       <c r="D214" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="E214" s="136" t="s">
-        <v>904</v>
-      </c>
-      <c r="F214" s="136"/>
+      <c r="E214" s="137" t="s">
+        <v>903</v>
+      </c>
+      <c r="F214" s="137"/>
       <c r="G214" s="36" t="s">
         <v>528</v>
       </c>
       <c r="H214" s="49" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I214" s="6"/>
       <c r="J214" s="6"/>
@@ -18513,24 +18515,24 @@
     </row>
     <row r="215">
       <c r="A215" s="108" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B215" s="75" t="s">
         <v>416</v>
       </c>
-      <c r="C215" s="140" t="s">
+      <c r="C215" s="141" t="s">
         <v>232</v>
       </c>
-      <c r="D215" s="141"/>
-      <c r="E215" s="136" t="s">
+      <c r="D215" s="142"/>
+      <c r="E215" s="137" t="s">
+        <v>906</v>
+      </c>
+      <c r="F215" s="137"/>
+      <c r="G215" s="36" t="s">
         <v>907</v>
       </c>
-      <c r="F215" s="136"/>
-      <c r="G215" s="36" t="s">
+      <c r="H215" s="49" t="s">
         <v>908</v>
-      </c>
-      <c r="H215" s="49" t="s">
-        <v>909</v>
       </c>
       <c r="I215" s="6"/>
       <c r="J215" s="6"/>
@@ -18538,26 +18540,26 @@
     </row>
     <row r="216">
       <c r="A216" s="94" t="s">
+        <v>909</v>
+      </c>
+      <c r="B216" s="55" t="s">
         <v>910</v>
       </c>
-      <c r="B216" s="55" t="s">
+      <c r="C216" s="142" t="s">
         <v>911</v>
       </c>
-      <c r="C216" s="141" t="s">
+      <c r="D216" s="142" t="s">
         <v>912</v>
       </c>
-      <c r="D216" s="141" t="s">
+      <c r="E216" s="137" t="s">
         <v>913</v>
       </c>
-      <c r="E216" s="136" t="s">
+      <c r="F216" s="137"/>
+      <c r="G216" s="4" t="s">
         <v>914</v>
       </c>
-      <c r="F216" s="136"/>
-      <c r="G216" s="4" t="s">
+      <c r="H216" s="39" t="s">
         <v>915</v>
-      </c>
-      <c r="H216" s="39" t="s">
-        <v>916</v>
       </c>
       <c r="I216" s="6"/>
       <c r="J216" s="6"/>
@@ -18565,24 +18567,24 @@
     </row>
     <row r="217">
       <c r="A217" s="108" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B217" s="75" t="s">
         <v>416</v>
       </c>
-      <c r="C217" s="140" t="s">
+      <c r="C217" s="141" t="s">
         <v>232</v>
       </c>
-      <c r="D217" s="141"/>
-      <c r="E217" s="136" t="s">
+      <c r="D217" s="142"/>
+      <c r="E217" s="137" t="s">
+        <v>917</v>
+      </c>
+      <c r="F217" s="137"/>
+      <c r="G217" s="4" t="s">
         <v>918</v>
       </c>
-      <c r="F217" s="136"/>
-      <c r="G217" s="4" t="s">
+      <c r="H217" s="39" t="s">
         <v>919</v>
-      </c>
-      <c r="H217" s="39" t="s">
-        <v>920</v>
       </c>
       <c r="I217" s="6"/>
       <c r="J217" s="6"/>
@@ -18590,26 +18592,26 @@
     </row>
     <row r="218">
       <c r="A218" s="94" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B218" s="55" t="s">
         <v>463</v>
       </c>
-      <c r="C218" s="141" t="s">
+      <c r="C218" s="142" t="s">
         <v>464</v>
       </c>
-      <c r="D218" s="141" t="s">
+      <c r="D218" s="142" t="s">
         <v>465</v>
       </c>
-      <c r="E218" s="136" t="s">
+      <c r="E218" s="137" t="s">
+        <v>921</v>
+      </c>
+      <c r="F218" s="137"/>
+      <c r="G218" s="36" t="s">
         <v>922</v>
       </c>
-      <c r="F218" s="136"/>
-      <c r="G218" s="36" t="s">
+      <c r="H218" s="49" t="s">
         <v>923</v>
-      </c>
-      <c r="H218" s="49" t="s">
-        <v>924</v>
       </c>
       <c r="I218" s="6"/>
       <c r="J218" s="6"/>
@@ -18617,24 +18619,24 @@
     </row>
     <row r="219">
       <c r="A219" s="108" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B219" s="75" t="s">
         <v>416</v>
       </c>
-      <c r="C219" s="140" t="s">
+      <c r="C219" s="141" t="s">
         <v>232</v>
       </c>
-      <c r="D219" s="141"/>
-      <c r="E219" s="136" t="s">
+      <c r="D219" s="142"/>
+      <c r="E219" s="137" t="s">
+        <v>925</v>
+      </c>
+      <c r="F219" s="137"/>
+      <c r="G219" s="36" t="s">
         <v>926</v>
       </c>
-      <c r="F219" s="136"/>
-      <c r="G219" s="36" t="s">
+      <c r="H219" s="49" t="s">
         <v>927</v>
-      </c>
-      <c r="H219" s="49" t="s">
-        <v>928</v>
       </c>
       <c r="I219" s="6"/>
       <c r="J219" s="6"/>
@@ -18642,26 +18644,26 @@
     </row>
     <row r="220">
       <c r="A220" s="94" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B220" s="55" t="s">
         <v>469</v>
       </c>
-      <c r="C220" s="141" t="s">
+      <c r="C220" s="142" t="s">
         <v>470</v>
       </c>
-      <c r="D220" s="141" t="s">
+      <c r="D220" s="142" t="s">
         <v>471</v>
       </c>
-      <c r="E220" s="136" t="s">
+      <c r="E220" s="137" t="s">
+        <v>929</v>
+      </c>
+      <c r="F220" s="137"/>
+      <c r="G220" s="36" t="s">
+        <v>922</v>
+      </c>
+      <c r="H220" s="49" t="s">
         <v>930</v>
-      </c>
-      <c r="F220" s="136"/>
-      <c r="G220" s="36" t="s">
-        <v>923</v>
-      </c>
-      <c r="H220" s="49" t="s">
-        <v>931</v>
       </c>
       <c r="I220" s="6"/>
       <c r="J220" s="6"/>
@@ -18669,24 +18671,24 @@
     </row>
     <row r="221">
       <c r="A221" s="108" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B221" s="75" t="s">
         <v>416</v>
       </c>
-      <c r="C221" s="142" t="s">
+      <c r="C221" s="143" t="s">
         <v>232</v>
       </c>
       <c r="D221" s="13"/>
-      <c r="E221" s="139" t="s">
+      <c r="E221" s="140" t="s">
+        <v>925</v>
+      </c>
+      <c r="F221" s="137"/>
+      <c r="G221" s="13" t="s">
         <v>926</v>
       </c>
-      <c r="F221" s="136"/>
-      <c r="G221" s="13" t="s">
-        <v>927</v>
-      </c>
       <c r="H221" s="63" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="I221" s="6"/>
       <c r="J221" s="6"/>
@@ -18694,17 +18696,17 @@
     </row>
     <row r="222">
       <c r="A222" s="48" t="s">
+        <v>933</v>
+      </c>
+      <c r="B222" s="64" t="s">
         <v>934</v>
       </c>
-      <c r="B222" s="64" t="s">
-        <v>935</v>
-      </c>
-      <c r="C222" s="131" t="s">
-        <v>785</v>
+      <c r="C222" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D222" s="13"/>
-      <c r="E222" s="141"/>
-      <c r="F222" s="141"/>
+      <c r="E222" s="142"/>
+      <c r="F222" s="142"/>
       <c r="G222" s="4"/>
       <c r="H222" s="4"/>
       <c r="I222" s="6"/>
@@ -18713,26 +18715,26 @@
     </row>
     <row r="223">
       <c r="A223" s="94" t="s">
+        <v>935</v>
+      </c>
+      <c r="B223" s="90" t="s">
         <v>936</v>
       </c>
-      <c r="B223" s="90" t="s">
+      <c r="C223" s="13" t="s">
         <v>937</v>
       </c>
-      <c r="C223" s="13" t="s">
+      <c r="D223" s="13" t="s">
         <v>938</v>
       </c>
-      <c r="D223" s="13" t="s">
+      <c r="E223" s="49" t="s">
         <v>939</v>
-      </c>
-      <c r="E223" s="49" t="s">
-        <v>940</v>
       </c>
       <c r="F223" s="63"/>
       <c r="G223" s="49" t="s">
+        <v>940</v>
+      </c>
+      <c r="H223" s="65" t="s">
         <v>941</v>
-      </c>
-      <c r="H223" s="65" t="s">
-        <v>942</v>
       </c>
       <c r="I223" s="6"/>
       <c r="J223" s="6"/>
@@ -18740,10 +18742,10 @@
     </row>
     <row r="224">
       <c r="A224" s="94" t="s">
+        <v>942</v>
+      </c>
+      <c r="B224" s="90" t="s">
         <v>943</v>
-      </c>
-      <c r="B224" s="90" t="s">
-        <v>944</v>
       </c>
       <c r="C224" s="6"/>
       <c r="D224" s="6"/>
@@ -18757,26 +18759,26 @@
     </row>
     <row r="225">
       <c r="A225" s="94" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B225" s="90" t="s">
         <v>409</v>
       </c>
       <c r="C225" s="63" t="s">
+        <v>945</v>
+      </c>
+      <c r="D225" s="63" t="s">
         <v>946</v>
       </c>
-      <c r="D225" s="63" t="s">
+      <c r="E225" s="137" t="s">
         <v>947</v>
       </c>
-      <c r="E225" s="136" t="s">
+      <c r="F225" s="137"/>
+      <c r="G225" s="36" t="s">
         <v>948</v>
       </c>
-      <c r="F225" s="136"/>
-      <c r="G225" s="36" t="s">
+      <c r="H225" s="49" t="s">
         <v>949</v>
-      </c>
-      <c r="H225" s="49" t="s">
-        <v>950</v>
       </c>
       <c r="I225" s="6"/>
       <c r="J225" s="6"/>
@@ -18784,24 +18786,24 @@
     </row>
     <row r="226">
       <c r="A226" s="94" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B226" s="90" t="s">
         <v>416</v>
       </c>
-      <c r="C226" s="142" t="s">
+      <c r="C226" s="143" t="s">
         <v>232</v>
       </c>
       <c r="D226" s="13"/>
-      <c r="E226" s="136" t="s">
+      <c r="E226" s="137" t="s">
+        <v>951</v>
+      </c>
+      <c r="F226" s="137"/>
+      <c r="G226" s="63" t="s">
         <v>952</v>
       </c>
-      <c r="F226" s="136"/>
-      <c r="G226" s="63" t="s">
+      <c r="H226" s="13" t="s">
         <v>953</v>
-      </c>
-      <c r="H226" s="13" t="s">
-        <v>954</v>
       </c>
       <c r="I226" s="6"/>
       <c r="J226" s="6"/>
@@ -18809,26 +18811,26 @@
     </row>
     <row r="227">
       <c r="A227" s="94" t="s">
+        <v>954</v>
+      </c>
+      <c r="B227" s="90" t="s">
         <v>955</v>
       </c>
-      <c r="B227" s="90" t="s">
+      <c r="C227" s="13" t="s">
         <v>956</v>
       </c>
-      <c r="C227" s="13" t="s">
+      <c r="D227" s="13" t="s">
         <v>957</v>
       </c>
-      <c r="D227" s="13" t="s">
+      <c r="E227" s="137" t="s">
         <v>958</v>
       </c>
-      <c r="E227" s="136" t="s">
+      <c r="F227" s="137"/>
+      <c r="G227" s="49" t="s">
         <v>959</v>
       </c>
-      <c r="F227" s="136"/>
-      <c r="G227" s="49" t="s">
+      <c r="H227" s="49" t="s">
         <v>960</v>
-      </c>
-      <c r="H227" s="49" t="s">
-        <v>961</v>
       </c>
       <c r="I227" s="6"/>
       <c r="J227" s="6"/>
@@ -18836,26 +18838,26 @@
     </row>
     <row r="228">
       <c r="A228" s="94" t="s">
+        <v>961</v>
+      </c>
+      <c r="B228" s="90" t="s">
         <v>962</v>
       </c>
-      <c r="B228" s="90" t="s">
+      <c r="C228" s="13" t="s">
         <v>963</v>
       </c>
-      <c r="C228" s="13" t="s">
+      <c r="D228" s="13" t="s">
         <v>964</v>
       </c>
-      <c r="D228" s="13" t="s">
+      <c r="E228" s="137" t="s">
         <v>965</v>
       </c>
-      <c r="E228" s="136" t="s">
+      <c r="F228" s="137"/>
+      <c r="G228" s="63" t="s">
         <v>966</v>
       </c>
-      <c r="F228" s="136"/>
-      <c r="G228" s="63" t="s">
+      <c r="H228" s="63" t="s">
         <v>967</v>
-      </c>
-      <c r="H228" s="63" t="s">
-        <v>968</v>
       </c>
       <c r="I228" s="6" t="s">
         <v>63</v>
@@ -18865,10 +18867,10 @@
     </row>
     <row r="229">
       <c r="A229" s="117" t="s">
+        <v>968</v>
+      </c>
+      <c r="B229" s="144" t="s">
         <v>969</v>
-      </c>
-      <c r="B229" s="143" t="s">
-        <v>970</v>
       </c>
       <c r="C229" s="6"/>
       <c r="D229" s="6"/>
@@ -18882,15 +18884,15 @@
     </row>
     <row r="230">
       <c r="A230" s="37" t="s">
+        <v>970</v>
+      </c>
+      <c r="B230" s="61" t="s">
         <v>971</v>
-      </c>
-      <c r="B230" s="61" t="s">
-        <v>972</v>
       </c>
       <c r="C230" s="98"/>
       <c r="D230" s="83"/>
-      <c r="E230" s="144"/>
-      <c r="F230" s="141"/>
+      <c r="E230" s="145"/>
+      <c r="F230" s="142"/>
       <c r="G230" s="63"/>
       <c r="H230" s="63"/>
       <c r="I230" s="6"/>
@@ -18899,24 +18901,24 @@
     </row>
     <row r="231">
       <c r="A231" s="46" t="s">
+        <v>972</v>
+      </c>
+      <c r="B231" s="64" t="s">
         <v>973</v>
       </c>
-      <c r="B231" s="64" t="s">
+      <c r="C231" s="98" t="s">
         <v>974</v>
       </c>
-      <c r="C231" s="98" t="s">
+      <c r="D231" s="83"/>
+      <c r="E231" s="145" t="s">
         <v>975</v>
       </c>
-      <c r="D231" s="83"/>
-      <c r="E231" s="144" t="s">
+      <c r="F231" s="142"/>
+      <c r="G231" s="4" t="s">
         <v>976</v>
       </c>
-      <c r="F231" s="141"/>
-      <c r="G231" s="4" t="s">
+      <c r="H231" s="105" t="s">
         <v>977</v>
-      </c>
-      <c r="H231" s="105" t="s">
-        <v>978</v>
       </c>
       <c r="I231" s="6"/>
       <c r="J231" s="6"/>
@@ -18924,24 +18926,24 @@
     </row>
     <row r="232">
       <c r="A232" s="46" t="s">
+        <v>978</v>
+      </c>
+      <c r="B232" s="64" t="s">
         <v>979</v>
       </c>
-      <c r="B232" s="64" t="s">
+      <c r="C232" s="98" t="s">
         <v>980</v>
       </c>
-      <c r="C232" s="98" t="s">
+      <c r="D232" s="83"/>
+      <c r="E232" s="145" t="s">
         <v>981</v>
       </c>
-      <c r="D232" s="83"/>
-      <c r="E232" s="144" t="s">
+      <c r="F232" s="142"/>
+      <c r="G232" s="4" t="s">
+        <v>976</v>
+      </c>
+      <c r="H232" s="105" t="s">
         <v>982</v>
-      </c>
-      <c r="F232" s="141"/>
-      <c r="G232" s="4" t="s">
-        <v>977</v>
-      </c>
-      <c r="H232" s="105" t="s">
-        <v>983</v>
       </c>
       <c r="I232" s="6"/>
       <c r="J232" s="6"/>
@@ -18949,24 +18951,24 @@
     </row>
     <row r="233">
       <c r="A233" s="46" t="s">
+        <v>983</v>
+      </c>
+      <c r="B233" s="64" t="s">
         <v>984</v>
       </c>
-      <c r="B233" s="64" t="s">
+      <c r="C233" s="98" t="s">
         <v>985</v>
       </c>
-      <c r="C233" s="98" t="s">
+      <c r="D233" s="83"/>
+      <c r="E233" s="145" t="s">
         <v>986</v>
       </c>
-      <c r="D233" s="83"/>
-      <c r="E233" s="144" t="s">
+      <c r="F233" s="142"/>
+      <c r="G233" s="4" t="s">
+        <v>976</v>
+      </c>
+      <c r="H233" s="105" t="s">
         <v>987</v>
-      </c>
-      <c r="F233" s="141"/>
-      <c r="G233" s="4" t="s">
-        <v>977</v>
-      </c>
-      <c r="H233" s="105" t="s">
-        <v>988</v>
       </c>
       <c r="I233" s="6"/>
       <c r="J233" s="6"/>
@@ -18974,7 +18976,7 @@
     </row>
     <row r="234">
       <c r="A234" s="91" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B234" s="61" t="s">
         <v>582</v>
@@ -18985,15 +18987,15 @@
       <c r="D234" s="6" t="s">
         <v>584</v>
       </c>
-      <c r="E234" s="136" t="s">
+      <c r="E234" s="137" t="s">
+        <v>989</v>
+      </c>
+      <c r="F234" s="137"/>
+      <c r="G234" s="146" t="s">
+        <v>372</v>
+      </c>
+      <c r="H234" s="147" t="s">
         <v>990</v>
-      </c>
-      <c r="F234" s="136"/>
-      <c r="G234" s="145" t="s">
-        <v>372</v>
-      </c>
-      <c r="H234" s="146" t="s">
-        <v>991</v>
       </c>
       <c r="I234" s="6" t="s">
         <v>63</v>
@@ -19003,17 +19005,17 @@
     </row>
     <row r="235">
       <c r="A235" s="91" t="s">
+        <v>991</v>
+      </c>
+      <c r="B235" s="61" t="s">
         <v>992</v>
       </c>
-      <c r="B235" s="61" t="s">
-        <v>993</v>
-      </c>
-      <c r="C235" s="131" t="s">
-        <v>785</v>
+      <c r="C235" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D235" s="6"/>
-      <c r="E235" s="141"/>
-      <c r="F235" s="141"/>
+      <c r="E235" s="142"/>
+      <c r="F235" s="142"/>
       <c r="G235" s="6"/>
       <c r="H235" s="6"/>
       <c r="I235" s="6"/>
@@ -19022,17 +19024,17 @@
     </row>
     <row r="236">
       <c r="A236" s="48" t="s">
+        <v>993</v>
+      </c>
+      <c r="B236" s="64" t="s">
         <v>994</v>
       </c>
-      <c r="B236" s="64" t="s">
-        <v>995</v>
-      </c>
-      <c r="C236" s="147" t="s">
-        <v>785</v>
+      <c r="C236" s="148" t="s">
+        <v>784</v>
       </c>
       <c r="D236" s="6"/>
       <c r="E236" s="88" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="F236" s="63"/>
       <c r="G236" s="13" t="s">
@@ -19047,7 +19049,7 @@
     </row>
     <row r="237">
       <c r="A237" s="94" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B237" s="90" t="s">
         <v>57</v>
@@ -19059,14 +19061,14 @@
         <v>59</v>
       </c>
       <c r="E237" s="63" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F237" s="63"/>
       <c r="G237" s="88" t="s">
         <v>61</v>
       </c>
       <c r="H237" s="88" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I237" s="6" t="s">
         <v>63</v>
@@ -19076,7 +19078,7 @@
     </row>
     <row r="238">
       <c r="A238" s="94" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B238" s="90" t="s">
         <v>73</v>
@@ -19088,14 +19090,14 @@
         <v>75</v>
       </c>
       <c r="E238" s="63" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F238" s="63"/>
       <c r="G238" s="88" t="s">
         <v>77</v>
       </c>
       <c r="H238" s="88" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="I238" s="6"/>
       <c r="J238" s="6"/>
@@ -19103,7 +19105,7 @@
     </row>
     <row r="239">
       <c r="A239" s="94" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B239" s="90" t="s">
         <v>80</v>
@@ -19115,14 +19117,14 @@
         <v>82</v>
       </c>
       <c r="E239" s="63" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F239" s="63"/>
       <c r="G239" s="88" t="s">
         <v>77</v>
       </c>
       <c r="H239" s="88" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="I239" s="6"/>
       <c r="J239" s="6"/>
@@ -19130,7 +19132,7 @@
     </row>
     <row r="240">
       <c r="A240" s="94" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B240" s="90" t="s">
         <v>94</v>
@@ -19139,17 +19141,17 @@
         <v>95</v>
       </c>
       <c r="D240" s="13" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E240" s="63" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F240" s="63"/>
       <c r="G240" s="88" t="s">
         <v>98</v>
       </c>
       <c r="H240" s="88" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="I240" s="6"/>
       <c r="J240" s="6"/>
@@ -19157,7 +19159,7 @@
     </row>
     <row r="241">
       <c r="A241" s="94" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B241" s="90" t="s">
         <v>101</v>
@@ -19169,14 +19171,14 @@
         <v>103</v>
       </c>
       <c r="E241" s="63" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F241" s="63"/>
       <c r="G241" s="63" t="s">
         <v>105</v>
       </c>
       <c r="H241" s="63" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="I241" s="6"/>
       <c r="J241" s="6"/>
@@ -19184,7 +19186,7 @@
     </row>
     <row r="242">
       <c r="A242" s="94" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B242" s="90" t="s">
         <v>121</v>
@@ -19196,14 +19198,14 @@
         <v>123</v>
       </c>
       <c r="E242" s="63" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F242" s="63"/>
       <c r="G242" s="63" t="s">
+        <v>877</v>
+      </c>
+      <c r="H242" s="63" t="s">
         <v>878</v>
-      </c>
-      <c r="H242" s="63" t="s">
-        <v>879</v>
       </c>
       <c r="I242" s="6"/>
       <c r="J242" s="6"/>
@@ -19211,7 +19213,7 @@
     </row>
     <row r="243">
       <c r="A243" s="94" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B243" s="90" t="s">
         <v>115</v>
@@ -19223,14 +19225,14 @@
         <v>117</v>
       </c>
       <c r="E243" s="63" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F243" s="63"/>
       <c r="G243" s="63" t="s">
+        <v>881</v>
+      </c>
+      <c r="H243" s="63" t="s">
         <v>882</v>
-      </c>
-      <c r="H243" s="63" t="s">
-        <v>883</v>
       </c>
       <c r="I243" s="6"/>
       <c r="J243" s="6"/>
@@ -19238,10 +19240,10 @@
     </row>
     <row r="244">
       <c r="A244" s="94" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B244" s="90" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C244" s="13" t="s">
         <v>137</v>
@@ -19250,14 +19252,14 @@
         <v>138</v>
       </c>
       <c r="E244" s="63" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F244" s="63"/>
       <c r="G244" s="60" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H244" s="60" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I244" s="6"/>
       <c r="J244" s="6"/>
@@ -19265,7 +19267,7 @@
     </row>
     <row r="245">
       <c r="A245" s="94" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B245" s="90" t="s">
         <v>128</v>
@@ -19277,14 +19279,14 @@
         <v>130</v>
       </c>
       <c r="E245" s="63" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F245" s="63"/>
       <c r="G245" s="63" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H245" s="63" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I245" s="6"/>
       <c r="J245" s="6"/>
@@ -19292,21 +19294,21 @@
     </row>
     <row r="246">
       <c r="A246" s="48" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B246" s="64" t="s">
         <v>1021</v>
       </c>
-      <c r="B246" s="64" t="s">
+      <c r="C246" s="148" t="s">
+        <v>784</v>
+      </c>
+      <c r="D246" s="149"/>
+      <c r="E246" s="88" t="s">
         <v>1022</v>
-      </c>
-      <c r="C246" s="147" t="s">
-        <v>785</v>
-      </c>
-      <c r="D246" s="148"/>
-      <c r="E246" s="88" t="s">
-        <v>1023</v>
       </c>
       <c r="F246" s="13"/>
       <c r="G246" s="13" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H246" s="13" t="s">
         <v>234</v>
@@ -19317,7 +19319,7 @@
     </row>
     <row r="247">
       <c r="A247" s="94" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B247" s="90" t="s">
         <v>57</v>
@@ -19329,14 +19331,14 @@
         <v>59</v>
       </c>
       <c r="E247" s="63" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F247" s="63"/>
       <c r="G247" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="H247" s="122" t="s">
-        <v>1027</v>
+      <c r="H247" s="123" t="s">
+        <v>1026</v>
       </c>
       <c r="I247" s="6" t="s">
         <v>63</v>
@@ -19346,7 +19348,7 @@
     </row>
     <row r="248">
       <c r="A248" s="94" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B248" s="90" t="s">
         <v>73</v>
@@ -19358,14 +19360,14 @@
         <v>75</v>
       </c>
       <c r="E248" s="63" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F248" s="63"/>
       <c r="G248" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="H248" s="122" t="s">
-        <v>1030</v>
+      <c r="H248" s="123" t="s">
+        <v>1029</v>
       </c>
       <c r="I248" s="6"/>
       <c r="J248" s="6"/>
@@ -19373,7 +19375,7 @@
     </row>
     <row r="249">
       <c r="A249" s="94" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B249" s="90" t="s">
         <v>80</v>
@@ -19385,14 +19387,14 @@
         <v>82</v>
       </c>
       <c r="E249" s="63" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F249" s="63"/>
       <c r="G249" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="H249" s="122" t="s">
-        <v>1033</v>
+      <c r="H249" s="123" t="s">
+        <v>1032</v>
       </c>
       <c r="I249" s="6"/>
       <c r="J249" s="6"/>
@@ -19400,7 +19402,7 @@
     </row>
     <row r="250">
       <c r="A250" s="94" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B250" s="90" t="s">
         <v>94</v>
@@ -19409,17 +19411,17 @@
         <v>95</v>
       </c>
       <c r="D250" s="13" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E250" s="63" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F250" s="63"/>
       <c r="G250" s="88" t="s">
         <v>98</v>
       </c>
       <c r="H250" s="88" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I250" s="6"/>
       <c r="J250" s="6"/>
@@ -19427,7 +19429,7 @@
     </row>
     <row r="251">
       <c r="A251" s="94" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B251" s="90" t="s">
         <v>101</v>
@@ -19439,14 +19441,14 @@
         <v>103</v>
       </c>
       <c r="E251" s="63" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F251" s="63"/>
       <c r="G251" s="88" t="s">
         <v>105</v>
       </c>
-      <c r="H251" s="122" t="s">
-        <v>1039</v>
+      <c r="H251" s="123" t="s">
+        <v>1038</v>
       </c>
       <c r="I251" s="6"/>
       <c r="J251" s="6"/>
@@ -19454,7 +19456,7 @@
     </row>
     <row r="252">
       <c r="A252" s="94" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B252" s="90" t="s">
         <v>121</v>
@@ -19466,14 +19468,14 @@
         <v>123</v>
       </c>
       <c r="E252" s="63" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F252" s="63"/>
       <c r="G252" s="63" t="s">
+        <v>877</v>
+      </c>
+      <c r="H252" s="150" t="s">
         <v>878</v>
-      </c>
-      <c r="H252" s="149" t="s">
-        <v>879</v>
       </c>
       <c r="I252" s="6"/>
       <c r="J252" s="6"/>
@@ -19481,7 +19483,7 @@
     </row>
     <row r="253">
       <c r="A253" s="94" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B253" s="90" t="s">
         <v>115</v>
@@ -19493,14 +19495,14 @@
         <v>117</v>
       </c>
       <c r="E253" s="63" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F253" s="63"/>
       <c r="G253" s="63" t="s">
+        <v>881</v>
+      </c>
+      <c r="H253" s="63" t="s">
         <v>882</v>
-      </c>
-      <c r="H253" s="63" t="s">
-        <v>883</v>
       </c>
       <c r="I253" s="6"/>
       <c r="J253" s="6"/>
@@ -19508,10 +19510,10 @@
     </row>
     <row r="254">
       <c r="A254" s="94" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B254" s="90" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C254" s="13" t="s">
         <v>137</v>
@@ -19520,14 +19522,14 @@
         <v>138</v>
       </c>
       <c r="E254" s="63" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F254" s="63"/>
       <c r="G254" s="60" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H254" s="60" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="I254" s="6"/>
       <c r="J254" s="6"/>
@@ -19535,7 +19537,7 @@
     </row>
     <row r="255">
       <c r="A255" s="94" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B255" s="90" t="s">
         <v>128</v>
@@ -19547,14 +19549,14 @@
         <v>130</v>
       </c>
       <c r="E255" s="63" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="F255" s="63"/>
       <c r="G255" s="63" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H255" s="63" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I255" s="6"/>
       <c r="J255" s="6"/>
@@ -19562,26 +19564,26 @@
     </row>
     <row r="256">
       <c r="A256" s="48" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B256" s="64" t="s">
         <v>1049</v>
       </c>
-      <c r="B256" s="64" t="s">
+      <c r="C256" s="13" t="s">
         <v>1050</v>
       </c>
-      <c r="C256" s="13" t="s">
+      <c r="D256" s="13" t="s">
         <v>1051</v>
       </c>
-      <c r="D256" s="13" t="s">
+      <c r="E256" s="63" t="s">
         <v>1052</v>
-      </c>
-      <c r="E256" s="63" t="s">
-        <v>1053</v>
       </c>
       <c r="F256" s="63"/>
       <c r="G256" s="88" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H256" s="147" t="s">
         <v>1054</v>
-      </c>
-      <c r="H256" s="146" t="s">
-        <v>1055</v>
       </c>
       <c r="I256" s="6"/>
       <c r="J256" s="6"/>
@@ -19589,21 +19591,21 @@
     </row>
     <row r="257">
       <c r="A257" s="48" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B257" s="64" t="s">
         <v>1056</v>
-      </c>
-      <c r="B257" s="64" t="s">
-        <v>1057</v>
       </c>
       <c r="C257" s="6"/>
       <c r="D257" s="6"/>
       <c r="E257" s="88" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="F257" s="13"/>
       <c r="G257" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H257" s="150" t="s">
+      <c r="H257" s="151" t="s">
         <v>234</v>
       </c>
       <c r="I257" s="6"/>
@@ -19612,7 +19614,7 @@
     </row>
     <row r="258">
       <c r="A258" s="94" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B258" s="90" t="s">
         <v>57</v>
@@ -19624,14 +19626,14 @@
         <v>59</v>
       </c>
       <c r="E258" s="63" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F258" s="63"/>
       <c r="G258" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="H258" s="122" t="s">
-        <v>1061</v>
+      <c r="H258" s="123" t="s">
+        <v>1060</v>
       </c>
       <c r="I258" s="6" t="s">
         <v>63</v>
@@ -19641,7 +19643,7 @@
     </row>
     <row r="259">
       <c r="A259" s="94" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B259" s="90" t="s">
         <v>73</v>
@@ -19653,14 +19655,14 @@
         <v>75</v>
       </c>
       <c r="E259" s="63" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F259" s="63"/>
       <c r="G259" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="H259" s="122" t="s">
-        <v>1064</v>
+      <c r="H259" s="123" t="s">
+        <v>1063</v>
       </c>
       <c r="I259" s="6"/>
       <c r="J259" s="6"/>
@@ -19668,7 +19670,7 @@
     </row>
     <row r="260">
       <c r="A260" s="94" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B260" s="90" t="s">
         <v>80</v>
@@ -19680,14 +19682,14 @@
         <v>82</v>
       </c>
       <c r="E260" s="63" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F260" s="63"/>
       <c r="G260" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="H260" s="122" t="s">
-        <v>1067</v>
+      <c r="H260" s="123" t="s">
+        <v>1066</v>
       </c>
       <c r="I260" s="6"/>
       <c r="J260" s="6"/>
@@ -19695,7 +19697,7 @@
     </row>
     <row r="261">
       <c r="A261" s="94" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B261" s="90" t="s">
         <v>94</v>
@@ -19704,17 +19706,17 @@
         <v>95</v>
       </c>
       <c r="D261" s="13" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E261" s="63" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F261" s="63"/>
       <c r="G261" s="88" t="s">
         <v>98</v>
       </c>
       <c r="H261" s="88" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I261" s="6"/>
       <c r="J261" s="6"/>
@@ -19722,7 +19724,7 @@
     </row>
     <row r="262">
       <c r="A262" s="94" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B262" s="90" t="s">
         <v>101</v>
@@ -19734,14 +19736,14 @@
         <v>103</v>
       </c>
       <c r="E262" s="63" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="F262" s="63"/>
       <c r="G262" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="H262" s="149" t="s">
-        <v>1073</v>
+      <c r="H262" s="150" t="s">
+        <v>1072</v>
       </c>
       <c r="I262" s="6"/>
       <c r="J262" s="6"/>
@@ -19749,7 +19751,7 @@
     </row>
     <row r="263">
       <c r="A263" s="94" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B263" s="90" t="s">
         <v>121</v>
@@ -19761,14 +19763,14 @@
         <v>123</v>
       </c>
       <c r="E263" s="63" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F263" s="63"/>
       <c r="G263" s="63" t="s">
+        <v>877</v>
+      </c>
+      <c r="H263" s="150" t="s">
         <v>878</v>
-      </c>
-      <c r="H263" s="149" t="s">
-        <v>879</v>
       </c>
       <c r="I263" s="6"/>
       <c r="J263" s="6"/>
@@ -19776,7 +19778,7 @@
     </row>
     <row r="264">
       <c r="A264" s="94" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B264" s="90" t="s">
         <v>115</v>
@@ -19788,14 +19790,14 @@
         <v>117</v>
       </c>
       <c r="E264" s="63" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F264" s="63"/>
       <c r="G264" s="63" t="s">
+        <v>881</v>
+      </c>
+      <c r="H264" s="150" t="s">
         <v>882</v>
-      </c>
-      <c r="H264" s="149" t="s">
-        <v>883</v>
       </c>
       <c r="I264" s="6"/>
       <c r="J264" s="6"/>
@@ -19803,10 +19805,10 @@
     </row>
     <row r="265">
       <c r="A265" s="94" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B265" s="90" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C265" s="13" t="s">
         <v>137</v>
@@ -19815,14 +19817,14 @@
         <v>138</v>
       </c>
       <c r="E265" s="63" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F265" s="63"/>
       <c r="G265" s="60" t="s">
-        <v>878</v>
-      </c>
-      <c r="H265" s="151" t="s">
-        <v>1080</v>
+        <v>877</v>
+      </c>
+      <c r="H265" s="152" t="s">
+        <v>1079</v>
       </c>
       <c r="I265" s="6"/>
       <c r="J265" s="6"/>
@@ -19830,7 +19832,7 @@
     </row>
     <row r="266">
       <c r="A266" s="94" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B266" s="90" t="s">
         <v>128</v>
@@ -19842,14 +19844,14 @@
         <v>130</v>
       </c>
       <c r="E266" s="63" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F266" s="63"/>
       <c r="G266" s="63" t="s">
-        <v>882</v>
-      </c>
-      <c r="H266" s="149" t="s">
-        <v>890</v>
+        <v>881</v>
+      </c>
+      <c r="H266" s="150" t="s">
+        <v>889</v>
       </c>
       <c r="I266" s="6"/>
       <c r="J266" s="6"/>
@@ -19857,26 +19859,26 @@
     </row>
     <row r="267">
       <c r="A267" s="91" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B267" s="61" t="s">
         <v>1083</v>
       </c>
-      <c r="B267" s="61" t="s">
+      <c r="C267" s="153" t="s">
         <v>1084</v>
       </c>
-      <c r="C267" s="152" t="s">
+      <c r="D267" s="153" t="s">
         <v>1085</v>
       </c>
-      <c r="D267" s="152" t="s">
+      <c r="E267" s="154" t="s">
         <v>1086</v>
       </c>
-      <c r="E267" s="153" t="s">
+      <c r="F267" s="154"/>
+      <c r="G267" s="88" t="s">
         <v>1087</v>
       </c>
-      <c r="F267" s="153"/>
-      <c r="G267" s="88" t="s">
+      <c r="H267" s="155" t="s">
         <v>1088</v>
-      </c>
-      <c r="H267" s="154" t="s">
-        <v>1089</v>
       </c>
       <c r="I267" s="6"/>
       <c r="J267" s="6"/>
@@ -19884,10 +19886,10 @@
     </row>
     <row r="268">
       <c r="A268" s="117" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B268" s="144" t="s">
         <v>1090</v>
-      </c>
-      <c r="B268" s="143" t="s">
-        <v>1091</v>
       </c>
       <c r="C268" s="6"/>
       <c r="D268" s="6"/>
@@ -19901,17 +19903,17 @@
     </row>
     <row r="269">
       <c r="A269" s="91" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B269" s="61" t="s">
         <v>1092</v>
       </c>
-      <c r="B269" s="61" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C269" s="131" t="s">
-        <v>785</v>
+      <c r="C269" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D269" s="13"/>
       <c r="E269" s="63" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="F269" s="6"/>
       <c r="G269" s="6"/>
@@ -19922,16 +19924,16 @@
     </row>
     <row r="270">
       <c r="A270" s="48" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B270" s="64" t="s">
         <v>1095</v>
       </c>
-      <c r="B270" s="64" t="s">
+      <c r="C270" s="132" t="s">
         <v>1096</v>
       </c>
-      <c r="C270" s="131" t="s">
+      <c r="D270" s="13" t="s">
         <v>1097</v>
-      </c>
-      <c r="D270" s="13" t="s">
-        <v>1098</v>
       </c>
       <c r="E270" s="88"/>
       <c r="F270" s="6"/>
@@ -19943,53 +19945,53 @@
     </row>
     <row r="271">
       <c r="A271" s="94" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B271" s="90" t="s">
         <v>662</v>
       </c>
       <c r="C271" s="13" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D271" s="13" t="s">
         <v>1100</v>
       </c>
-      <c r="D271" s="13" t="s">
+      <c r="E271" s="63" t="s">
         <v>1101</v>
-      </c>
-      <c r="E271" s="63" t="s">
-        <v>1102</v>
       </c>
       <c r="F271" s="13"/>
       <c r="G271" s="88" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H271" s="123" t="s">
         <v>1103</v>
-      </c>
-      <c r="H271" s="122" t="s">
-        <v>1104</v>
       </c>
       <c r="I271" s="6"/>
       <c r="J271" s="6"/>
       <c r="K271" s="6"/>
     </row>
     <row r="272">
-      <c r="A272" s="155" t="s">
+      <c r="A272" s="156" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B272" s="157" t="s">
+        <v>662</v>
+      </c>
+      <c r="C272" s="158" t="s">
         <v>1099</v>
       </c>
-      <c r="B272" s="156" t="s">
-        <v>662</v>
-      </c>
-      <c r="C272" s="157" t="s">
+      <c r="D272" s="158" t="s">
         <v>1100</v>
       </c>
-      <c r="D272" s="157" t="s">
+      <c r="E272" s="122" t="s">
         <v>1101</v>
-      </c>
-      <c r="E272" s="158" t="s">
-        <v>1102</v>
       </c>
       <c r="F272" s="13"/>
       <c r="G272" s="6" t="s">
+        <v>1104</v>
+      </c>
+      <c r="H272" s="123" t="s">
         <v>1105</v>
-      </c>
-      <c r="H272" s="122" t="s">
-        <v>1106</v>
       </c>
       <c r="I272" s="6"/>
       <c r="J272" s="6"/>
@@ -19997,53 +19999,53 @@
     </row>
     <row r="273">
       <c r="A273" s="94" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B273" s="90" t="s">
         <v>1107</v>
       </c>
-      <c r="B273" s="90" t="s">
+      <c r="C273" s="13" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D273" s="13" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E273" s="63" t="s">
         <v>1108</v>
-      </c>
-      <c r="C273" s="13" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D273" s="13" t="s">
-        <v>1101</v>
-      </c>
-      <c r="E273" s="63" t="s">
-        <v>1109</v>
       </c>
       <c r="F273" s="13"/>
       <c r="G273" s="88" t="s">
-        <v>1103</v>
-      </c>
-      <c r="H273" s="122" t="s">
-        <v>1110</v>
+        <v>1102</v>
+      </c>
+      <c r="H273" s="123" t="s">
+        <v>1109</v>
       </c>
       <c r="I273" s="6"/>
       <c r="J273" s="6"/>
       <c r="K273" s="6"/>
     </row>
     <row r="274">
-      <c r="A274" s="155" t="s">
+      <c r="A274" s="156" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B274" s="157" t="s">
         <v>1107</v>
       </c>
-      <c r="B274" s="156" t="s">
+      <c r="C274" s="158" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D274" s="158" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E274" s="122" t="s">
         <v>1108</v>
-      </c>
-      <c r="C274" s="157" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D274" s="157" t="s">
-        <v>1101</v>
-      </c>
-      <c r="E274" s="158" t="s">
-        <v>1109</v>
       </c>
       <c r="F274" s="13"/>
       <c r="G274" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H274" s="122" t="s">
-        <v>1111</v>
+        <v>1104</v>
+      </c>
+      <c r="H274" s="123" t="s">
+        <v>1110</v>
       </c>
       <c r="I274" s="6"/>
       <c r="J274" s="6"/>
@@ -20051,13 +20053,13 @@
     </row>
     <row r="275">
       <c r="A275" s="48" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B275" s="64" t="s">
         <v>1112</v>
       </c>
-      <c r="B275" s="64" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C275" s="131" t="s">
-        <v>785</v>
+      <c r="C275" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D275" s="13"/>
       <c r="E275" s="13"/>
@@ -20070,26 +20072,26 @@
     </row>
     <row r="276">
       <c r="A276" s="94" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B276" s="90" t="s">
         <v>1114</v>
       </c>
-      <c r="B276" s="90" t="s">
+      <c r="C276" s="13" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D276" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E276" s="63" t="s">
         <v>1115</v>
-      </c>
-      <c r="C276" s="13" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D276" s="13" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E276" s="63" t="s">
-        <v>1116</v>
       </c>
       <c r="F276" s="6"/>
       <c r="G276" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H276" s="122" t="s">
-        <v>1117</v>
+        <v>1104</v>
+      </c>
+      <c r="H276" s="123" t="s">
+        <v>1116</v>
       </c>
       <c r="I276" s="6"/>
       <c r="J276" s="6"/>
@@ -20097,26 +20099,26 @@
     </row>
     <row r="277">
       <c r="A277" s="94" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B277" s="90" t="s">
         <v>1118</v>
       </c>
-      <c r="B277" s="90" t="s">
+      <c r="C277" s="13" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D277" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E277" s="63" t="s">
         <v>1119</v>
-      </c>
-      <c r="C277" s="13" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D277" s="13" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E277" s="63" t="s">
-        <v>1120</v>
       </c>
       <c r="F277" s="6"/>
       <c r="G277" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H277" s="122" t="s">
-        <v>1121</v>
+        <v>1104</v>
+      </c>
+      <c r="H277" s="123" t="s">
+        <v>1120</v>
       </c>
       <c r="I277" s="6"/>
       <c r="J277" s="6"/>
@@ -20124,26 +20126,26 @@
     </row>
     <row r="278">
       <c r="A278" s="94" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B278" s="90" t="s">
         <v>1122</v>
       </c>
-      <c r="B278" s="90" t="s">
+      <c r="C278" s="13" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D278" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E278" s="63" t="s">
         <v>1123</v>
-      </c>
-      <c r="C278" s="13" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D278" s="13" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E278" s="63" t="s">
-        <v>1124</v>
       </c>
       <c r="F278" s="6"/>
       <c r="G278" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H278" s="122" t="s">
-        <v>1125</v>
+        <v>1104</v>
+      </c>
+      <c r="H278" s="123" t="s">
+        <v>1124</v>
       </c>
       <c r="I278" s="6"/>
       <c r="J278" s="6"/>
@@ -20151,26 +20153,26 @@
     </row>
     <row r="279">
       <c r="A279" s="48" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B279" s="64" t="s">
         <v>1126</v>
       </c>
-      <c r="B279" s="64" t="s">
+      <c r="C279" s="132" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D279" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E279" s="63" t="s">
         <v>1127</v>
-      </c>
-      <c r="C279" s="131" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D279" s="13" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E279" s="63" t="s">
-        <v>1128</v>
       </c>
       <c r="F279" s="6"/>
       <c r="G279" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H279" s="122" t="s">
-        <v>1129</v>
+        <v>1104</v>
+      </c>
+      <c r="H279" s="123" t="s">
+        <v>1128</v>
       </c>
       <c r="I279" s="6"/>
       <c r="J279" s="6"/>
@@ -20178,26 +20180,26 @@
     </row>
     <row r="280">
       <c r="A280" s="48" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B280" s="64" t="s">
         <v>1130</v>
       </c>
-      <c r="B280" s="64" t="s">
+      <c r="C280" s="132" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D280" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E280" s="63" t="s">
         <v>1131</v>
-      </c>
-      <c r="C280" s="131" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D280" s="13" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E280" s="63" t="s">
-        <v>1132</v>
       </c>
       <c r="F280" s="6"/>
       <c r="G280" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H280" s="122" t="s">
-        <v>1133</v>
+        <v>1104</v>
+      </c>
+      <c r="H280" s="123" t="s">
+        <v>1132</v>
       </c>
       <c r="I280" s="6"/>
       <c r="J280" s="6"/>
@@ -20205,13 +20207,13 @@
     </row>
     <row r="281">
       <c r="A281" s="48" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B281" s="64" t="s">
         <v>1134</v>
       </c>
-      <c r="B281" s="64" t="s">
-        <v>1135</v>
-      </c>
-      <c r="C281" s="131" t="s">
-        <v>785</v>
+      <c r="C281" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D281" s="13"/>
       <c r="E281" s="13"/>
@@ -20224,26 +20226,26 @@
     </row>
     <row r="282">
       <c r="A282" s="94" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B282" s="90" t="s">
         <v>1136</v>
       </c>
-      <c r="B282" s="90" t="s">
+      <c r="C282" s="13" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D282" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E282" s="63" t="s">
         <v>1137</v>
-      </c>
-      <c r="C282" s="13" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D282" s="13" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E282" s="63" t="s">
-        <v>1138</v>
       </c>
       <c r="F282" s="6"/>
       <c r="G282" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H282" s="122" t="s">
-        <v>1139</v>
+        <v>1104</v>
+      </c>
+      <c r="H282" s="123" t="s">
+        <v>1138</v>
       </c>
       <c r="I282" s="6"/>
       <c r="J282" s="6"/>
@@ -20251,26 +20253,26 @@
     </row>
     <row r="283">
       <c r="A283" s="94" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B283" s="90" t="s">
         <v>1140</v>
       </c>
-      <c r="B283" s="90" t="s">
+      <c r="C283" s="13" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D283" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E283" s="63" t="s">
         <v>1141</v>
-      </c>
-      <c r="C283" s="13" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D283" s="13" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E283" s="63" t="s">
-        <v>1142</v>
       </c>
       <c r="F283" s="6"/>
       <c r="G283" s="6" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H283" s="122" t="s">
-        <v>1143</v>
+        <v>1104</v>
+      </c>
+      <c r="H283" s="123" t="s">
+        <v>1142</v>
       </c>
       <c r="I283" s="6"/>
       <c r="J283" s="6"/>
@@ -20278,13 +20280,13 @@
     </row>
     <row r="284">
       <c r="A284" s="91" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B284" s="61" t="s">
         <v>1144</v>
       </c>
-      <c r="B284" s="61" t="s">
-        <v>1145</v>
-      </c>
-      <c r="C284" s="131" t="s">
-        <v>785</v>
+      <c r="C284" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D284" s="13"/>
       <c r="E284" s="13"/>
@@ -20297,24 +20299,24 @@
     </row>
     <row r="285">
       <c r="A285" s="48" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B285" s="64" t="s">
         <v>1146</v>
-      </c>
-      <c r="B285" s="64" t="s">
-        <v>1147</v>
       </c>
       <c r="C285" s="159" t="s">
         <v>637</v>
       </c>
       <c r="D285" s="13"/>
       <c r="E285" s="63" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F285" s="6"/>
       <c r="G285" s="13" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H285" s="149" t="s">
-        <v>1149</v>
+        <v>1104</v>
+      </c>
+      <c r="H285" s="150" t="s">
+        <v>1148</v>
       </c>
       <c r="I285" s="6"/>
       <c r="J285" s="6"/>
@@ -20322,13 +20324,13 @@
     </row>
     <row r="286">
       <c r="A286" s="91" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B286" s="61" t="s">
         <v>1150</v>
       </c>
-      <c r="B286" s="61" t="s">
-        <v>1151</v>
-      </c>
-      <c r="C286" s="131" t="s">
-        <v>785</v>
+      <c r="C286" s="132" t="s">
+        <v>784</v>
       </c>
       <c r="D286" s="13"/>
       <c r="E286" s="13"/>
@@ -20341,29 +20343,29 @@
     </row>
     <row r="287">
       <c r="A287" s="48" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B287" s="160" t="s">
         <v>1152</v>
       </c>
-      <c r="B287" s="160" t="s">
+      <c r="C287" s="132" t="s">
         <v>1153</v>
       </c>
-      <c r="C287" s="131" t="s">
+      <c r="D287" s="13" t="s">
         <v>1154</v>
       </c>
-      <c r="D287" s="13" t="s">
+      <c r="E287" s="154" t="s">
         <v>1155</v>
-      </c>
-      <c r="E287" s="153" t="s">
-        <v>1156</v>
       </c>
       <c r="F287" s="6"/>
       <c r="G287" s="6" t="s">
+        <v>1156</v>
+      </c>
+      <c r="H287" s="88" t="s">
         <v>1157</v>
       </c>
-      <c r="H287" s="88" t="s">
+      <c r="I287" s="6" t="s">
         <v>1158</v>
-      </c>
-      <c r="I287" s="6" t="s">
-        <v>1159</v>
       </c>
       <c r="J287" s="6"/>
       <c r="K287" s="6"/>
@@ -20500,14 +20502,14 @@
         <v>425</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="88" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F2" s="88" t="s">
         <v>1161</v>
-      </c>
-      <c r="F2" s="88" t="s">
-        <v>1162</v>
       </c>
     </row>
     <row r="3">
@@ -20518,92 +20520,92 @@
         <v>425</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="88" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F3" s="88" t="s">
         <v>1163</v>
-      </c>
-      <c r="F3" s="88" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B4" s="88" t="s">
         <v>1165</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="C4" s="63" t="s">
         <v>1166</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="D4" s="63" t="s">
         <v>1167</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="E4" s="88" t="s">
         <v>1168</v>
       </c>
-      <c r="E4" s="88" t="s">
+      <c r="F4" s="88" t="s">
         <v>1169</v>
-      </c>
-      <c r="F4" s="88" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="B5" s="88" t="s">
         <v>773</v>
       </c>
-      <c r="B5" s="88" t="s">
+      <c r="C5" s="6" t="s">
         <v>774</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>775</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>776</v>
-      </c>
       <c r="E5" s="88" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F5" s="88" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
+        <v>846</v>
+      </c>
+      <c r="B6" s="88" t="s">
         <v>847</v>
       </c>
-      <c r="B6" s="88" t="s">
+      <c r="C6" s="163" t="s">
         <v>848</v>
-      </c>
-      <c r="C6" s="163" t="s">
-        <v>849</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="88" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F6" s="88" t="s">
         <v>1172</v>
-      </c>
-      <c r="F6" s="88" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>890</v>
+      </c>
+      <c r="B7" s="88" t="s">
         <v>891</v>
       </c>
-      <c r="B7" s="88" t="s">
+      <c r="C7" s="6" t="s">
         <v>892</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>893</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>894</v>
-      </c>
       <c r="E7" s="88" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F7" s="88" t="s">
         <v>1174</v>
-      </c>
-      <c r="F7" s="88" t="s">
-        <v>1175</v>
       </c>
     </row>
   </sheetData>
@@ -20627,36 +20629,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="164" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B2" s="165" t="s">
         <v>1176</v>
-      </c>
-      <c r="B2" s="165" t="s">
-        <v>1177</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="166" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B3" s="165" t="s">
         <v>1178</v>
-      </c>
-      <c r="B3" s="165" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="167" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="168" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B6" s="165" t="s">
         <v>1181</v>
-      </c>
-      <c r="B6" s="165" t="s">
-        <v>1182</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="165" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="8">
@@ -20667,41 +20669,41 @@
     </row>
     <row r="10">
       <c r="A10" s="168" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="168" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B11" s="169" t="s">
         <v>1185</v>
-      </c>
-      <c r="B11" s="169" t="s">
-        <v>1186</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="170" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="171"/>
       <c r="B13" s="172" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="173" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="174" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="175" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="17">
@@ -20710,24 +20712,24 @@
     </row>
     <row r="18">
       <c r="A18" s="168" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B18" s="176" t="s">
         <v>1192</v>
-      </c>
-      <c r="B18" s="176" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B19" s="82"/>
     </row>
     <row r="21">
       <c r="A21" s="168" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B21" s="177" t="s">
         <v>1195</v>
-      </c>
-      <c r="B21" s="177" t="s">
-        <v>1196</v>
       </c>
     </row>
   </sheetData>
@@ -20753,52 +20755,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="168" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="178" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="179" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="178" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="179" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="179" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="179" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="178" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="179" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="179" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
   </sheetData>
@@ -20824,58 +20826,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B1" s="180" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>1208</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>1209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="165" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
   </sheetData>
@@ -20919,35 +20921,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="181" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C1" s="182" t="s">
         <v>1218</v>
-      </c>
-      <c r="C1" s="182" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1220</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1221</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1222</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>1224</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="C3" s="6" t="s">
         <v>1225</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1226</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -20978,13 +20980,13 @@
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B4" s="39" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>1225</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1226</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="1"/>
@@ -21015,13 +21017,13 @@
     </row>
     <row r="5">
       <c r="A5" s="39" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>1228</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>1229</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -21049,16 +21051,16 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>1230</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>1231</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>1232</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -21085,16 +21087,16 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>1233</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D7" s="183" t="s">
         <v>1234</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D7" s="183" t="s">
-        <v>1235</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -21121,16 +21123,16 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>1236</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>1237</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1238</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -21157,16 +21159,16 @@
     </row>
     <row r="9">
       <c r="A9" s="88" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>1239</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>1240</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>1241</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -21193,16 +21195,16 @@
     </row>
     <row r="10">
       <c r="A10" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>1242</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>1240</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>1243</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -21229,16 +21231,16 @@
     </row>
     <row r="11">
       <c r="A11" s="88" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>1244</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>1245</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>1246</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -21265,16 +21267,16 @@
     </row>
     <row r="12">
       <c r="A12" s="88" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>1247</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>1245</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>1248</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -21301,16 +21303,16 @@
     </row>
     <row r="13">
       <c r="A13" s="184" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B13" s="184" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C13" s="185" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D13" s="185" t="s">
         <v>1249</v>
-      </c>
-      <c r="B13" s="184" t="s">
-        <v>1229</v>
-      </c>
-      <c r="C13" s="185" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D13" s="185" t="s">
-        <v>1250</v>
       </c>
       <c r="E13" s="185"/>
       <c r="F13" s="185"/>
@@ -21337,16 +21339,16 @@
     </row>
     <row r="14">
       <c r="A14" s="184" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B14" s="184" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C14" s="185" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D14" s="185" t="s">
         <v>1251</v>
-      </c>
-      <c r="B14" s="184" t="s">
-        <v>1229</v>
-      </c>
-      <c r="C14" s="185" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D14" s="185" t="s">
-        <v>1252</v>
       </c>
       <c r="E14" s="185"/>
       <c r="F14" s="185"/>
@@ -21398,58 +21400,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="181" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C1" s="182" t="s">
         <v>1218</v>
-      </c>
-      <c r="C1" s="182" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1220</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1221</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="180" t="s">
         <v>1222</v>
-      </c>
-      <c r="D2" s="180" t="s">
-        <v>1223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>1253</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1254</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1255</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>1256</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>1257</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="186" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>1258</v>
-      </c>
-      <c r="C5" s="186" t="s">
-        <v>1256</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>1259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgraded CM to v.6.3.1 for F21 and F22, to include notes for issue #323.
</commit_message>
<xml_diff>
--- a/mappings/package_F21/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F21/transformation/conceptual_mappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="1259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1260">
   <si>
     <t>Field</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.3.0</t>
+    <t>6.3.1</t>
   </si>
   <si>
     <r>
@@ -4625,6 +4625,11 @@
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
+  </si>
+  <si>
+    <t>In the XPATH condition, we likely don't need to add the conditions for notice types:
+- "PRI", as in case of F23 this information will only appear in the "PRI notices (and should not appear in "CONCESSION_AWARD_CONTRACT" notices
+- "QSU_ONLY" and "PER_ONLY", as for those type of notices we should not have this type of information specified; however, in case they are (by mistake/oversight), we will map it to this property</t>
   </si>
   <si>
     <t>IV.2.3</t>
@@ -17409,11 +17414,13 @@
       </c>
       <c r="I170" s="6"/>
       <c r="J170" s="6"/>
-      <c r="K170" s="6"/>
+      <c r="K170" s="21" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="46" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B171" s="47" t="s">
         <v>720</v>
@@ -17426,13 +17433,13 @@
         <v>721</v>
       </c>
       <c r="F171" s="88" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="G171" s="88" t="s">
         <v>723</v>
       </c>
       <c r="H171" s="123" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="I171" s="6"/>
       <c r="J171" s="6"/>
@@ -17440,24 +17447,24 @@
     </row>
     <row r="172">
       <c r="A172" s="46" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B172" s="47" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D172" s="4"/>
       <c r="E172" s="80" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F172" s="18"/>
       <c r="G172" s="4" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="H172" s="124" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="I172" s="6"/>
       <c r="J172" s="6"/>
@@ -17465,24 +17472,24 @@
     </row>
     <row r="173">
       <c r="A173" s="46" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B173" s="47" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>637</v>
       </c>
       <c r="D173" s="6"/>
       <c r="E173" s="18" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="F173" s="18"/>
       <c r="G173" s="88" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="H173" s="88" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="I173" s="6"/>
       <c r="J173" s="6"/>
@@ -17490,10 +17497,10 @@
     </row>
     <row r="174">
       <c r="A174" s="48" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B174" s="47" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C174" s="6"/>
       <c r="D174" s="6"/>
@@ -17507,26 +17514,26 @@
     </row>
     <row r="175">
       <c r="A175" s="94" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B175" s="55" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D175" s="13" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="E175" s="49" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="F175" s="49"/>
       <c r="G175" s="36" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="H175" s="36" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="I175" s="6"/>
       <c r="J175" s="6"/>
@@ -17534,24 +17541,24 @@
     </row>
     <row r="176">
       <c r="A176" s="117" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B176" s="34" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C176" s="6"/>
       <c r="D176" s="6"/>
       <c r="E176" s="39" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="F176" s="49" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="G176" s="4" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="H176" s="4" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="I176" s="6"/>
       <c r="J176" s="6"/>
@@ -17559,49 +17566,49 @@
     </row>
     <row r="177">
       <c r="A177" s="125" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B177" s="126" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C177" s="127"/>
       <c r="D177" s="127"/>
       <c r="E177" s="56" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="F177" s="40" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="G177" s="40" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="H177" s="128" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="I177" s="6"/>
       <c r="J177" s="6"/>
       <c r="K177" s="6" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="125" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B178" s="126" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C178" s="13"/>
       <c r="D178" s="13"/>
       <c r="E178" s="129" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="F178" s="36"/>
       <c r="G178" s="36" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="H178" s="36" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="I178" s="6"/>
       <c r="J178" s="6"/>
@@ -17609,28 +17616,28 @@
     </row>
     <row r="179">
       <c r="A179" s="48" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B179" s="47" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C179" s="13" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D179" s="13" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="E179" s="49" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="F179" s="49" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="G179" s="4" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H179" s="4" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="I179" s="6" t="s">
         <v>71</v>
@@ -17640,28 +17647,28 @@
     </row>
     <row r="180">
       <c r="A180" s="48" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B180" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C180" s="36" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D180" s="13" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="E180" s="49" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F180" s="49" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="G180" s="4" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H180" s="105" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="I180" s="6" t="s">
         <v>63</v>
@@ -17671,26 +17678,26 @@
     </row>
     <row r="181">
       <c r="A181" s="48" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B181" s="47" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C181" s="13" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D181" s="13" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="E181" s="39" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="F181" s="4"/>
       <c r="G181" s="4" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="H181" s="39" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="I181" s="6"/>
       <c r="J181" s="6"/>
@@ -17698,26 +17705,26 @@
     </row>
     <row r="182">
       <c r="A182" s="130" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B182" s="131" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C182" s="113" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D182" s="113" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="E182" s="39" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F182" s="4"/>
       <c r="G182" s="4" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H182" s="124" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="I182" s="6"/>
       <c r="J182" s="6"/>
@@ -17725,13 +17732,13 @@
     </row>
     <row r="183">
       <c r="A183" s="91" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B183" s="38" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C183" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D183" s="13"/>
       <c r="E183" s="4"/>
@@ -17744,13 +17751,13 @@
     </row>
     <row r="184">
       <c r="A184" s="48" t="s">
+        <v>786</v>
+      </c>
+      <c r="B184" s="47" t="s">
+        <v>787</v>
+      </c>
+      <c r="C184" s="132" t="s">
         <v>785</v>
-      </c>
-      <c r="B184" s="47" t="s">
-        <v>786</v>
-      </c>
-      <c r="C184" s="132" t="s">
-        <v>784</v>
       </c>
       <c r="D184" s="13"/>
       <c r="E184" s="36"/>
@@ -17763,26 +17770,26 @@
     </row>
     <row r="185">
       <c r="A185" s="94" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B185" s="55" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D185" s="13" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="E185" s="49" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F185" s="49"/>
       <c r="G185" s="36" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="H185" s="104" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="I185" s="6"/>
       <c r="J185" s="6"/>
@@ -17790,26 +17797,26 @@
     </row>
     <row r="186">
       <c r="A186" s="94" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B186" s="55" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C186" s="13" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D186" s="13" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="E186" s="49" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F186" s="49"/>
       <c r="G186" s="4" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="H186" s="124" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="I186" s="6"/>
       <c r="J186" s="6"/>
@@ -17817,24 +17824,24 @@
     </row>
     <row r="187">
       <c r="A187" s="94" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B187" s="55" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C187" s="133" t="s">
         <v>637</v>
       </c>
       <c r="D187" s="13"/>
       <c r="E187" s="40" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="F187" s="40"/>
       <c r="G187" s="40" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H187" s="40" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="I187" s="6"/>
       <c r="J187" s="6"/>
@@ -17842,13 +17849,13 @@
     </row>
     <row r="188">
       <c r="A188" s="91" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B188" s="38" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C188" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D188" s="13"/>
       <c r="E188" s="36"/>
@@ -17861,20 +17868,20 @@
     </row>
     <row r="189">
       <c r="A189" s="94" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B189" s="55"/>
       <c r="C189" s="13"/>
       <c r="D189" s="6"/>
       <c r="E189" s="56" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="F189" s="49"/>
       <c r="G189" s="36" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="H189" s="104" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="I189" s="6"/>
       <c r="J189" s="6"/>
@@ -17882,49 +17889,49 @@
     </row>
     <row r="190">
       <c r="A190" s="94" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B190" s="89"/>
       <c r="C190" s="36"/>
       <c r="D190" s="6"/>
       <c r="E190" s="56" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="F190" s="49"/>
       <c r="G190" s="36" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="H190" s="49" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="I190" s="6"/>
       <c r="J190" s="6"/>
       <c r="K190" s="6" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="48" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B191" s="47" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="D191" s="13" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="E191" s="49" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="F191" s="49"/>
       <c r="G191" s="39" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="H191" s="124" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="I191" s="6"/>
       <c r="J191" s="6"/>
@@ -17932,51 +17939,51 @@
     </row>
     <row r="192">
       <c r="A192" s="48" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B192" s="47" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="C192" s="134"/>
       <c r="D192" s="134"/>
       <c r="E192" s="56" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="F192" s="135"/>
       <c r="G192" s="49" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="H192" s="36" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="I192" s="6" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="J192" s="6"/>
       <c r="K192" s="6"/>
     </row>
     <row r="193">
       <c r="A193" s="94" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B193" s="55" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="D193" s="13" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="E193" s="49" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="F193" s="49"/>
       <c r="G193" s="36" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="H193" s="36" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="I193" s="6"/>
       <c r="J193" s="6"/>
@@ -17984,22 +17991,22 @@
     </row>
     <row r="194">
       <c r="A194" s="94" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B194" s="55" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
       <c r="E194" s="49" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="F194" s="49"/>
       <c r="G194" s="4" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="H194" s="39" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="I194" s="6"/>
       <c r="J194" s="6"/>
@@ -18007,22 +18014,22 @@
     </row>
     <row r="195">
       <c r="A195" s="94" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B195" s="55" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C195" s="13"/>
       <c r="D195" s="13"/>
       <c r="E195" s="49" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="F195" s="63"/>
       <c r="G195" s="4" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="H195" s="39" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="I195" s="6"/>
       <c r="J195" s="6"/>
@@ -18030,22 +18037,22 @@
     </row>
     <row r="196">
       <c r="A196" s="94" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B196" s="55" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C196" s="13"/>
       <c r="D196" s="13"/>
       <c r="E196" s="49" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="F196" s="49"/>
       <c r="G196" s="4" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="H196" s="124" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="I196" s="6"/>
       <c r="J196" s="6"/>
@@ -18053,22 +18060,22 @@
     </row>
     <row r="197">
       <c r="A197" s="94" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B197" s="55" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C197" s="13"/>
       <c r="D197" s="13"/>
       <c r="E197" s="49" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="F197" s="49"/>
       <c r="G197" s="4" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="H197" s="121" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="I197" s="6"/>
       <c r="J197" s="6"/>
@@ -18076,17 +18083,17 @@
     </row>
     <row r="198">
       <c r="A198" s="94" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B198" s="55" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C198" s="136" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D198" s="13"/>
       <c r="E198" s="49" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="F198" s="39"/>
       <c r="G198" s="36" t="s">
@@ -18101,13 +18108,13 @@
     </row>
     <row r="199">
       <c r="A199" s="48" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B199" s="47" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C199" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D199" s="13"/>
       <c r="E199" s="39"/>
@@ -18120,7 +18127,7 @@
     </row>
     <row r="200">
       <c r="A200" s="94" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B200" s="55" t="s">
         <v>57</v>
@@ -18132,14 +18139,14 @@
         <v>59</v>
       </c>
       <c r="E200" s="49" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="F200" s="49"/>
       <c r="G200" s="43" t="s">
         <v>61</v>
       </c>
       <c r="H200" s="43" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="I200" s="6" t="s">
         <v>63</v>
@@ -18149,7 +18156,7 @@
     </row>
     <row r="201">
       <c r="A201" s="94" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B201" s="55" t="s">
         <v>65</v>
@@ -18161,14 +18168,14 @@
         <v>67</v>
       </c>
       <c r="E201" s="49" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="F201" s="49"/>
       <c r="G201" s="45" t="s">
         <v>69</v>
       </c>
       <c r="H201" s="45" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="I201" s="6" t="s">
         <v>71</v>
@@ -18178,7 +18185,7 @@
     </row>
     <row r="202">
       <c r="A202" s="94" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B202" s="55" t="s">
         <v>73</v>
@@ -18190,14 +18197,14 @@
         <v>75</v>
       </c>
       <c r="E202" s="49" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="F202" s="49"/>
       <c r="G202" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H202" s="39" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="I202" s="6"/>
       <c r="J202" s="6"/>
@@ -18205,7 +18212,7 @@
     </row>
     <row r="203">
       <c r="A203" s="94" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B203" s="55" t="s">
         <v>80</v>
@@ -18217,14 +18224,14 @@
         <v>82</v>
       </c>
       <c r="E203" s="137" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="F203" s="137"/>
       <c r="G203" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H203" s="39" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="I203" s="6"/>
       <c r="J203" s="6"/>
@@ -18232,7 +18239,7 @@
     </row>
     <row r="204">
       <c r="A204" s="94" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B204" s="55" t="s">
         <v>86</v>
@@ -18244,16 +18251,16 @@
         <v>88</v>
       </c>
       <c r="E204" s="80" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="F204" s="80" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="G204" s="36" t="s">
         <v>91</v>
       </c>
       <c r="H204" s="49" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="I204" s="6"/>
       <c r="J204" s="6"/>
@@ -18261,7 +18268,7 @@
     </row>
     <row r="205">
       <c r="A205" s="94" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B205" s="55" t="s">
         <v>94</v>
@@ -18270,17 +18277,17 @@
         <v>95</v>
       </c>
       <c r="D205" s="138" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E205" s="137" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="F205" s="137"/>
       <c r="G205" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H205" s="39" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="I205" s="6"/>
       <c r="J205" s="6"/>
@@ -18288,7 +18295,7 @@
     </row>
     <row r="206">
       <c r="A206" s="94" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B206" s="55" t="s">
         <v>101</v>
@@ -18300,14 +18307,14 @@
         <v>103</v>
       </c>
       <c r="E206" s="137" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="F206" s="137"/>
       <c r="G206" s="78" t="s">
         <v>105</v>
       </c>
       <c r="H206" s="78" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I206" s="6"/>
       <c r="J206" s="6"/>
@@ -18315,7 +18322,7 @@
     </row>
     <row r="207">
       <c r="A207" s="94" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B207" s="55" t="s">
         <v>121</v>
@@ -18327,14 +18334,14 @@
         <v>123</v>
       </c>
       <c r="E207" s="137" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="F207" s="137"/>
       <c r="G207" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H207" s="63" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I207" s="6"/>
       <c r="J207" s="6"/>
@@ -18342,7 +18349,7 @@
     </row>
     <row r="208">
       <c r="A208" s="94" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B208" s="55" t="s">
         <v>115</v>
@@ -18354,14 +18361,14 @@
         <v>117</v>
       </c>
       <c r="E208" s="137" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="F208" s="137"/>
       <c r="G208" s="49" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="H208" s="49" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="I208" s="6"/>
       <c r="J208" s="6"/>
@@ -18369,10 +18376,10 @@
     </row>
     <row r="209">
       <c r="A209" s="94" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B209" s="55" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C209" s="13" t="s">
         <v>137</v>
@@ -18381,14 +18388,14 @@
         <v>138</v>
       </c>
       <c r="E209" s="137" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="F209" s="137"/>
       <c r="G209" s="45" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H209" s="45" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="I209" s="6"/>
       <c r="J209" s="6"/>
@@ -18396,7 +18403,7 @@
     </row>
     <row r="210">
       <c r="A210" s="94" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B210" s="55" t="s">
         <v>128</v>
@@ -18408,14 +18415,14 @@
         <v>130</v>
       </c>
       <c r="E210" s="137" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="F210" s="137"/>
       <c r="G210" s="49" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="H210" s="49" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="I210" s="6"/>
       <c r="J210" s="6"/>
@@ -18423,26 +18430,26 @@
     </row>
     <row r="211">
       <c r="A211" s="94" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B211" s="55" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C211" s="13" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="D211" s="13" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="E211" s="137" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="F211" s="80"/>
       <c r="G211" s="4" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="H211" s="139" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="I211" s="6"/>
       <c r="J211" s="6"/>
@@ -18454,14 +18461,14 @@
       <c r="C212" s="13"/>
       <c r="D212" s="13"/>
       <c r="E212" s="140" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="F212" s="80"/>
       <c r="G212" s="78" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="H212" s="78" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="I212" s="6"/>
       <c r="J212" s="6"/>
@@ -18469,13 +18476,13 @@
     </row>
     <row r="213">
       <c r="A213" s="48" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B213" s="47" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C213" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D213" s="13"/>
       <c r="E213" s="36"/>
@@ -18488,10 +18495,10 @@
     </row>
     <row r="214">
       <c r="A214" s="94" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B214" s="55" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C214" s="13" t="s">
         <v>526</v>
@@ -18500,14 +18507,14 @@
         <v>411</v>
       </c>
       <c r="E214" s="137" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="F214" s="137"/>
       <c r="G214" s="36" t="s">
         <v>528</v>
       </c>
       <c r="H214" s="49" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="I214" s="6"/>
       <c r="J214" s="6"/>
@@ -18515,7 +18522,7 @@
     </row>
     <row r="215">
       <c r="A215" s="108" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B215" s="75" t="s">
         <v>416</v>
@@ -18525,14 +18532,14 @@
       </c>
       <c r="D215" s="142"/>
       <c r="E215" s="137" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="F215" s="137"/>
       <c r="G215" s="36" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="H215" s="49" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="I215" s="6"/>
       <c r="J215" s="6"/>
@@ -18540,26 +18547,26 @@
     </row>
     <row r="216">
       <c r="A216" s="94" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B216" s="55" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C216" s="142" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="D216" s="142" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="E216" s="137" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="F216" s="137"/>
       <c r="G216" s="4" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="H216" s="39" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="I216" s="6"/>
       <c r="J216" s="6"/>
@@ -18567,7 +18574,7 @@
     </row>
     <row r="217">
       <c r="A217" s="108" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B217" s="75" t="s">
         <v>416</v>
@@ -18577,14 +18584,14 @@
       </c>
       <c r="D217" s="142"/>
       <c r="E217" s="137" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="F217" s="137"/>
       <c r="G217" s="4" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="H217" s="39" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="I217" s="6"/>
       <c r="J217" s="6"/>
@@ -18592,7 +18599,7 @@
     </row>
     <row r="218">
       <c r="A218" s="94" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B218" s="55" t="s">
         <v>463</v>
@@ -18604,14 +18611,14 @@
         <v>465</v>
       </c>
       <c r="E218" s="137" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F218" s="137"/>
       <c r="G218" s="36" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H218" s="49" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="I218" s="6"/>
       <c r="J218" s="6"/>
@@ -18619,7 +18626,7 @@
     </row>
     <row r="219">
       <c r="A219" s="108" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B219" s="75" t="s">
         <v>416</v>
@@ -18629,14 +18636,14 @@
       </c>
       <c r="D219" s="142"/>
       <c r="E219" s="137" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="F219" s="137"/>
       <c r="G219" s="36" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="H219" s="49" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="I219" s="6"/>
       <c r="J219" s="6"/>
@@ -18644,7 +18651,7 @@
     </row>
     <row r="220">
       <c r="A220" s="94" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B220" s="55" t="s">
         <v>469</v>
@@ -18656,14 +18663,14 @@
         <v>471</v>
       </c>
       <c r="E220" s="137" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="F220" s="137"/>
       <c r="G220" s="36" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H220" s="49" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="I220" s="6"/>
       <c r="J220" s="6"/>
@@ -18671,7 +18678,7 @@
     </row>
     <row r="221">
       <c r="A221" s="108" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B221" s="75" t="s">
         <v>416</v>
@@ -18681,14 +18688,14 @@
       </c>
       <c r="D221" s="13"/>
       <c r="E221" s="140" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="F221" s="137"/>
       <c r="G221" s="13" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="H221" s="63" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="I221" s="6"/>
       <c r="J221" s="6"/>
@@ -18696,13 +18703,13 @@
     </row>
     <row r="222">
       <c r="A222" s="48" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B222" s="64" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C222" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D222" s="13"/>
       <c r="E222" s="142"/>
@@ -18715,26 +18722,26 @@
     </row>
     <row r="223">
       <c r="A223" s="94" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B223" s="90" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="D223" s="13" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E223" s="49" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="F223" s="63"/>
       <c r="G223" s="49" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="H223" s="65" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="I223" s="6"/>
       <c r="J223" s="6"/>
@@ -18742,10 +18749,10 @@
     </row>
     <row r="224">
       <c r="A224" s="94" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B224" s="90" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C224" s="6"/>
       <c r="D224" s="6"/>
@@ -18759,26 +18766,26 @@
     </row>
     <row r="225">
       <c r="A225" s="94" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B225" s="90" t="s">
         <v>409</v>
       </c>
       <c r="C225" s="63" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="D225" s="63" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E225" s="137" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="F225" s="137"/>
       <c r="G225" s="36" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="H225" s="49" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="I225" s="6"/>
       <c r="J225" s="6"/>
@@ -18786,7 +18793,7 @@
     </row>
     <row r="226">
       <c r="A226" s="94" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B226" s="90" t="s">
         <v>416</v>
@@ -18796,14 +18803,14 @@
       </c>
       <c r="D226" s="13"/>
       <c r="E226" s="137" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="F226" s="137"/>
       <c r="G226" s="63" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="H226" s="13" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="I226" s="6"/>
       <c r="J226" s="6"/>
@@ -18811,26 +18818,26 @@
     </row>
     <row r="227">
       <c r="A227" s="94" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B227" s="90" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C227" s="13" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="D227" s="13" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="E227" s="137" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="F227" s="137"/>
       <c r="G227" s="49" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="H227" s="49" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="I227" s="6"/>
       <c r="J227" s="6"/>
@@ -18838,26 +18845,26 @@
     </row>
     <row r="228">
       <c r="A228" s="94" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B228" s="90" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C228" s="13" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D228" s="13" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="E228" s="137" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="F228" s="137"/>
       <c r="G228" s="63" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="H228" s="63" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="I228" s="6" t="s">
         <v>63</v>
@@ -18867,10 +18874,10 @@
     </row>
     <row r="229">
       <c r="A229" s="117" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B229" s="144" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C229" s="6"/>
       <c r="D229" s="6"/>
@@ -18884,10 +18891,10 @@
     </row>
     <row r="230">
       <c r="A230" s="37" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B230" s="61" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C230" s="98"/>
       <c r="D230" s="83"/>
@@ -18901,24 +18908,24 @@
     </row>
     <row r="231">
       <c r="A231" s="46" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B231" s="64" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C231" s="98" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="D231" s="83"/>
       <c r="E231" s="145" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="F231" s="142"/>
       <c r="G231" s="4" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="H231" s="105" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="I231" s="6"/>
       <c r="J231" s="6"/>
@@ -18926,24 +18933,24 @@
     </row>
     <row r="232">
       <c r="A232" s="46" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B232" s="64" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C232" s="98" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="D232" s="83"/>
       <c r="E232" s="145" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="F232" s="142"/>
       <c r="G232" s="4" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="H232" s="105" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="I232" s="6"/>
       <c r="J232" s="6"/>
@@ -18951,24 +18958,24 @@
     </row>
     <row r="233">
       <c r="A233" s="46" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B233" s="64" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C233" s="98" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="D233" s="83"/>
       <c r="E233" s="145" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="F233" s="142"/>
       <c r="G233" s="4" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="H233" s="105" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="I233" s="6"/>
       <c r="J233" s="6"/>
@@ -18976,7 +18983,7 @@
     </row>
     <row r="234">
       <c r="A234" s="91" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B234" s="61" t="s">
         <v>582</v>
@@ -18988,14 +18995,14 @@
         <v>584</v>
       </c>
       <c r="E234" s="137" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="F234" s="137"/>
       <c r="G234" s="146" t="s">
         <v>372</v>
       </c>
       <c r="H234" s="147" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I234" s="6" t="s">
         <v>63</v>
@@ -19005,13 +19012,13 @@
     </row>
     <row r="235">
       <c r="A235" s="91" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B235" s="61" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C235" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D235" s="6"/>
       <c r="E235" s="142"/>
@@ -19024,17 +19031,17 @@
     </row>
     <row r="236">
       <c r="A236" s="48" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B236" s="64" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C236" s="148" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D236" s="6"/>
       <c r="E236" s="88" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="F236" s="63"/>
       <c r="G236" s="13" t="s">
@@ -19049,7 +19056,7 @@
     </row>
     <row r="237">
       <c r="A237" s="94" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B237" s="90" t="s">
         <v>57</v>
@@ -19061,14 +19068,14 @@
         <v>59</v>
       </c>
       <c r="E237" s="63" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="F237" s="63"/>
       <c r="G237" s="88" t="s">
         <v>61</v>
       </c>
       <c r="H237" s="88" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="I237" s="6" t="s">
         <v>63</v>
@@ -19078,7 +19085,7 @@
     </row>
     <row r="238">
       <c r="A238" s="94" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B238" s="90" t="s">
         <v>73</v>
@@ -19090,14 +19097,14 @@
         <v>75</v>
       </c>
       <c r="E238" s="63" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="F238" s="63"/>
       <c r="G238" s="88" t="s">
         <v>77</v>
       </c>
       <c r="H238" s="88" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="I238" s="6"/>
       <c r="J238" s="6"/>
@@ -19105,7 +19112,7 @@
     </row>
     <row r="239">
       <c r="A239" s="94" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B239" s="90" t="s">
         <v>80</v>
@@ -19117,14 +19124,14 @@
         <v>82</v>
       </c>
       <c r="E239" s="63" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="F239" s="63"/>
       <c r="G239" s="88" t="s">
         <v>77</v>
       </c>
       <c r="H239" s="88" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="I239" s="6"/>
       <c r="J239" s="6"/>
@@ -19132,7 +19139,7 @@
     </row>
     <row r="240">
       <c r="A240" s="94" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B240" s="90" t="s">
         <v>94</v>
@@ -19141,17 +19148,17 @@
         <v>95</v>
       </c>
       <c r="D240" s="13" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E240" s="63" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="F240" s="63"/>
       <c r="G240" s="88" t="s">
         <v>98</v>
       </c>
       <c r="H240" s="88" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="I240" s="6"/>
       <c r="J240" s="6"/>
@@ -19159,7 +19166,7 @@
     </row>
     <row r="241">
       <c r="A241" s="94" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B241" s="90" t="s">
         <v>101</v>
@@ -19171,14 +19178,14 @@
         <v>103</v>
       </c>
       <c r="E241" s="63" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="F241" s="63"/>
       <c r="G241" s="63" t="s">
         <v>105</v>
       </c>
       <c r="H241" s="63" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="I241" s="6"/>
       <c r="J241" s="6"/>
@@ -19186,7 +19193,7 @@
     </row>
     <row r="242">
       <c r="A242" s="94" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B242" s="90" t="s">
         <v>121</v>
@@ -19198,14 +19205,14 @@
         <v>123</v>
       </c>
       <c r="E242" s="63" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="F242" s="63"/>
       <c r="G242" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H242" s="63" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I242" s="6"/>
       <c r="J242" s="6"/>
@@ -19213,7 +19220,7 @@
     </row>
     <row r="243">
       <c r="A243" s="94" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B243" s="90" t="s">
         <v>115</v>
@@ -19225,14 +19232,14 @@
         <v>117</v>
       </c>
       <c r="E243" s="63" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="F243" s="63"/>
       <c r="G243" s="63" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="H243" s="63" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="I243" s="6"/>
       <c r="J243" s="6"/>
@@ -19240,10 +19247,10 @@
     </row>
     <row r="244">
       <c r="A244" s="94" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B244" s="90" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C244" s="13" t="s">
         <v>137</v>
@@ -19252,14 +19259,14 @@
         <v>138</v>
       </c>
       <c r="E244" s="63" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F244" s="63"/>
       <c r="G244" s="60" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H244" s="60" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="I244" s="6"/>
       <c r="J244" s="6"/>
@@ -19267,7 +19274,7 @@
     </row>
     <row r="245">
       <c r="A245" s="94" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B245" s="90" t="s">
         <v>128</v>
@@ -19279,14 +19286,14 @@
         <v>130</v>
       </c>
       <c r="E245" s="63" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F245" s="63"/>
       <c r="G245" s="63" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="H245" s="63" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="I245" s="6"/>
       <c r="J245" s="6"/>
@@ -19294,21 +19301,21 @@
     </row>
     <row r="246">
       <c r="A246" s="48" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B246" s="64" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C246" s="148" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D246" s="149"/>
       <c r="E246" s="88" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="F246" s="13"/>
       <c r="G246" s="13" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="H246" s="13" t="s">
         <v>234</v>
@@ -19319,7 +19326,7 @@
     </row>
     <row r="247">
       <c r="A247" s="94" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B247" s="90" t="s">
         <v>57</v>
@@ -19331,14 +19338,14 @@
         <v>59</v>
       </c>
       <c r="E247" s="63" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="F247" s="63"/>
       <c r="G247" s="88" t="s">
         <v>61</v>
       </c>
       <c r="H247" s="123" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="I247" s="6" t="s">
         <v>63</v>
@@ -19348,7 +19355,7 @@
     </row>
     <row r="248">
       <c r="A248" s="94" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B248" s="90" t="s">
         <v>73</v>
@@ -19360,14 +19367,14 @@
         <v>75</v>
       </c>
       <c r="E248" s="63" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F248" s="63"/>
       <c r="G248" s="88" t="s">
         <v>77</v>
       </c>
       <c r="H248" s="123" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I248" s="6"/>
       <c r="J248" s="6"/>
@@ -19375,7 +19382,7 @@
     </row>
     <row r="249">
       <c r="A249" s="94" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B249" s="90" t="s">
         <v>80</v>
@@ -19387,14 +19394,14 @@
         <v>82</v>
       </c>
       <c r="E249" s="63" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="F249" s="63"/>
       <c r="G249" s="88" t="s">
         <v>77</v>
       </c>
       <c r="H249" s="123" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="I249" s="6"/>
       <c r="J249" s="6"/>
@@ -19402,7 +19409,7 @@
     </row>
     <row r="250">
       <c r="A250" s="94" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B250" s="90" t="s">
         <v>94</v>
@@ -19411,17 +19418,17 @@
         <v>95</v>
       </c>
       <c r="D250" s="13" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E250" s="63" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="F250" s="63"/>
       <c r="G250" s="88" t="s">
         <v>98</v>
       </c>
       <c r="H250" s="88" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="I250" s="6"/>
       <c r="J250" s="6"/>
@@ -19429,7 +19436,7 @@
     </row>
     <row r="251">
       <c r="A251" s="94" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B251" s="90" t="s">
         <v>101</v>
@@ -19441,14 +19448,14 @@
         <v>103</v>
       </c>
       <c r="E251" s="63" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F251" s="63"/>
       <c r="G251" s="88" t="s">
         <v>105</v>
       </c>
       <c r="H251" s="123" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="I251" s="6"/>
       <c r="J251" s="6"/>
@@ -19456,7 +19463,7 @@
     </row>
     <row r="252">
       <c r="A252" s="94" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B252" s="90" t="s">
         <v>121</v>
@@ -19468,14 +19475,14 @@
         <v>123</v>
       </c>
       <c r="E252" s="63" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="F252" s="63"/>
       <c r="G252" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H252" s="150" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I252" s="6"/>
       <c r="J252" s="6"/>
@@ -19483,7 +19490,7 @@
     </row>
     <row r="253">
       <c r="A253" s="94" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B253" s="90" t="s">
         <v>115</v>
@@ -19495,14 +19502,14 @@
         <v>117</v>
       </c>
       <c r="E253" s="63" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="F253" s="63"/>
       <c r="G253" s="63" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="H253" s="63" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="I253" s="6"/>
       <c r="J253" s="6"/>
@@ -19510,10 +19517,10 @@
     </row>
     <row r="254">
       <c r="A254" s="94" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B254" s="90" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C254" s="13" t="s">
         <v>137</v>
@@ -19522,14 +19529,14 @@
         <v>138</v>
       </c>
       <c r="E254" s="63" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="F254" s="63"/>
       <c r="G254" s="60" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H254" s="60" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="I254" s="6"/>
       <c r="J254" s="6"/>
@@ -19537,7 +19544,7 @@
     </row>
     <row r="255">
       <c r="A255" s="94" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B255" s="90" t="s">
         <v>128</v>
@@ -19549,14 +19556,14 @@
         <v>130</v>
       </c>
       <c r="E255" s="63" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="F255" s="63"/>
       <c r="G255" s="63" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="H255" s="63" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="I255" s="6"/>
       <c r="J255" s="6"/>
@@ -19564,26 +19571,26 @@
     </row>
     <row r="256">
       <c r="A256" s="48" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B256" s="64" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C256" s="13" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D256" s="13" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="E256" s="63" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="F256" s="63"/>
       <c r="G256" s="88" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="H256" s="147" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="I256" s="6"/>
       <c r="J256" s="6"/>
@@ -19591,15 +19598,15 @@
     </row>
     <row r="257">
       <c r="A257" s="48" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B257" s="64" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C257" s="6"/>
       <c r="D257" s="6"/>
       <c r="E257" s="88" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="F257" s="13"/>
       <c r="G257" s="13" t="s">
@@ -19614,7 +19621,7 @@
     </row>
     <row r="258">
       <c r="A258" s="94" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B258" s="90" t="s">
         <v>57</v>
@@ -19626,14 +19633,14 @@
         <v>59</v>
       </c>
       <c r="E258" s="63" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="F258" s="63"/>
       <c r="G258" s="88" t="s">
         <v>61</v>
       </c>
       <c r="H258" s="123" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="I258" s="6" t="s">
         <v>63</v>
@@ -19643,7 +19650,7 @@
     </row>
     <row r="259">
       <c r="A259" s="94" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B259" s="90" t="s">
         <v>73</v>
@@ -19655,14 +19662,14 @@
         <v>75</v>
       </c>
       <c r="E259" s="63" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="F259" s="63"/>
       <c r="G259" s="88" t="s">
         <v>77</v>
       </c>
       <c r="H259" s="123" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="I259" s="6"/>
       <c r="J259" s="6"/>
@@ -19670,7 +19677,7 @@
     </row>
     <row r="260">
       <c r="A260" s="94" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B260" s="90" t="s">
         <v>80</v>
@@ -19682,14 +19689,14 @@
         <v>82</v>
       </c>
       <c r="E260" s="63" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="F260" s="63"/>
       <c r="G260" s="88" t="s">
         <v>77</v>
       </c>
       <c r="H260" s="123" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="I260" s="6"/>
       <c r="J260" s="6"/>
@@ -19697,7 +19704,7 @@
     </row>
     <row r="261">
       <c r="A261" s="94" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B261" s="90" t="s">
         <v>94</v>
@@ -19706,17 +19713,17 @@
         <v>95</v>
       </c>
       <c r="D261" s="13" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E261" s="63" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="F261" s="63"/>
       <c r="G261" s="88" t="s">
         <v>98</v>
       </c>
       <c r="H261" s="88" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="I261" s="6"/>
       <c r="J261" s="6"/>
@@ -19724,7 +19731,7 @@
     </row>
     <row r="262">
       <c r="A262" s="94" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B262" s="90" t="s">
         <v>101</v>
@@ -19736,14 +19743,14 @@
         <v>103</v>
       </c>
       <c r="E262" s="63" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="F262" s="63"/>
       <c r="G262" s="63" t="s">
         <v>105</v>
       </c>
       <c r="H262" s="150" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="I262" s="6"/>
       <c r="J262" s="6"/>
@@ -19751,7 +19758,7 @@
     </row>
     <row r="263">
       <c r="A263" s="94" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B263" s="90" t="s">
         <v>121</v>
@@ -19763,14 +19770,14 @@
         <v>123</v>
       </c>
       <c r="E263" s="63" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="F263" s="63"/>
       <c r="G263" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H263" s="150" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I263" s="6"/>
       <c r="J263" s="6"/>
@@ -19778,7 +19785,7 @@
     </row>
     <row r="264">
       <c r="A264" s="94" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B264" s="90" t="s">
         <v>115</v>
@@ -19790,14 +19797,14 @@
         <v>117</v>
       </c>
       <c r="E264" s="63" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="F264" s="63"/>
       <c r="G264" s="63" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="H264" s="150" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="I264" s="6"/>
       <c r="J264" s="6"/>
@@ -19805,10 +19812,10 @@
     </row>
     <row r="265">
       <c r="A265" s="94" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B265" s="90" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C265" s="13" t="s">
         <v>137</v>
@@ -19817,14 +19824,14 @@
         <v>138</v>
       </c>
       <c r="E265" s="63" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="F265" s="63"/>
       <c r="G265" s="60" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H265" s="152" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="I265" s="6"/>
       <c r="J265" s="6"/>
@@ -19832,7 +19839,7 @@
     </row>
     <row r="266">
       <c r="A266" s="94" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B266" s="90" t="s">
         <v>128</v>
@@ -19844,14 +19851,14 @@
         <v>130</v>
       </c>
       <c r="E266" s="63" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="F266" s="63"/>
       <c r="G266" s="63" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="H266" s="150" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="I266" s="6"/>
       <c r="J266" s="6"/>
@@ -19859,26 +19866,26 @@
     </row>
     <row r="267">
       <c r="A267" s="91" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B267" s="61" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C267" s="153" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="D267" s="153" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="E267" s="154" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="F267" s="154"/>
       <c r="G267" s="88" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="H267" s="155" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="I267" s="6"/>
       <c r="J267" s="6"/>
@@ -19886,10 +19893,10 @@
     </row>
     <row r="268">
       <c r="A268" s="117" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B268" s="144" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C268" s="6"/>
       <c r="D268" s="6"/>
@@ -19903,17 +19910,17 @@
     </row>
     <row r="269">
       <c r="A269" s="91" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B269" s="61" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C269" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D269" s="13"/>
       <c r="E269" s="63" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="F269" s="6"/>
       <c r="G269" s="6"/>
@@ -19924,16 +19931,16 @@
     </row>
     <row r="270">
       <c r="A270" s="48" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B270" s="64" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="C270" s="132" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D270" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E270" s="88"/>
       <c r="F270" s="6"/>
@@ -19945,26 +19952,26 @@
     </row>
     <row r="271">
       <c r="A271" s="94" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B271" s="90" t="s">
         <v>662</v>
       </c>
       <c r="C271" s="13" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="D271" s="13" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="E271" s="63" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="F271" s="13"/>
       <c r="G271" s="88" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="H271" s="123" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="I271" s="6"/>
       <c r="J271" s="6"/>
@@ -19972,26 +19979,26 @@
     </row>
     <row r="272">
       <c r="A272" s="156" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B272" s="157" t="s">
         <v>662</v>
       </c>
       <c r="C272" s="158" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="D272" s="158" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="E272" s="122" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="F272" s="13"/>
       <c r="G272" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H272" s="123" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="I272" s="6"/>
       <c r="J272" s="6"/>
@@ -19999,26 +20006,26 @@
     </row>
     <row r="273">
       <c r="A273" s="94" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B273" s="90" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C273" s="13" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="D273" s="13" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="E273" s="63" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="F273" s="13"/>
       <c r="G273" s="88" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="H273" s="123" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="I273" s="6"/>
       <c r="J273" s="6"/>
@@ -20026,26 +20033,26 @@
     </row>
     <row r="274">
       <c r="A274" s="156" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B274" s="157" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C274" s="158" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="D274" s="158" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="E274" s="122" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="F274" s="13"/>
       <c r="G274" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H274" s="123" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="I274" s="6"/>
       <c r="J274" s="6"/>
@@ -20053,13 +20060,13 @@
     </row>
     <row r="275">
       <c r="A275" s="48" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B275" s="64" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="C275" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D275" s="13"/>
       <c r="E275" s="13"/>
@@ -20072,26 +20079,26 @@
     </row>
     <row r="276">
       <c r="A276" s="94" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B276" s="90" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="C276" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D276" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E276" s="63" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="F276" s="6"/>
       <c r="G276" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H276" s="123" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="I276" s="6"/>
       <c r="J276" s="6"/>
@@ -20099,26 +20106,26 @@
     </row>
     <row r="277">
       <c r="A277" s="94" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B277" s="90" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="C277" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D277" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E277" s="63" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="F277" s="6"/>
       <c r="G277" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H277" s="123" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="I277" s="6"/>
       <c r="J277" s="6"/>
@@ -20126,26 +20133,26 @@
     </row>
     <row r="278">
       <c r="A278" s="94" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B278" s="90" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="C278" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D278" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E278" s="63" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="F278" s="6"/>
       <c r="G278" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H278" s="123" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="I278" s="6"/>
       <c r="J278" s="6"/>
@@ -20153,26 +20160,26 @@
     </row>
     <row r="279">
       <c r="A279" s="48" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B279" s="64" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="C279" s="132" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D279" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E279" s="63" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="F279" s="6"/>
       <c r="G279" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H279" s="123" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="I279" s="6"/>
       <c r="J279" s="6"/>
@@ -20180,26 +20187,26 @@
     </row>
     <row r="280">
       <c r="A280" s="48" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B280" s="64" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="C280" s="132" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D280" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E280" s="63" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="F280" s="6"/>
       <c r="G280" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H280" s="123" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="I280" s="6"/>
       <c r="J280" s="6"/>
@@ -20207,13 +20214,13 @@
     </row>
     <row r="281">
       <c r="A281" s="48" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B281" s="64" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="C281" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D281" s="13"/>
       <c r="E281" s="13"/>
@@ -20226,26 +20233,26 @@
     </row>
     <row r="282">
       <c r="A282" s="94" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B282" s="90" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C282" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D282" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E282" s="63" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="F282" s="6"/>
       <c r="G282" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H282" s="123" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="I282" s="6"/>
       <c r="J282" s="6"/>
@@ -20253,26 +20260,26 @@
     </row>
     <row r="283">
       <c r="A283" s="94" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B283" s="90" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="C283" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D283" s="13" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E283" s="63" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="F283" s="6"/>
       <c r="G283" s="6" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H283" s="123" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="I283" s="6"/>
       <c r="J283" s="6"/>
@@ -20280,13 +20287,13 @@
     </row>
     <row r="284">
       <c r="A284" s="91" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="B284" s="61" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="C284" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D284" s="13"/>
       <c r="E284" s="13"/>
@@ -20299,24 +20306,24 @@
     </row>
     <row r="285">
       <c r="A285" s="48" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="B285" s="64" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C285" s="159" t="s">
         <v>637</v>
       </c>
       <c r="D285" s="13"/>
       <c r="E285" s="63" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="F285" s="6"/>
       <c r="G285" s="13" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H285" s="150" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="I285" s="6"/>
       <c r="J285" s="6"/>
@@ -20324,13 +20331,13 @@
     </row>
     <row r="286">
       <c r="A286" s="91" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="B286" s="61" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="C286" s="132" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D286" s="13"/>
       <c r="E286" s="13"/>
@@ -20343,29 +20350,29 @@
     </row>
     <row r="287">
       <c r="A287" s="48" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B287" s="160" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="C287" s="132" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="D287" s="13" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="E287" s="154" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="F287" s="6"/>
       <c r="G287" s="6" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="H287" s="88" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="I287" s="6" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="J287" s="6"/>
       <c r="K287" s="6"/>
@@ -20502,14 +20509,14 @@
         <v>425</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D2" s="63"/>
       <c r="E2" s="88" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="F2" s="88" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="3">
@@ -20520,92 +20527,92 @@
         <v>425</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="88" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="F3" s="88" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="B4" s="88" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="E4" s="88" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="F4" s="88" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="E5" s="88" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F5" s="88" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C6" s="163" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="88" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="F6" s="88" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="E7" s="88" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="F7" s="88" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
     </row>
   </sheetData>
@@ -20629,36 +20636,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="164" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B2" s="165" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="166" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B3" s="165" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="167" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="168" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="B6" s="165" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="165" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="8">
@@ -20669,41 +20676,41 @@
     </row>
     <row r="10">
       <c r="A10" s="168" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="168" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="B11" s="169" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="170" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="171"/>
       <c r="B13" s="172" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="173" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="174" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="175" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="17">
@@ -20712,24 +20719,24 @@
     </row>
     <row r="18">
       <c r="A18" s="168" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B18" s="176" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B19" s="82"/>
     </row>
     <row r="21">
       <c r="A21" s="168" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B21" s="177" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
     </row>
   </sheetData>
@@ -20755,52 +20762,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="168" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="178" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="179" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="178" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="179" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="179" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="179" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="178" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="179" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="179" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
     </row>
   </sheetData>
@@ -20826,58 +20833,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B1" s="180" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="165" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
     </row>
   </sheetData>
@@ -20921,35 +20928,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="181" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="C1" s="182" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -20980,13 +20987,13 @@
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>1226</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1225</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="1"/>
@@ -21017,13 +21024,13 @@
     </row>
     <row r="5">
       <c r="A5" s="39" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -21051,16 +21058,16 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -21087,16 +21094,16 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D7" s="183" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -21123,16 +21130,16 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -21159,16 +21166,16 @@
     </row>
     <row r="9">
       <c r="A9" s="88" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -21195,16 +21202,16 @@
     </row>
     <row r="10">
       <c r="A10" s="88" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -21231,16 +21238,16 @@
     </row>
     <row r="11">
       <c r="A11" s="88" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -21267,16 +21274,16 @@
     </row>
     <row r="12">
       <c r="A12" s="88" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -21303,16 +21310,16 @@
     </row>
     <row r="13">
       <c r="A13" s="184" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="B13" s="184" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="C13" s="185" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D13" s="185" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="E13" s="185"/>
       <c r="F13" s="185"/>
@@ -21339,16 +21346,16 @@
     </row>
     <row r="14">
       <c r="A14" s="184" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="B14" s="184" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="C14" s="185" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D14" s="185" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="E14" s="185"/>
       <c r="F14" s="185"/>
@@ -21400,58 +21407,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="181" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="C1" s="182" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D2" s="180" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C5" s="186" t="s">
         <v>1256</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>1257</v>
-      </c>
-      <c r="C5" s="186" t="s">
-        <v>1255</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CM (v6.5.1) of forms F20-F25 to address issue #336.
</commit_message>
<xml_diff>
--- a/mappings/package_F21/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F21/transformation/conceptual_mappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="1261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1262">
   <si>
     <t>Field</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.5.0</t>
+    <t>6.5.1</t>
   </si>
   <si>
     <r>
@@ -3704,7 +3704,7 @@
     <t>OBJECT_CONTRACT/OBJECT_DESCR/DURATION</t>
   </si>
   <si>
-    <t>epo:Lot / epo:ContractTerm / epo:Duration / xsd:decimal</t>
+    <t>epo:Lot / epo:ContractTerm / epo:SpecificDuration / xsd:decimal</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -3720,7 +3720,7 @@
     <t xml:space="preserve">If(.="MONTH") </t>
   </si>
   <si>
-    <t>epo:Lot / epo:ContractTerm / epo:Duration / time:TemporalUnit</t>
+    <t>epo:Lot / epo:ContractTerm / epo:SpecificDuration / time:TemporalUnit</t>
   </si>
   <si>
     <t>?this epo:foreseesContractSpecificTerm / epo:definesContractDuration / time:unitType time:unitMonth.</t>
@@ -4005,6 +4005,9 @@
   </si>
   <si>
     <t>BT-71</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
   <si>
     <t>LEFTI/RESTRICTED_SHELTERED_WORKSHOP</t>
@@ -16336,7 +16339,7 @@
         <v>535</v>
       </c>
       <c r="F125" s="93"/>
-      <c r="G125" s="93" t="s">
+      <c r="G125" s="95" t="s">
         <v>536</v>
       </c>
       <c r="H125" s="93" t="s">
@@ -16359,7 +16362,7 @@
       <c r="F126" s="93" t="s">
         <v>540</v>
       </c>
-      <c r="G126" s="93" t="s">
+      <c r="G126" s="95" t="s">
         <v>541</v>
       </c>
       <c r="H126" s="93" t="s">
@@ -16382,7 +16385,7 @@
       <c r="F127" s="93" t="s">
         <v>544</v>
       </c>
-      <c r="G127" s="93" t="s">
+      <c r="G127" s="95" t="s">
         <v>541</v>
       </c>
       <c r="H127" s="109" t="s">
@@ -16707,18 +16710,20 @@
       <c r="C141" s="13" t="s">
         <v>605</v>
       </c>
-      <c r="D141" s="13"/>
+      <c r="D141" s="63" t="s">
+        <v>606</v>
+      </c>
       <c r="E141" s="49" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F141" s="36" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="G141" s="49" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="H141" s="118" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="I141" s="6"/>
       <c r="J141" s="6"/>
@@ -16726,26 +16731,26 @@
     </row>
     <row r="142">
       <c r="A142" s="54" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B142" s="55" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C142" s="13" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D142" s="13"/>
       <c r="E142" s="49" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F142" s="36" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="G142" s="49" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="H142" s="118" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="I142" s="6"/>
       <c r="J142" s="6"/>
@@ -16753,26 +16758,26 @@
     </row>
     <row r="143">
       <c r="A143" s="54" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B143" s="55" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C143" s="36" t="s">
         <v>605</v>
       </c>
       <c r="D143" s="13"/>
       <c r="E143" s="49" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="F143" s="36" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="G143" s="49" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="H143" s="119" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="I143" s="6"/>
       <c r="J143" s="6"/>
@@ -16780,10 +16785,10 @@
     </row>
     <row r="144">
       <c r="A144" s="37" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B144" s="38" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C144" s="13"/>
       <c r="D144" s="13"/>
@@ -16797,10 +16802,10 @@
     </row>
     <row r="145">
       <c r="A145" s="46" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B145" s="47" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C145" s="13"/>
       <c r="D145" s="13"/>
@@ -16814,26 +16819,26 @@
     </row>
     <row r="146">
       <c r="A146" s="54" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B146" s="55" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C146" s="97" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D146" s="97"/>
       <c r="E146" s="80" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F146" s="96" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="G146" s="4" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="H146" s="39" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="I146" s="6"/>
       <c r="J146" s="6"/>
@@ -16841,17 +16846,17 @@
     </row>
     <row r="147">
       <c r="A147" s="54" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B147" s="55" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C147" s="82" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D147" s="97"/>
       <c r="E147" s="80" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F147" s="96"/>
       <c r="G147" s="4" t="s">
@@ -16868,24 +16873,24 @@
     </row>
     <row r="148">
       <c r="A148" s="46" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B148" s="47" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C148" s="82" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D148" s="97"/>
       <c r="E148" s="80" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F148" s="96"/>
       <c r="G148" s="4" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="H148" s="39" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="I148" s="6"/>
       <c r="J148" s="6"/>
@@ -16893,10 +16898,10 @@
     </row>
     <row r="149">
       <c r="A149" s="46" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B149" s="47" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C149" s="13"/>
       <c r="D149" s="13"/>
@@ -16910,26 +16915,26 @@
     </row>
     <row r="150">
       <c r="A150" s="54" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B150" s="55" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C150" s="97" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D150" s="97"/>
       <c r="E150" s="80" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F150" s="96" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="G150" s="4" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="H150" s="39" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="I150" s="6"/>
       <c r="J150" s="6"/>
@@ -16937,26 +16942,26 @@
     </row>
     <row r="151">
       <c r="A151" s="54" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B151" s="55" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C151" s="97" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D151" s="97"/>
       <c r="E151" s="56" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F151" s="96" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="G151" s="4" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="H151" s="39" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="I151" s="6"/>
       <c r="J151" s="6"/>
@@ -16964,15 +16969,15 @@
     </row>
     <row r="152">
       <c r="A152" s="120" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B152" s="92" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C152" s="4"/>
       <c r="D152" s="6"/>
       <c r="E152" s="39" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F152" s="4"/>
       <c r="G152" s="40"/>
@@ -16983,7 +16988,7 @@
     </row>
     <row r="153">
       <c r="A153" s="91" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B153" s="38" t="s">
         <v>8</v>
@@ -17000,10 +17005,10 @@
     </row>
     <row r="154">
       <c r="A154" s="48" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B154" s="47" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C154" s="6"/>
       <c r="D154" s="6"/>
@@ -17017,26 +17022,26 @@
     </row>
     <row r="155">
       <c r="A155" s="94" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B155" s="55" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C155" s="13" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D155" s="13" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E155" s="49" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F155" s="49"/>
       <c r="G155" s="36" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H155" s="121" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="I155" s="6"/>
       <c r="J155" s="6"/>
@@ -17044,26 +17049,26 @@
     </row>
     <row r="156">
       <c r="A156" s="94" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B156" s="55" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C156" s="13" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D156" s="13" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E156" s="49" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="F156" s="49"/>
       <c r="G156" s="36" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H156" s="121" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I156" s="6"/>
       <c r="J156" s="6"/>
@@ -17071,26 +17076,26 @@
     </row>
     <row r="157">
       <c r="A157" s="94" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B157" s="55" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C157" s="13" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D157" s="13" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="F157" s="6"/>
       <c r="G157" s="4" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H157" s="122" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="I157" s="6"/>
       <c r="J157" s="6"/>
@@ -17098,26 +17103,26 @@
     </row>
     <row r="158">
       <c r="A158" s="94" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B158" s="55" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C158" s="13" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D158" s="13" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E158" s="49" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="F158" s="49"/>
       <c r="G158" s="36" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H158" s="121" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="I158" s="6"/>
       <c r="J158" s="6"/>
@@ -17125,10 +17130,10 @@
     </row>
     <row r="159">
       <c r="A159" s="46" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B159" s="47" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C159" s="13"/>
       <c r="D159" s="13"/>
@@ -17142,26 +17147,26 @@
     </row>
     <row r="160">
       <c r="A160" s="94" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B160" s="55" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D160" s="13" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="E160" s="49" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="F160" s="49"/>
       <c r="G160" s="36" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="H160" s="119" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="I160" s="6"/>
       <c r="J160" s="6"/>
@@ -17169,37 +17174,37 @@
     </row>
     <row r="161">
       <c r="A161" s="54" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B161" s="55" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="C161" s="88" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="D161" s="88"/>
       <c r="E161" s="80" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="F161" s="49"/>
       <c r="G161" s="4" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="H161" s="39" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="I161" s="6" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="J161" s="6"/>
       <c r="K161" s="6"/>
     </row>
     <row r="162">
       <c r="A162" s="46" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B162" s="47" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C162" s="97"/>
       <c r="D162" s="88"/>
@@ -17213,24 +17218,24 @@
     </row>
     <row r="163">
       <c r="A163" s="54" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B163" s="55" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C163" s="123" t="s">
         <v>233</v>
       </c>
       <c r="D163" s="88"/>
       <c r="E163" s="80" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="F163" s="4"/>
       <c r="G163" s="4" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="H163" s="103" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="I163" s="6"/>
       <c r="J163" s="6"/>
@@ -17238,24 +17243,24 @@
     </row>
     <row r="164">
       <c r="A164" s="46" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B164" s="47" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C164" s="97" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D164" s="88"/>
       <c r="E164" s="88" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="F164" s="6"/>
       <c r="G164" s="6" t="s">
         <v>367</v>
       </c>
       <c r="H164" s="6" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="I164" s="6"/>
       <c r="J164" s="6"/>
@@ -17263,10 +17268,10 @@
     </row>
     <row r="165">
       <c r="A165" s="91" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B165" s="38" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C165" s="6"/>
       <c r="D165" s="6"/>
@@ -17280,22 +17285,22 @@
     </row>
     <row r="166">
       <c r="A166" s="48" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B166" s="47"/>
       <c r="C166" s="6"/>
       <c r="D166" s="6"/>
       <c r="E166" s="108" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F166" s="87" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="G166" s="4" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H166" s="100" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="I166" s="6"/>
       <c r="J166" s="6"/>
@@ -17303,22 +17308,22 @@
     </row>
     <row r="167">
       <c r="A167" s="48" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B167" s="47" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C167" s="36"/>
       <c r="D167" s="36"/>
       <c r="E167" s="49" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="F167" s="36"/>
       <c r="G167" s="49" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="H167" s="65" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="I167" s="6" t="s">
         <v>72</v>
@@ -17328,55 +17333,55 @@
     </row>
     <row r="168">
       <c r="A168" s="46" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B168" s="47" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D168" s="6"/>
       <c r="E168" s="39" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="F168" s="39" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="G168" s="39" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="H168" s="39" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="I168" s="6"/>
       <c r="J168" s="6"/>
       <c r="K168" s="6" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="46" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B169" s="47" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D169" s="6"/>
       <c r="E169" s="56" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="F169" s="39" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="G169" s="39" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="H169" s="39" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="I169" s="6"/>
       <c r="J169" s="6"/>
@@ -17384,24 +17389,24 @@
     </row>
     <row r="170">
       <c r="A170" s="46" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B170" s="47" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="D170" s="6"/>
       <c r="E170" s="39" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F170" s="4"/>
       <c r="G170" s="4" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="H170" s="39" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="I170" s="6"/>
       <c r="J170" s="6"/>
@@ -17409,24 +17414,24 @@
     </row>
     <row r="171">
       <c r="A171" s="46" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B171" s="47" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D171" s="6"/>
       <c r="E171" s="6" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="87" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="H171" s="124" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="I171" s="6"/>
       <c r="J171" s="6"/>
@@ -17434,10 +17439,10 @@
     </row>
     <row r="172">
       <c r="A172" s="48" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B172" s="47" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C172" s="6"/>
       <c r="D172" s="4"/>
@@ -17451,26 +17456,26 @@
     </row>
     <row r="173">
       <c r="A173" s="94" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B173" s="55" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D173" s="13" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E173" s="125" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="F173" s="125"/>
       <c r="G173" s="13" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="H173" s="13" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="I173" s="6"/>
       <c r="J173" s="6"/>
@@ -17478,24 +17483,24 @@
     </row>
     <row r="174">
       <c r="A174" s="120" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B174" s="34" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C174" s="6"/>
       <c r="D174" s="6"/>
       <c r="E174" s="39" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="F174" s="49" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="G174" s="4" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="H174" s="4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="I174" s="6"/>
       <c r="J174" s="6"/>
@@ -17503,49 +17508,49 @@
     </row>
     <row r="175">
       <c r="A175" s="126" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B175" s="127" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C175" s="128"/>
       <c r="D175" s="128"/>
       <c r="E175" s="56" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="F175" s="40" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="G175" s="40" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="H175" s="129" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="I175" s="6"/>
       <c r="J175" s="6"/>
       <c r="K175" s="6" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="126" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B176" s="127" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C176" s="13"/>
       <c r="D176" s="13"/>
       <c r="E176" s="130" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="F176" s="36"/>
       <c r="G176" s="36" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="H176" s="36" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="I176" s="6"/>
       <c r="J176" s="6"/>
@@ -17553,28 +17558,28 @@
     </row>
     <row r="177">
       <c r="A177" s="48" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B177" s="47" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="D177" s="13" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="E177" s="49" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="F177" s="49" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="G177" s="4" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="H177" s="4" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="I177" s="6" t="s">
         <v>72</v>
@@ -17584,28 +17589,28 @@
     </row>
     <row r="178">
       <c r="A178" s="48" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B178" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="D178" s="13" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="E178" s="49" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="F178" s="49" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="G178" s="4" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H178" s="103" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="I178" s="6" t="s">
         <v>64</v>
@@ -17615,26 +17620,26 @@
     </row>
     <row r="179">
       <c r="A179" s="48" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B179" s="47" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C179" s="13" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D179" s="13" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="E179" s="39" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="F179" s="4"/>
       <c r="G179" s="4" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="H179" s="39" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="I179" s="6"/>
       <c r="J179" s="6"/>
@@ -17642,26 +17647,26 @@
     </row>
     <row r="180">
       <c r="A180" s="131" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B180" s="132" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C180" s="133" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D180" s="113" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="E180" s="39" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="F180" s="4"/>
       <c r="G180" s="4" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="H180" s="39" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="I180" s="6"/>
       <c r="J180" s="6"/>
@@ -17669,13 +17674,13 @@
     </row>
     <row r="181">
       <c r="A181" s="91" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B181" s="38" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C181" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D181" s="13"/>
       <c r="E181" s="4"/>
@@ -17688,13 +17693,13 @@
     </row>
     <row r="182">
       <c r="A182" s="48" t="s">
+        <v>782</v>
+      </c>
+      <c r="B182" s="47" t="s">
+        <v>783</v>
+      </c>
+      <c r="C182" s="134" t="s">
         <v>781</v>
-      </c>
-      <c r="B182" s="47" t="s">
-        <v>782</v>
-      </c>
-      <c r="C182" s="134" t="s">
-        <v>780</v>
       </c>
       <c r="D182" s="13"/>
       <c r="E182" s="36"/>
@@ -17707,26 +17712,26 @@
     </row>
     <row r="183">
       <c r="A183" s="94" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B183" s="55" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C183" s="13" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="D183" s="13" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="E183" s="49" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="F183" s="49"/>
       <c r="G183" s="36" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="H183" s="119" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="I183" s="6"/>
       <c r="J183" s="6"/>
@@ -17734,26 +17739,26 @@
     </row>
     <row r="184">
       <c r="A184" s="94" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B184" s="55" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C184" s="13" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="D184" s="13" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="E184" s="49" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F184" s="63"/>
       <c r="G184" s="4" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="H184" s="122" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="I184" s="6"/>
       <c r="J184" s="6"/>
@@ -17761,24 +17766,24 @@
     </row>
     <row r="185">
       <c r="A185" s="94" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B185" s="55" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C185" s="135" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D185" s="13"/>
       <c r="E185" s="40" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F185" s="40"/>
       <c r="G185" s="40" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="H185" s="136" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="I185" s="6"/>
       <c r="J185" s="6"/>
@@ -17786,13 +17791,13 @@
     </row>
     <row r="186">
       <c r="A186" s="91" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B186" s="38" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C186" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D186" s="13"/>
       <c r="E186" s="36"/>
@@ -17805,20 +17810,20 @@
     </row>
     <row r="187">
       <c r="A187" s="94" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B187" s="55"/>
       <c r="C187" s="13"/>
       <c r="D187" s="6"/>
       <c r="E187" s="56" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="F187" s="49"/>
       <c r="G187" s="36" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="H187" s="49" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="I187" s="6"/>
       <c r="J187" s="6"/>
@@ -17826,49 +17831,49 @@
     </row>
     <row r="188">
       <c r="A188" s="94" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B188" s="81"/>
       <c r="C188" s="13"/>
       <c r="D188" s="6"/>
       <c r="E188" s="56" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="F188" s="49"/>
       <c r="G188" s="36" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="H188" s="49" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="I188" s="6"/>
       <c r="J188" s="6"/>
       <c r="K188" s="6" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="48" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B189" s="47" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C189" s="13" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="D189" s="13" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="E189" s="49" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="F189" s="49"/>
       <c r="G189" s="39" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H189" s="122" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="I189" s="6"/>
       <c r="J189" s="6"/>
@@ -17876,51 +17881,51 @@
     </row>
     <row r="190">
       <c r="A190" s="48" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B190" s="47" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C190" s="137"/>
       <c r="D190" s="138"/>
       <c r="E190" s="56" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="F190" s="137"/>
       <c r="G190" s="49" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="H190" s="36" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="I190" s="6" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="J190" s="6"/>
       <c r="K190" s="6"/>
     </row>
     <row r="191">
       <c r="A191" s="94" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B191" s="55" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="D191" s="13" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="E191" s="49" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="F191" s="49"/>
       <c r="G191" s="36" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="H191" s="100" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="I191" s="6"/>
       <c r="J191" s="6"/>
@@ -17928,22 +17933,22 @@
     </row>
     <row r="192">
       <c r="A192" s="94" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B192" s="55" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C192" s="13"/>
       <c r="D192" s="13"/>
       <c r="E192" s="49" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="F192" s="49"/>
       <c r="G192" s="4" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H192" s="39" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="I192" s="6"/>
       <c r="J192" s="6"/>
@@ -17951,22 +17956,22 @@
     </row>
     <row r="193">
       <c r="A193" s="94" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B193" s="55" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C193" s="13"/>
       <c r="D193" s="13"/>
       <c r="E193" s="49" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="F193" s="49"/>
       <c r="G193" s="4" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H193" s="39" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="I193" s="6"/>
       <c r="J193" s="6"/>
@@ -17974,22 +17979,22 @@
     </row>
     <row r="194">
       <c r="A194" s="94" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B194" s="55" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
       <c r="E194" s="49" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="F194" s="49"/>
       <c r="G194" s="4" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H194" s="39" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="I194" s="6"/>
       <c r="J194" s="6"/>
@@ -17997,22 +18002,22 @@
     </row>
     <row r="195">
       <c r="A195" s="94" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B195" s="55" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C195" s="13"/>
       <c r="D195" s="13"/>
       <c r="E195" s="49" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="F195" s="63"/>
       <c r="G195" s="4" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H195" s="4" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="I195" s="6"/>
       <c r="J195" s="6"/>
@@ -18020,17 +18025,17 @@
     </row>
     <row r="196">
       <c r="A196" s="94" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B196" s="55" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C196" s="139" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D196" s="13"/>
       <c r="E196" s="49" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F196" s="39"/>
       <c r="G196" s="36" t="s">
@@ -18045,13 +18050,13 @@
     </row>
     <row r="197">
       <c r="A197" s="48" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B197" s="47" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C197" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D197" s="13"/>
       <c r="E197" s="39"/>
@@ -18064,7 +18069,7 @@
     </row>
     <row r="198">
       <c r="A198" s="94" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B198" s="55" t="s">
         <v>58</v>
@@ -18076,14 +18081,14 @@
         <v>60</v>
       </c>
       <c r="E198" s="49" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="F198" s="49"/>
       <c r="G198" s="43" t="s">
         <v>62</v>
       </c>
       <c r="H198" s="43" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="I198" s="6" t="s">
         <v>64</v>
@@ -18093,7 +18098,7 @@
     </row>
     <row r="199">
       <c r="A199" s="94" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B199" s="55" t="s">
         <v>66</v>
@@ -18105,14 +18110,14 @@
         <v>68</v>
       </c>
       <c r="E199" s="49" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="F199" s="49"/>
       <c r="G199" s="45" t="s">
         <v>70</v>
       </c>
       <c r="H199" s="45" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="I199" s="6" t="s">
         <v>72</v>
@@ -18122,7 +18127,7 @@
     </row>
     <row r="200">
       <c r="A200" s="94" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B200" s="55" t="s">
         <v>74</v>
@@ -18134,14 +18139,14 @@
         <v>76</v>
       </c>
       <c r="E200" s="49" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="F200" s="49"/>
       <c r="G200" s="4" t="s">
         <v>78</v>
       </c>
       <c r="H200" s="39" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="I200" s="6"/>
       <c r="J200" s="6"/>
@@ -18149,7 +18154,7 @@
     </row>
     <row r="201">
       <c r="A201" s="94" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B201" s="55" t="s">
         <v>81</v>
@@ -18161,14 +18166,14 @@
         <v>83</v>
       </c>
       <c r="E201" s="49" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="F201" s="49"/>
       <c r="G201" s="4" t="s">
         <v>78</v>
       </c>
       <c r="H201" s="39" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="I201" s="6"/>
       <c r="J201" s="6"/>
@@ -18176,7 +18181,7 @@
     </row>
     <row r="202">
       <c r="A202" s="94" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B202" s="55" t="s">
         <v>87</v>
@@ -18188,16 +18193,16 @@
         <v>89</v>
       </c>
       <c r="E202" s="39" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="F202" s="39" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="G202" s="36" t="s">
         <v>92</v>
       </c>
       <c r="H202" s="49" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="I202" s="6"/>
       <c r="J202" s="6"/>
@@ -18205,7 +18210,7 @@
     </row>
     <row r="203">
       <c r="A203" s="94" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B203" s="55" t="s">
         <v>95</v>
@@ -18214,17 +18219,17 @@
         <v>96</v>
       </c>
       <c r="D203" s="13" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E203" s="125" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="F203" s="125"/>
       <c r="G203" s="4" t="s">
         <v>99</v>
       </c>
       <c r="H203" s="39" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="I203" s="6"/>
       <c r="J203" s="6"/>
@@ -18232,7 +18237,7 @@
     </row>
     <row r="204">
       <c r="A204" s="94" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B204" s="55" t="s">
         <v>102</v>
@@ -18244,14 +18249,14 @@
         <v>104</v>
       </c>
       <c r="E204" s="125" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="F204" s="125"/>
       <c r="G204" s="43" t="s">
         <v>106</v>
       </c>
       <c r="H204" s="43" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="I204" s="6"/>
       <c r="J204" s="6"/>
@@ -18259,7 +18264,7 @@
     </row>
     <row r="205">
       <c r="A205" s="94" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B205" s="55" t="s">
         <v>122</v>
@@ -18271,14 +18276,14 @@
         <v>124</v>
       </c>
       <c r="E205" s="125" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="F205" s="125"/>
       <c r="G205" s="49" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H205" s="49" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I205" s="6"/>
       <c r="J205" s="6"/>
@@ -18286,7 +18291,7 @@
     </row>
     <row r="206">
       <c r="A206" s="94" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B206" s="55" t="s">
         <v>116</v>
@@ -18298,14 +18303,14 @@
         <v>118</v>
       </c>
       <c r="E206" s="125" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="F206" s="125"/>
       <c r="G206" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H206" s="63" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I206" s="6"/>
       <c r="J206" s="6"/>
@@ -18313,10 +18318,10 @@
     </row>
     <row r="207">
       <c r="A207" s="94" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B207" s="55" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C207" s="13" t="s">
         <v>138</v>
@@ -18325,14 +18330,14 @@
         <v>139</v>
       </c>
       <c r="E207" s="125" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="F207" s="125"/>
       <c r="G207" s="60" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H207" s="60" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="I207" s="6"/>
       <c r="J207" s="6"/>
@@ -18340,7 +18345,7 @@
     </row>
     <row r="208">
       <c r="A208" s="94" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B208" s="55" t="s">
         <v>129</v>
@@ -18352,14 +18357,14 @@
         <v>131</v>
       </c>
       <c r="E208" s="125" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="F208" s="125"/>
       <c r="G208" s="49" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H208" s="49" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="I208" s="6"/>
       <c r="J208" s="6"/>
@@ -18367,26 +18372,26 @@
     </row>
     <row r="209">
       <c r="A209" s="94" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B209" s="55" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="D209" s="13" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="E209" s="125" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="F209" s="90"/>
       <c r="G209" s="4" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="H209" s="141" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="I209" s="6"/>
       <c r="J209" s="6"/>
@@ -18398,14 +18403,14 @@
       <c r="C210" s="13"/>
       <c r="D210" s="13"/>
       <c r="E210" s="142" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="F210" s="90"/>
       <c r="G210" s="43" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="H210" s="43" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="I210" s="6"/>
       <c r="J210" s="6"/>
@@ -18413,13 +18418,13 @@
     </row>
     <row r="211">
       <c r="A211" s="48" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B211" s="47" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C211" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D211" s="13"/>
       <c r="E211" s="143"/>
@@ -18432,10 +18437,10 @@
     </row>
     <row r="212">
       <c r="A212" s="94" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B212" s="55" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C212" s="13" t="s">
         <v>521</v>
@@ -18444,14 +18449,14 @@
         <v>406</v>
       </c>
       <c r="E212" s="125" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="F212" s="125"/>
       <c r="G212" s="13" t="s">
         <v>523</v>
       </c>
       <c r="H212" s="63" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="I212" s="6"/>
       <c r="J212" s="6"/>
@@ -18459,7 +18464,7 @@
     </row>
     <row r="213">
       <c r="A213" s="106" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B213" s="75" t="s">
         <v>411</v>
@@ -18469,14 +18474,14 @@
       </c>
       <c r="D213" s="13"/>
       <c r="E213" s="49" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="F213" s="63"/>
       <c r="G213" s="36" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="H213" s="49" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="I213" s="6"/>
       <c r="J213" s="6"/>
@@ -18484,26 +18489,26 @@
     </row>
     <row r="214">
       <c r="A214" s="94" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B214" s="55" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C214" s="13" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="D214" s="13" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="E214" s="125" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="F214" s="125"/>
       <c r="G214" s="4" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="H214" s="39" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="I214" s="6"/>
       <c r="J214" s="6"/>
@@ -18511,7 +18516,7 @@
     </row>
     <row r="215">
       <c r="A215" s="106" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B215" s="75" t="s">
         <v>411</v>
@@ -18521,14 +18526,14 @@
       </c>
       <c r="D215" s="143"/>
       <c r="E215" s="125" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="F215" s="125"/>
       <c r="G215" s="4" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="H215" s="39" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="I215" s="6"/>
       <c r="J215" s="6"/>
@@ -18536,7 +18541,7 @@
     </row>
     <row r="216">
       <c r="A216" s="94" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B216" s="55" t="s">
         <v>458</v>
@@ -18548,14 +18553,14 @@
         <v>460</v>
       </c>
       <c r="E216" s="125" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="F216" s="125"/>
       <c r="G216" s="36" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="H216" s="49" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="I216" s="6"/>
       <c r="J216" s="6"/>
@@ -18563,7 +18568,7 @@
     </row>
     <row r="217">
       <c r="A217" s="106" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B217" s="75" t="s">
         <v>411</v>
@@ -18573,14 +18578,14 @@
       </c>
       <c r="D217" s="143"/>
       <c r="E217" s="125" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F217" s="125"/>
       <c r="G217" s="36" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H217" s="49" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="I217" s="6"/>
       <c r="J217" s="6"/>
@@ -18588,7 +18593,7 @@
     </row>
     <row r="218">
       <c r="A218" s="94" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B218" s="55" t="s">
         <v>464</v>
@@ -18600,14 +18605,14 @@
         <v>466</v>
       </c>
       <c r="E218" s="125" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="F218" s="125"/>
       <c r="G218" s="36" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="H218" s="49" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I218" s="6"/>
       <c r="J218" s="6"/>
@@ -18615,7 +18620,7 @@
     </row>
     <row r="219">
       <c r="A219" s="106" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B219" s="75" t="s">
         <v>411</v>
@@ -18625,14 +18630,14 @@
       </c>
       <c r="D219" s="143"/>
       <c r="E219" s="142" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F219" s="125"/>
       <c r="G219" s="36" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H219" s="49" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="I219" s="6"/>
       <c r="J219" s="6"/>
@@ -18640,13 +18645,13 @@
     </row>
     <row r="220">
       <c r="A220" s="48" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B220" s="47" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C220" s="146" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D220" s="143"/>
       <c r="E220" s="143"/>
@@ -18659,26 +18664,26 @@
     </row>
     <row r="221">
       <c r="A221" s="94" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B221" s="55" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="D221" s="13" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E221" s="125" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="F221" s="125"/>
       <c r="G221" s="63" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="H221" s="147" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="I221" s="6"/>
       <c r="J221" s="6"/>
@@ -18686,10 +18691,10 @@
     </row>
     <row r="222">
       <c r="A222" s="94" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B222" s="89" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C222" s="6"/>
       <c r="D222" s="6"/>
@@ -18703,26 +18708,26 @@
     </row>
     <row r="223">
       <c r="A223" s="94" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B223" s="89" t="s">
         <v>404</v>
       </c>
       <c r="C223" s="63" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="D223" s="63" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E223" s="49" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="F223" s="63"/>
       <c r="G223" s="36" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="H223" s="49" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="I223" s="6"/>
       <c r="J223" s="6"/>
@@ -18730,7 +18735,7 @@
     </row>
     <row r="224">
       <c r="A224" s="94" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B224" s="89" t="s">
         <v>411</v>
@@ -18740,14 +18745,14 @@
       </c>
       <c r="D224" s="13"/>
       <c r="E224" s="63" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="F224" s="63"/>
       <c r="G224" s="63" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="H224" s="13" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="I224" s="6"/>
       <c r="J224" s="6"/>
@@ -18755,26 +18760,26 @@
     </row>
     <row r="225">
       <c r="A225" s="94" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B225" s="89" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="C225" s="13" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="D225" s="13" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="E225" s="125" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="F225" s="125"/>
       <c r="G225" s="49" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="H225" s="49" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I225" s="6"/>
       <c r="J225" s="6"/>
@@ -18782,26 +18787,26 @@
     </row>
     <row r="226">
       <c r="A226" s="94" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B226" s="89" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C226" s="13" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="D226" s="13" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E226" s="125" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="F226" s="125"/>
       <c r="G226" s="63" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="H226" s="63" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="I226" s="6" t="s">
         <v>64</v>
@@ -18811,10 +18816,10 @@
     </row>
     <row r="227">
       <c r="A227" s="120" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B227" s="148" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C227" s="6"/>
       <c r="D227" s="6"/>
@@ -18828,10 +18833,10 @@
     </row>
     <row r="228">
       <c r="A228" s="37" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B228" s="61" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C228" s="97"/>
       <c r="D228" s="88"/>
@@ -18845,24 +18850,24 @@
     </row>
     <row r="229">
       <c r="A229" s="46" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B229" s="64" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C229" s="97" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="D229" s="88"/>
       <c r="E229" s="149" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="F229" s="143"/>
       <c r="G229" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H229" s="32" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="I229" s="6"/>
       <c r="J229" s="6"/>
@@ -18870,24 +18875,24 @@
     </row>
     <row r="230">
       <c r="A230" s="46" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B230" s="64" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C230" s="97" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="D230" s="88"/>
       <c r="E230" s="149" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="F230" s="143"/>
       <c r="G230" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H230" s="32" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="I230" s="6"/>
       <c r="J230" s="6"/>
@@ -18895,24 +18900,24 @@
     </row>
     <row r="231">
       <c r="A231" s="46" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B231" s="64" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C231" s="97" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D231" s="88"/>
       <c r="E231" s="149" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="F231" s="143"/>
       <c r="G231" s="4" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H231" s="103" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="I231" s="6"/>
       <c r="J231" s="6"/>
@@ -18920,7 +18925,7 @@
     </row>
     <row r="232">
       <c r="A232" s="91" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B232" s="61" t="s">
         <v>577</v>
@@ -18932,14 +18937,14 @@
         <v>579</v>
       </c>
       <c r="E232" s="125" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="F232" s="125"/>
       <c r="G232" s="150" t="s">
         <v>367</v>
       </c>
       <c r="H232" s="151" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="I232" s="6" t="s">
         <v>64</v>
@@ -18949,13 +18954,13 @@
     </row>
     <row r="233">
       <c r="A233" s="91" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B233" s="61" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="C233" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D233" s="6"/>
       <c r="E233" s="143"/>
@@ -18968,17 +18973,17 @@
     </row>
     <row r="234">
       <c r="A234" s="48" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B234" s="64" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C234" s="152" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D234" s="6"/>
       <c r="E234" s="90" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="F234" s="125"/>
       <c r="G234" s="13" t="s">
@@ -18993,7 +18998,7 @@
     </row>
     <row r="235">
       <c r="A235" s="94" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B235" s="89" t="s">
         <v>58</v>
@@ -19005,14 +19010,14 @@
         <v>60</v>
       </c>
       <c r="E235" s="125" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F235" s="125"/>
       <c r="G235" s="87" t="s">
         <v>62</v>
       </c>
       <c r="H235" s="87" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="I235" s="6" t="s">
         <v>64</v>
@@ -19022,7 +19027,7 @@
     </row>
     <row r="236">
       <c r="A236" s="94" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B236" s="89" t="s">
         <v>74</v>
@@ -19034,14 +19039,14 @@
         <v>76</v>
       </c>
       <c r="E236" s="63" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F236" s="63"/>
       <c r="G236" s="87" t="s">
         <v>78</v>
       </c>
       <c r="H236" s="87" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I236" s="6"/>
       <c r="J236" s="6"/>
@@ -19049,7 +19054,7 @@
     </row>
     <row r="237">
       <c r="A237" s="94" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B237" s="89" t="s">
         <v>81</v>
@@ -19061,14 +19066,14 @@
         <v>83</v>
       </c>
       <c r="E237" s="63" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F237" s="63"/>
       <c r="G237" s="87" t="s">
         <v>78</v>
       </c>
       <c r="H237" s="87" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I237" s="6"/>
       <c r="J237" s="6"/>
@@ -19076,7 +19081,7 @@
     </row>
     <row r="238">
       <c r="A238" s="94" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B238" s="89" t="s">
         <v>95</v>
@@ -19085,17 +19090,17 @@
         <v>96</v>
       </c>
       <c r="D238" s="13" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E238" s="63" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="F238" s="63"/>
       <c r="G238" s="87" t="s">
         <v>99</v>
       </c>
       <c r="H238" s="87" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="I238" s="6"/>
       <c r="J238" s="6"/>
@@ -19103,7 +19108,7 @@
     </row>
     <row r="239">
       <c r="A239" s="94" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B239" s="89" t="s">
         <v>102</v>
@@ -19115,14 +19120,14 @@
         <v>104</v>
       </c>
       <c r="E239" s="63" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="F239" s="63"/>
       <c r="G239" s="63" t="s">
         <v>106</v>
       </c>
       <c r="H239" s="63" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I239" s="6"/>
       <c r="J239" s="6"/>
@@ -19130,7 +19135,7 @@
     </row>
     <row r="240">
       <c r="A240" s="94" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B240" s="89" t="s">
         <v>122</v>
@@ -19142,14 +19147,14 @@
         <v>124</v>
       </c>
       <c r="E240" s="63" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="F240" s="63"/>
       <c r="G240" s="63" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H240" s="63" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I240" s="6"/>
       <c r="J240" s="6"/>
@@ -19157,7 +19162,7 @@
     </row>
     <row r="241">
       <c r="A241" s="94" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B241" s="89" t="s">
         <v>116</v>
@@ -19169,14 +19174,14 @@
         <v>118</v>
       </c>
       <c r="E241" s="63" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="F241" s="63"/>
       <c r="G241" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H241" s="63" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I241" s="6"/>
       <c r="J241" s="6"/>
@@ -19184,10 +19189,10 @@
     </row>
     <row r="242">
       <c r="A242" s="94" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B242" s="89" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C242" s="13" t="s">
         <v>138</v>
@@ -19196,14 +19201,14 @@
         <v>139</v>
       </c>
       <c r="E242" s="63" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="F242" s="63"/>
       <c r="G242" s="60" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H242" s="60" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="I242" s="6"/>
       <c r="J242" s="6"/>
@@ -19211,7 +19216,7 @@
     </row>
     <row r="243">
       <c r="A243" s="94" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B243" s="89" t="s">
         <v>129</v>
@@ -19223,14 +19228,14 @@
         <v>131</v>
       </c>
       <c r="E243" s="63" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="F243" s="63"/>
       <c r="G243" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H243" s="63" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="I243" s="6"/>
       <c r="J243" s="6"/>
@@ -19238,21 +19243,21 @@
     </row>
     <row r="244">
       <c r="A244" s="48" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B244" s="64" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C244" s="152" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D244" s="153"/>
       <c r="E244" s="87" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="F244" s="13"/>
       <c r="G244" s="13" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="H244" s="13" t="s">
         <v>235</v>
@@ -19263,7 +19268,7 @@
     </row>
     <row r="245">
       <c r="A245" s="94" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B245" s="89" t="s">
         <v>58</v>
@@ -19275,14 +19280,14 @@
         <v>60</v>
       </c>
       <c r="E245" s="63" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="F245" s="63"/>
       <c r="G245" s="87" t="s">
         <v>62</v>
       </c>
       <c r="H245" s="87" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="I245" s="6" t="s">
         <v>64</v>
@@ -19292,7 +19297,7 @@
     </row>
     <row r="246">
       <c r="A246" s="94" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B246" s="89" t="s">
         <v>74</v>
@@ -19304,14 +19309,14 @@
         <v>76</v>
       </c>
       <c r="E246" s="63" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="F246" s="63"/>
       <c r="G246" s="87" t="s">
         <v>78</v>
       </c>
       <c r="H246" s="87" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="I246" s="6"/>
       <c r="J246" s="6"/>
@@ -19319,7 +19324,7 @@
     </row>
     <row r="247">
       <c r="A247" s="94" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B247" s="89" t="s">
         <v>81</v>
@@ -19331,14 +19336,14 @@
         <v>83</v>
       </c>
       <c r="E247" s="63" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="F247" s="63"/>
       <c r="G247" s="87" t="s">
         <v>78</v>
       </c>
       <c r="H247" s="124" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="I247" s="6"/>
       <c r="J247" s="6"/>
@@ -19346,7 +19351,7 @@
     </row>
     <row r="248">
       <c r="A248" s="94" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B248" s="89" t="s">
         <v>95</v>
@@ -19355,17 +19360,17 @@
         <v>96</v>
       </c>
       <c r="D248" s="13" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E248" s="63" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="F248" s="63"/>
       <c r="G248" s="87" t="s">
         <v>99</v>
       </c>
       <c r="H248" s="124" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="I248" s="6"/>
       <c r="J248" s="6"/>
@@ -19373,7 +19378,7 @@
     </row>
     <row r="249">
       <c r="A249" s="94" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B249" s="89" t="s">
         <v>102</v>
@@ -19385,14 +19390,14 @@
         <v>104</v>
       </c>
       <c r="E249" s="63" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="F249" s="63"/>
       <c r="G249" s="87" t="s">
         <v>106</v>
       </c>
       <c r="H249" s="124" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I249" s="6"/>
       <c r="J249" s="6"/>
@@ -19400,7 +19405,7 @@
     </row>
     <row r="250">
       <c r="A250" s="94" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B250" s="89" t="s">
         <v>122</v>
@@ -19412,14 +19417,14 @@
         <v>124</v>
       </c>
       <c r="E250" s="63" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="F250" s="63"/>
       <c r="G250" s="63" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H250" s="63" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I250" s="6"/>
       <c r="J250" s="6"/>
@@ -19427,7 +19432,7 @@
     </row>
     <row r="251">
       <c r="A251" s="94" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B251" s="89" t="s">
         <v>116</v>
@@ -19439,14 +19444,14 @@
         <v>118</v>
       </c>
       <c r="E251" s="63" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F251" s="63"/>
       <c r="G251" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H251" s="154" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I251" s="6"/>
       <c r="J251" s="6"/>
@@ -19454,10 +19459,10 @@
     </row>
     <row r="252">
       <c r="A252" s="94" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B252" s="89" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C252" s="13" t="s">
         <v>138</v>
@@ -19466,14 +19471,14 @@
         <v>139</v>
       </c>
       <c r="E252" s="63" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="F252" s="63"/>
       <c r="G252" s="60" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H252" s="155" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="I252" s="6"/>
       <c r="J252" s="6"/>
@@ -19481,7 +19486,7 @@
     </row>
     <row r="253">
       <c r="A253" s="94" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B253" s="89" t="s">
         <v>129</v>
@@ -19493,14 +19498,14 @@
         <v>131</v>
       </c>
       <c r="E253" s="63" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F253" s="63"/>
       <c r="G253" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H253" s="63" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="I253" s="6"/>
       <c r="J253" s="6"/>
@@ -19508,26 +19513,26 @@
     </row>
     <row r="254">
       <c r="A254" s="48" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B254" s="64" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="C254" s="13" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="D254" s="13" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="E254" s="63" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="F254" s="63"/>
       <c r="G254" s="87" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="H254" s="156" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="I254" s="6"/>
       <c r="J254" s="6"/>
@@ -19535,15 +19540,15 @@
     </row>
     <row r="255">
       <c r="A255" s="48" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B255" s="64" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C255" s="6"/>
       <c r="D255" s="6"/>
       <c r="E255" s="87" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F255" s="13"/>
       <c r="G255" s="13" t="s">
@@ -19558,7 +19563,7 @@
     </row>
     <row r="256">
       <c r="A256" s="94" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B256" s="89" t="s">
         <v>58</v>
@@ -19570,14 +19575,14 @@
         <v>60</v>
       </c>
       <c r="E256" s="63" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="F256" s="63"/>
       <c r="G256" s="87" t="s">
         <v>62</v>
       </c>
       <c r="H256" s="87" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="I256" s="6" t="s">
         <v>64</v>
@@ -19587,7 +19592,7 @@
     </row>
     <row r="257">
       <c r="A257" s="94" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B257" s="89" t="s">
         <v>74</v>
@@ -19599,14 +19604,14 @@
         <v>76</v>
       </c>
       <c r="E257" s="63" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="F257" s="63"/>
       <c r="G257" s="87" t="s">
         <v>78</v>
       </c>
       <c r="H257" s="124" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="I257" s="6"/>
       <c r="J257" s="6"/>
@@ -19614,7 +19619,7 @@
     </row>
     <row r="258">
       <c r="A258" s="94" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B258" s="89" t="s">
         <v>81</v>
@@ -19626,14 +19631,14 @@
         <v>83</v>
       </c>
       <c r="E258" s="63" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="F258" s="63"/>
       <c r="G258" s="87" t="s">
         <v>78</v>
       </c>
       <c r="H258" s="124" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="I258" s="6"/>
       <c r="J258" s="6"/>
@@ -19641,7 +19646,7 @@
     </row>
     <row r="259">
       <c r="A259" s="94" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B259" s="89" t="s">
         <v>95</v>
@@ -19650,17 +19655,17 @@
         <v>96</v>
       </c>
       <c r="D259" s="13" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E259" s="63" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="F259" s="63"/>
       <c r="G259" s="87" t="s">
         <v>99</v>
       </c>
       <c r="H259" s="124" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="I259" s="6"/>
       <c r="J259" s="6"/>
@@ -19668,7 +19673,7 @@
     </row>
     <row r="260">
       <c r="A260" s="94" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B260" s="89" t="s">
         <v>102</v>
@@ -19680,14 +19685,14 @@
         <v>104</v>
       </c>
       <c r="E260" s="63" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="F260" s="63"/>
       <c r="G260" s="63" t="s">
         <v>106</v>
       </c>
       <c r="H260" s="154" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="I260" s="6"/>
       <c r="J260" s="6"/>
@@ -19695,7 +19700,7 @@
     </row>
     <row r="261">
       <c r="A261" s="94" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="B261" s="89" t="s">
         <v>122</v>
@@ -19707,14 +19712,14 @@
         <v>124</v>
       </c>
       <c r="E261" s="63" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="F261" s="63"/>
       <c r="G261" s="63" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H261" s="63" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I261" s="6"/>
       <c r="J261" s="6"/>
@@ -19722,7 +19727,7 @@
     </row>
     <row r="262">
       <c r="A262" s="94" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B262" s="89" t="s">
         <v>116</v>
@@ -19734,14 +19739,14 @@
         <v>118</v>
       </c>
       <c r="E262" s="63" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="F262" s="63"/>
       <c r="G262" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H262" s="154" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I262" s="6"/>
       <c r="J262" s="6"/>
@@ -19749,10 +19754,10 @@
     </row>
     <row r="263">
       <c r="A263" s="94" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B263" s="89" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C263" s="13" t="s">
         <v>138</v>
@@ -19761,14 +19766,14 @@
         <v>139</v>
       </c>
       <c r="E263" s="63" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="F263" s="63"/>
       <c r="G263" s="60" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H263" s="155" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="I263" s="6"/>
       <c r="J263" s="6"/>
@@ -19776,7 +19781,7 @@
     </row>
     <row r="264">
       <c r="A264" s="94" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B264" s="89" t="s">
         <v>129</v>
@@ -19788,14 +19793,14 @@
         <v>131</v>
       </c>
       <c r="E264" s="63" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="F264" s="63"/>
       <c r="G264" s="63" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H264" s="154" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="I264" s="6"/>
       <c r="J264" s="6"/>
@@ -19803,26 +19808,26 @@
     </row>
     <row r="265">
       <c r="A265" s="91" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B265" s="61" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C265" s="157" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="D265" s="157" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="E265" s="158" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="F265" s="158"/>
       <c r="G265" s="87" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="H265" s="159" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="I265" s="6"/>
       <c r="J265" s="6"/>
@@ -19830,10 +19835,10 @@
     </row>
     <row r="266">
       <c r="A266" s="120" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B266" s="148" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C266" s="6"/>
       <c r="D266" s="6"/>
@@ -19847,17 +19852,17 @@
     </row>
     <row r="267">
       <c r="A267" s="91" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B267" s="61" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C267" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D267" s="13"/>
       <c r="E267" s="63" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="F267" s="6"/>
       <c r="G267" s="6"/>
@@ -19868,16 +19873,16 @@
     </row>
     <row r="268">
       <c r="A268" s="48" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B268" s="64" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="C268" s="134" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D268" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E268" s="87"/>
       <c r="F268" s="6"/>
@@ -19889,26 +19894,26 @@
     </row>
     <row r="269">
       <c r="A269" s="94" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B269" s="89" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C269" s="13" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="D269" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="E269" s="63" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="F269" s="13"/>
       <c r="G269" s="87" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="H269" s="124" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="I269" s="6"/>
       <c r="J269" s="6"/>
@@ -19916,26 +19921,26 @@
     </row>
     <row r="270">
       <c r="A270" s="160" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B270" s="161" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C270" s="162" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="D270" s="162" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="E270" s="108" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="F270" s="13"/>
       <c r="G270" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H270" s="124" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="I270" s="6"/>
       <c r="J270" s="6"/>
@@ -19943,26 +19948,26 @@
     </row>
     <row r="271">
       <c r="A271" s="94" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B271" s="89" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C271" s="13" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="D271" s="13" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="E271" s="63" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="F271" s="13"/>
       <c r="G271" s="87" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="H271" s="124" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="I271" s="6"/>
       <c r="J271" s="6"/>
@@ -19970,26 +19975,26 @@
     </row>
     <row r="272">
       <c r="A272" s="160" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B272" s="161" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C272" s="162" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="D272" s="162" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="E272" s="108" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="F272" s="13"/>
       <c r="G272" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H272" s="124" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="I272" s="6"/>
       <c r="J272" s="6"/>
@@ -19997,13 +20002,13 @@
     </row>
     <row r="273">
       <c r="A273" s="48" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B273" s="64" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="C273" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D273" s="13"/>
       <c r="E273" s="13"/>
@@ -20016,26 +20021,26 @@
     </row>
     <row r="274">
       <c r="A274" s="94" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="B274" s="89" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C274" s="13" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D274" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E274" s="63" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="F274" s="6"/>
       <c r="G274" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H274" s="124" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="I274" s="6"/>
       <c r="J274" s="6"/>
@@ -20043,26 +20048,26 @@
     </row>
     <row r="275">
       <c r="A275" s="94" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B275" s="89" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="C275" s="13" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D275" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E275" s="63" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="F275" s="6"/>
       <c r="G275" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H275" s="124" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="I275" s="6"/>
       <c r="J275" s="6"/>
@@ -20070,26 +20075,26 @@
     </row>
     <row r="276">
       <c r="A276" s="94" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B276" s="89" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="C276" s="13" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D276" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E276" s="63" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="F276" s="6"/>
       <c r="G276" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H276" s="124" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="I276" s="6"/>
       <c r="J276" s="6"/>
@@ -20097,26 +20102,26 @@
     </row>
     <row r="277">
       <c r="A277" s="48" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B277" s="64" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="C277" s="134" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D277" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E277" s="63" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="F277" s="6"/>
       <c r="G277" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H277" s="124" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="I277" s="6"/>
       <c r="J277" s="6"/>
@@ -20124,26 +20129,26 @@
     </row>
     <row r="278">
       <c r="A278" s="48" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B278" s="64" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="C278" s="134" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D278" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E278" s="63" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="F278" s="6"/>
       <c r="G278" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H278" s="124" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="I278" s="6"/>
       <c r="J278" s="6"/>
@@ -20151,13 +20156,13 @@
     </row>
     <row r="279">
       <c r="A279" s="48" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B279" s="64" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="C279" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D279" s="13"/>
       <c r="E279" s="13"/>
@@ -20170,26 +20175,26 @@
     </row>
     <row r="280">
       <c r="A280" s="94" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="B280" s="89" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="C280" s="13" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D280" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E280" s="63" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="F280" s="6"/>
       <c r="G280" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H280" s="124" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="I280" s="6"/>
       <c r="J280" s="6"/>
@@ -20197,26 +20202,26 @@
     </row>
     <row r="281">
       <c r="A281" s="94" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B281" s="89" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C281" s="13" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D281" s="13" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E281" s="63" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="F281" s="6"/>
       <c r="G281" s="6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H281" s="124" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="I281" s="6"/>
       <c r="J281" s="6"/>
@@ -20224,13 +20229,13 @@
     </row>
     <row r="282">
       <c r="A282" s="91" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B282" s="61" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="C282" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D282" s="13"/>
       <c r="E282" s="13"/>
@@ -20243,24 +20248,24 @@
     </row>
     <row r="283">
       <c r="A283" s="48" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="B283" s="64" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C283" s="163" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D283" s="13"/>
       <c r="E283" s="63" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="F283" s="6"/>
       <c r="G283" s="13" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="H283" s="154" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="I283" s="6"/>
       <c r="J283" s="6"/>
@@ -20268,13 +20273,13 @@
     </row>
     <row r="284">
       <c r="A284" s="91" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="B284" s="61" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C284" s="134" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D284" s="13"/>
       <c r="E284" s="13"/>
@@ -20287,29 +20292,29 @@
     </row>
     <row r="285">
       <c r="A285" s="48" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B285" s="164" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="C285" s="134" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="D285" s="13" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="E285" s="158" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="F285" s="6"/>
       <c r="G285" s="6" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="H285" s="124" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="I285" s="6" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="J285" s="6"/>
       <c r="K285" s="6"/>
@@ -20436,7 +20441,7 @@
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="B2" s="87" t="s">
         <v>143</v>
@@ -20448,15 +20453,15 @@
         <v>145</v>
       </c>
       <c r="E2" s="87" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="F2" s="87" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="B3" s="87" t="s">
         <v>143</v>
@@ -20468,10 +20473,10 @@
         <v>145</v>
       </c>
       <c r="E3" s="87" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="F3" s="87" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="4">
@@ -20482,14 +20487,14 @@
         <v>420</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="87" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="F4" s="87" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="5">
@@ -20500,92 +20505,92 @@
         <v>420</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="D5" s="63"/>
       <c r="E5" s="87" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D6" s="63" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="E6" s="87" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="F6" s="87" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B7" s="87" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="E7" s="87" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="F7" s="87" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B8" s="87" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C8" s="167" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="87" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B9" s="87" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="E9" s="87" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="F9" s="87" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
     </row>
   </sheetData>
@@ -20609,36 +20614,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="168" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B2" s="169" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="170" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B3" s="169" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="171" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="172" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B6" s="169" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="169" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="8">
@@ -20649,41 +20654,41 @@
     </row>
     <row r="10">
       <c r="A10" s="172" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="172" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B11" s="173" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="174" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="175"/>
       <c r="B13" s="176" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="177" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="178" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="179" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="17">
@@ -20692,24 +20697,24 @@
     </row>
     <row r="18">
       <c r="A18" s="172" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B18" s="180" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B19" s="82"/>
     </row>
     <row r="21">
       <c r="A21" s="172" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B21" s="181" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
     </row>
   </sheetData>
@@ -20735,52 +20740,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="172" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="182" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="183" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="182" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="183" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="183" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="183" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="182" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="183" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="183" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
     </row>
   </sheetData>
@@ -20806,58 +20811,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B1" s="184" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="169" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
     </row>
   </sheetData>
@@ -20901,35 +20906,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="185" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="C1" s="186" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -20960,13 +20965,13 @@
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>1228</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>1226</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1227</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="1"/>
@@ -20997,13 +21002,13 @@
     </row>
     <row r="5">
       <c r="A5" s="39" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -21031,16 +21036,16 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -21067,16 +21072,16 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D7" s="187" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -21103,16 +21108,16 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -21139,16 +21144,16 @@
     </row>
     <row r="9">
       <c r="A9" s="87" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -21175,16 +21180,16 @@
     </row>
     <row r="10">
       <c r="A10" s="87" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -21211,16 +21216,16 @@
     </row>
     <row r="11">
       <c r="A11" s="87" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -21247,16 +21252,16 @@
     </row>
     <row r="12">
       <c r="A12" s="87" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -21283,16 +21288,16 @@
     </row>
     <row r="13">
       <c r="A13" s="188" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="B13" s="188" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="C13" s="189" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D13" s="189" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="E13" s="189"/>
       <c r="F13" s="189"/>
@@ -21319,16 +21324,16 @@
     </row>
     <row r="14">
       <c r="A14" s="188" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="B14" s="188" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="C14" s="189" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D14" s="189" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="E14" s="189"/>
       <c r="F14" s="189"/>
@@ -21380,58 +21385,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="185" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="C1" s="186" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D2" s="184" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C5" s="190" t="s">
         <v>1258</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C5" s="190" t="s">
-        <v>1257</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>